<commit_message>
update data from update_data
</commit_message>
<xml_diff>
--- a/data/tn.xlsx
+++ b/data/tn.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="ALL_AGE_FINAL"/>
   </sheets>
   <definedNames>
-    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$1959</definedName>
+    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$2009</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -347,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1959"/>
+  <dimension ref="A1:H2009"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -53940,6 +53940,1406 @@
         <v>0</v>
       </c>
       <c r="H1959" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1960">
+      <c r="A1960" s="1">
+        <v>44106</v>
+      </c>
+      <c r="B1960" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C1960" s="0">
+        <v>9807</v>
+      </c>
+      <c r="D1960" s="0">
+        <v>4.94296961235465E-02</v>
+      </c>
+      <c r="E1960" s="0">
+        <v>83</v>
+      </c>
+      <c r="F1960" s="0">
+        <v>8.54788877445932E-02</v>
+      </c>
+      <c r="G1960" s="0">
+        <v>5</v>
+      </c>
+      <c r="H1960" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1961">
+      <c r="A1961" s="1">
+        <v>44106</v>
+      </c>
+      <c r="B1961" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C1961" s="0">
+        <v>26497</v>
+      </c>
+      <c r="D1961" s="0">
+        <v>0.133551407992823</v>
+      </c>
+      <c r="E1961" s="0">
+        <v>147</v>
+      </c>
+      <c r="F1961" s="0">
+        <v>0.151390319258496</v>
+      </c>
+      <c r="G1961" s="0">
+        <v>2</v>
+      </c>
+      <c r="H1961" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1962">
+      <c r="A1962" s="1">
+        <v>44106</v>
+      </c>
+      <c r="B1962" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C1962" s="0">
+        <v>41277</v>
+      </c>
+      <c r="D1962" s="0">
+        <v>0.208046249300666</v>
+      </c>
+      <c r="E1962" s="0">
+        <v>136</v>
+      </c>
+      <c r="F1962" s="0">
+        <v>0.140061791967044</v>
+      </c>
+      <c r="G1962" s="0">
+        <v>19</v>
+      </c>
+      <c r="H1962" s="0">
+        <v>-1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1963">
+      <c r="A1963" s="1">
+        <v>44106</v>
+      </c>
+      <c r="B1963" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C1963" s="0">
+        <v>32958</v>
+      </c>
+      <c r="D1963" s="0">
+        <v>0.166116439771576</v>
+      </c>
+      <c r="E1963" s="0">
+        <v>150</v>
+      </c>
+      <c r="F1963" s="0">
+        <v>0.154479917610711</v>
+      </c>
+      <c r="G1963" s="0">
+        <v>37</v>
+      </c>
+      <c r="H1963" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1964">
+      <c r="A1964" s="1">
+        <v>44106</v>
+      </c>
+      <c r="B1964" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C1964" s="0">
+        <v>29544</v>
+      </c>
+      <c r="D1964" s="0">
+        <v>0.14890903867381</v>
+      </c>
+      <c r="E1964" s="0">
+        <v>115</v>
+      </c>
+      <c r="F1964" s="0">
+        <v>0.118434603501545</v>
+      </c>
+      <c r="G1964" s="0">
+        <v>107</v>
+      </c>
+      <c r="H1964" s="0">
+        <v>-2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1965">
+      <c r="A1965" s="1">
+        <v>44106</v>
+      </c>
+      <c r="B1965" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C1965" s="0">
+        <v>25564</v>
+      </c>
+      <c r="D1965" s="0">
+        <v>0.128848858132185</v>
+      </c>
+      <c r="E1965" s="0">
+        <v>144</v>
+      </c>
+      <c r="F1965" s="0">
+        <v>0.148300720906282</v>
+      </c>
+      <c r="G1965" s="0">
+        <v>253</v>
+      </c>
+      <c r="H1965" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1966">
+      <c r="A1966" s="1">
+        <v>44106</v>
+      </c>
+      <c r="B1966" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C1966" s="0">
+        <v>17188</v>
+      </c>
+      <c r="D1966" s="0">
+        <v>8.66317545601629E-02</v>
+      </c>
+      <c r="E1966" s="0">
+        <v>117</v>
+      </c>
+      <c r="F1966" s="0">
+        <v>0.120494335736354</v>
+      </c>
+      <c r="G1966" s="0">
+        <v>500</v>
+      </c>
+      <c r="H1966" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1967">
+      <c r="A1967" s="1">
+        <v>44106</v>
+      </c>
+      <c r="B1967" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C1967" s="0">
+        <v>9869</v>
+      </c>
+      <c r="D1967" s="0">
+        <v>4.97421913983156E-02</v>
+      </c>
+      <c r="E1967" s="0">
+        <v>63</v>
+      </c>
+      <c r="F1967" s="0">
+        <v>6.48815653964985E-02</v>
+      </c>
+      <c r="G1967" s="0">
+        <v>750</v>
+      </c>
+      <c r="H1967" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1968">
+      <c r="A1968" s="1">
+        <v>44106</v>
+      </c>
+      <c r="B1968" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C1968" s="0">
+        <v>5398</v>
+      </c>
+      <c r="D1968" s="0">
+        <v>2.72072498903746E-02</v>
+      </c>
+      <c r="E1968" s="0">
+        <v>41</v>
+      </c>
+      <c r="F1968" s="0">
+        <v>4.22245108135942E-02</v>
+      </c>
+      <c r="G1968" s="0">
+        <v>842</v>
+      </c>
+      <c r="H1968" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1969">
+      <c r="A1969" s="1">
+        <v>44106</v>
+      </c>
+      <c r="B1969" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C1969" s="0">
+        <v>301</v>
+      </c>
+      <c r="D1969" s="0">
+        <v>1.51711415653997E-03</v>
+      </c>
+      <c r="E1969" s="0">
+        <v>-25</v>
+      </c>
+      <c r="F1969" s="0">
+        <v>-2.57466529351184E-02</v>
+      </c>
+      <c r="G1969" s="0">
+        <v>0</v>
+      </c>
+      <c r="H1969" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1970">
+      <c r="A1970" s="1">
+        <v>44107</v>
+      </c>
+      <c r="B1970" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C1970" s="0">
+        <v>9879</v>
+      </c>
+      <c r="D1970" s="0">
+        <v>4.94952278363686E-02</v>
+      </c>
+      <c r="E1970" s="0">
+        <v>72</v>
+      </c>
+      <c r="F1970" s="0">
+        <v>6.04026845637584E-02</v>
+      </c>
+      <c r="G1970" s="0">
+        <v>5</v>
+      </c>
+      <c r="H1970" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1971">
+      <c r="A1971" s="1">
+        <v>44107</v>
+      </c>
+      <c r="B1971" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C1971" s="0">
+        <v>26654</v>
+      </c>
+      <c r="D1971" s="0">
+        <v>0.133540419349182</v>
+      </c>
+      <c r="E1971" s="0">
+        <v>157</v>
+      </c>
+      <c r="F1971" s="0">
+        <v>0.131711409395973</v>
+      </c>
+      <c r="G1971" s="0">
+        <v>1</v>
+      </c>
+      <c r="H1971" s="0">
+        <v>-1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1972">
+      <c r="A1972" s="1">
+        <v>44107</v>
+      </c>
+      <c r="B1972" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C1972" s="0">
+        <v>41482</v>
+      </c>
+      <c r="D1972" s="0">
+        <v>0.20783085748641</v>
+      </c>
+      <c r="E1972" s="0">
+        <v>205</v>
+      </c>
+      <c r="F1972" s="0">
+        <v>0.171979865771812</v>
+      </c>
+      <c r="G1972" s="0">
+        <v>19</v>
+      </c>
+      <c r="H1972" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1973">
+      <c r="A1973" s="1">
+        <v>44107</v>
+      </c>
+      <c r="B1973" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C1973" s="0">
+        <v>33113</v>
+      </c>
+      <c r="D1973" s="0">
+        <v>0.165900949422581</v>
+      </c>
+      <c r="E1973" s="0">
+        <v>155</v>
+      </c>
+      <c r="F1973" s="0">
+        <v>0.13003355704698</v>
+      </c>
+      <c r="G1973" s="0">
+        <v>38</v>
+      </c>
+      <c r="H1973" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1974">
+      <c r="A1974" s="1">
+        <v>44107</v>
+      </c>
+      <c r="B1974" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C1974" s="0">
+        <v>29712</v>
+      </c>
+      <c r="D1974" s="0">
+        <v>0.148861444424961</v>
+      </c>
+      <c r="E1974" s="0">
+        <v>168</v>
+      </c>
+      <c r="F1974" s="0">
+        <v>0.140939597315436</v>
+      </c>
+      <c r="G1974" s="0">
+        <v>107</v>
+      </c>
+      <c r="H1974" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1975">
+      <c r="A1975" s="1">
+        <v>44107</v>
+      </c>
+      <c r="B1975" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C1975" s="0">
+        <v>25716</v>
+      </c>
+      <c r="D1975" s="0">
+        <v>0.128840902828227</v>
+      </c>
+      <c r="E1975" s="0">
+        <v>152</v>
+      </c>
+      <c r="F1975" s="0">
+        <v>0.12751677852349</v>
+      </c>
+      <c r="G1975" s="0">
+        <v>258</v>
+      </c>
+      <c r="H1975" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1976">
+      <c r="A1976" s="1">
+        <v>44107</v>
+      </c>
+      <c r="B1976" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C1976" s="0">
+        <v>17306</v>
+      </c>
+      <c r="D1976" s="0">
+        <v>8.67055787970641E-02</v>
+      </c>
+      <c r="E1976" s="0">
+        <v>118</v>
+      </c>
+      <c r="F1976" s="0">
+        <v>0.098993288590604</v>
+      </c>
+      <c r="G1976" s="0">
+        <v>510</v>
+      </c>
+      <c r="H1976" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1977">
+      <c r="A1977" s="1">
+        <v>44107</v>
+      </c>
+      <c r="B1977" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C1977" s="0">
+        <v>9945</v>
+      </c>
+      <c r="D1977" s="0">
+        <v>4.98258974423207E-02</v>
+      </c>
+      <c r="E1977" s="0">
+        <v>76</v>
+      </c>
+      <c r="F1977" s="0">
+        <v>0.063758389261745</v>
+      </c>
+      <c r="G1977" s="0">
+        <v>758</v>
+      </c>
+      <c r="H1977" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1978">
+      <c r="A1978" s="1">
+        <v>44107</v>
+      </c>
+      <c r="B1978" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C1978" s="0">
+        <v>5436</v>
+      </c>
+      <c r="D1978" s="0">
+        <v>2.72351511811418E-02</v>
+      </c>
+      <c r="E1978" s="0">
+        <v>38</v>
+      </c>
+      <c r="F1978" s="0">
+        <v>3.18791946308725E-02</v>
+      </c>
+      <c r="G1978" s="0">
+        <v>864</v>
+      </c>
+      <c r="H1978" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1979">
+      <c r="A1979" s="1">
+        <v>44107</v>
+      </c>
+      <c r="B1979" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C1979" s="0">
+        <v>352</v>
+      </c>
+      <c r="D1979" s="0">
+        <v>1.76357123174428E-03</v>
+      </c>
+      <c r="E1979" s="0">
+        <v>51</v>
+      </c>
+      <c r="F1979" s="0">
+        <v>4.27852348993289E-02</v>
+      </c>
+      <c r="G1979" s="0">
+        <v>0</v>
+      </c>
+      <c r="H1979" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1980">
+      <c r="A1980" s="1">
+        <v>44108</v>
+      </c>
+      <c r="B1980" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C1980" s="0">
+        <v>9970</v>
+      </c>
+      <c r="D1980" s="0">
+        <v>4.95502211619701E-02</v>
+      </c>
+      <c r="E1980" s="0">
+        <v>91</v>
+      </c>
+      <c r="F1980" s="0">
+        <v>5.63467492260062E-02</v>
+      </c>
+      <c r="G1980" s="0">
+        <v>5</v>
+      </c>
+      <c r="H1980" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1981">
+      <c r="A1981" s="1">
+        <v>44108</v>
+      </c>
+      <c r="B1981" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C1981" s="0">
+        <v>26885</v>
+      </c>
+      <c r="D1981" s="0">
+        <v>0.133616619452314</v>
+      </c>
+      <c r="E1981" s="0">
+        <v>231</v>
+      </c>
+      <c r="F1981" s="0">
+        <v>0.143034055727554</v>
+      </c>
+      <c r="G1981" s="0">
+        <v>1</v>
+      </c>
+      <c r="H1981" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1982">
+      <c r="A1982" s="1">
+        <v>44108</v>
+      </c>
+      <c r="B1982" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C1982" s="0">
+        <v>41734</v>
+      </c>
+      <c r="D1982" s="0">
+        <v>0.207415138412604</v>
+      </c>
+      <c r="E1982" s="0">
+        <v>252</v>
+      </c>
+      <c r="F1982" s="0">
+        <v>0.156037151702786</v>
+      </c>
+      <c r="G1982" s="0">
+        <v>19</v>
+      </c>
+      <c r="H1982" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1983">
+      <c r="A1983" s="1">
+        <v>44108</v>
+      </c>
+      <c r="B1983" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C1983" s="0">
+        <v>33336</v>
+      </c>
+      <c r="D1983" s="0">
+        <v>0.165677650216192</v>
+      </c>
+      <c r="E1983" s="0">
+        <v>223</v>
+      </c>
+      <c r="F1983" s="0">
+        <v>0.138080495356037</v>
+      </c>
+      <c r="G1983" s="0">
+        <v>38</v>
+      </c>
+      <c r="H1983" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1984">
+      <c r="A1984" s="1">
+        <v>44108</v>
+      </c>
+      <c r="B1984" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C1984" s="0">
+        <v>29947</v>
+      </c>
+      <c r="D1984" s="0">
+        <v>0.148834550966652</v>
+      </c>
+      <c r="E1984" s="0">
+        <v>235</v>
+      </c>
+      <c r="F1984" s="0">
+        <v>0.145510835913313</v>
+      </c>
+      <c r="G1984" s="0">
+        <v>108</v>
+      </c>
+      <c r="H1984" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1985">
+      <c r="A1985" s="1">
+        <v>44108</v>
+      </c>
+      <c r="B1985" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C1985" s="0">
+        <v>25957</v>
+      </c>
+      <c r="D1985" s="0">
+        <v>0.12900452263804</v>
+      </c>
+      <c r="E1985" s="0">
+        <v>241</v>
+      </c>
+      <c r="F1985" s="0">
+        <v>0.14922600619195</v>
+      </c>
+      <c r="G1985" s="0">
+        <v>260</v>
+      </c>
+      <c r="H1985" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1986">
+      <c r="A1986" s="1">
+        <v>44108</v>
+      </c>
+      <c r="B1986" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C1986" s="0">
+        <v>17496</v>
+      </c>
+      <c r="D1986" s="0">
+        <v>8.69539287311764E-02</v>
+      </c>
+      <c r="E1986" s="0">
+        <v>190</v>
+      </c>
+      <c r="F1986" s="0">
+        <v>0.117647058823529</v>
+      </c>
+      <c r="G1986" s="0">
+        <v>513</v>
+      </c>
+      <c r="H1986" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1987">
+      <c r="A1987" s="1">
+        <v>44108</v>
+      </c>
+      <c r="B1987" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C1987" s="0">
+        <v>10055</v>
+      </c>
+      <c r="D1987" s="0">
+        <v>4.99726653744844E-02</v>
+      </c>
+      <c r="E1987" s="0">
+        <v>110</v>
+      </c>
+      <c r="F1987" s="0">
+        <v>6.81114551083591E-02</v>
+      </c>
+      <c r="G1987" s="0">
+        <v>763</v>
+      </c>
+      <c r="H1987" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1988">
+      <c r="A1988" s="1">
+        <v>44108</v>
+      </c>
+      <c r="B1988" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C1988" s="0">
+        <v>5497</v>
+      </c>
+      <c r="D1988" s="0">
+        <v>2.73197157198946E-02</v>
+      </c>
+      <c r="E1988" s="0">
+        <v>61</v>
+      </c>
+      <c r="F1988" s="0">
+        <v>3.77708978328173E-02</v>
+      </c>
+      <c r="G1988" s="0">
+        <v>870</v>
+      </c>
+      <c r="H1988" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1989">
+      <c r="A1989" s="1">
+        <v>44108</v>
+      </c>
+      <c r="B1989" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C1989" s="0">
+        <v>333</v>
+      </c>
+      <c r="D1989" s="0">
+        <v>1.65498732667362E-03</v>
+      </c>
+      <c r="E1989" s="0">
+        <v>-19</v>
+      </c>
+      <c r="F1989" s="0">
+        <v>-1.17647058823529E-02</v>
+      </c>
+      <c r="G1989" s="0">
+        <v>0</v>
+      </c>
+      <c r="H1989" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1990">
+      <c r="A1990" s="1">
+        <v>44109</v>
+      </c>
+      <c r="B1990" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C1990" s="0">
+        <v>10112</v>
+      </c>
+      <c r="D1990" s="0">
+        <v>4.96418735487165E-02</v>
+      </c>
+      <c r="E1990" s="0">
+        <v>142</v>
+      </c>
+      <c r="F1990" s="0">
+        <v>5.70510245078345E-02</v>
+      </c>
+      <c r="G1990" s="0">
+        <v>5</v>
+      </c>
+      <c r="H1990" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1991">
+      <c r="A1991" s="1">
+        <v>44109</v>
+      </c>
+      <c r="B1991" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C1991" s="0">
+        <v>27241</v>
+      </c>
+      <c r="D1991" s="0">
+        <v>0.133731633439536</v>
+      </c>
+      <c r="E1991" s="0">
+        <v>356</v>
+      </c>
+      <c r="F1991" s="0">
+        <v>0.14302932904781</v>
+      </c>
+      <c r="G1991" s="0">
+        <v>1</v>
+      </c>
+      <c r="H1991" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1992">
+      <c r="A1992" s="1">
+        <v>44109</v>
+      </c>
+      <c r="B1992" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C1992" s="0">
+        <v>42162</v>
+      </c>
+      <c r="D1992" s="0">
+        <v>0.206981870308642</v>
+      </c>
+      <c r="E1992" s="0">
+        <v>428</v>
+      </c>
+      <c r="F1992" s="0">
+        <v>0.171956609079952</v>
+      </c>
+      <c r="G1992" s="0">
+        <v>19</v>
+      </c>
+      <c r="H1992" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1993">
+      <c r="A1993" s="1">
+        <v>44109</v>
+      </c>
+      <c r="B1993" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C1993" s="0">
+        <v>33643</v>
+      </c>
+      <c r="D1993" s="0">
+        <v>0.165160359157384</v>
+      </c>
+      <c r="E1993" s="0">
+        <v>307</v>
+      </c>
+      <c r="F1993" s="0">
+        <v>0.123342707914825</v>
+      </c>
+      <c r="G1993" s="0">
+        <v>38</v>
+      </c>
+      <c r="H1993" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1994">
+      <c r="A1994" s="1">
+        <v>44109</v>
+      </c>
+      <c r="B1994" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C1994" s="0">
+        <v>30279</v>
+      </c>
+      <c r="D1994" s="0">
+        <v>0.148645796002926</v>
+      </c>
+      <c r="E1994" s="0">
+        <v>332</v>
+      </c>
+      <c r="F1994" s="0">
+        <v>0.13338690237043</v>
+      </c>
+      <c r="G1994" s="0">
+        <v>108</v>
+      </c>
+      <c r="H1994" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1995">
+      <c r="A1995" s="1">
+        <v>44109</v>
+      </c>
+      <c r="B1995" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C1995" s="0">
+        <v>26314</v>
+      </c>
+      <c r="D1995" s="0">
+        <v>0.129180801083952</v>
+      </c>
+      <c r="E1995" s="0">
+        <v>357</v>
+      </c>
+      <c r="F1995" s="0">
+        <v>0.143431096826035</v>
+      </c>
+      <c r="G1995" s="0">
+        <v>261</v>
+      </c>
+      <c r="H1995" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1996">
+      <c r="A1996" s="1">
+        <v>44109</v>
+      </c>
+      <c r="B1996" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C1996" s="0">
+        <v>17772</v>
+      </c>
+      <c r="D1996" s="0">
+        <v>0.087246378234552</v>
+      </c>
+      <c r="E1996" s="0">
+        <v>276</v>
+      </c>
+      <c r="F1996" s="0">
+        <v>0.110887906789875</v>
+      </c>
+      <c r="G1996" s="0">
+        <v>518</v>
+      </c>
+      <c r="H1996" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1997">
+      <c r="A1997" s="1">
+        <v>44109</v>
+      </c>
+      <c r="B1997" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C1997" s="0">
+        <v>10242</v>
+      </c>
+      <c r="D1997" s="0">
+        <v>5.02800701034369E-02</v>
+      </c>
+      <c r="E1997" s="0">
+        <v>187</v>
+      </c>
+      <c r="F1997" s="0">
+        <v>7.51305745279229E-02</v>
+      </c>
+      <c r="G1997" s="0">
+        <v>770</v>
+      </c>
+      <c r="H1997" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1998">
+      <c r="A1998" s="1">
+        <v>44109</v>
+      </c>
+      <c r="B1998" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C1998" s="0">
+        <v>5595</v>
+      </c>
+      <c r="D1998" s="0">
+        <v>2.74669978743146E-02</v>
+      </c>
+      <c r="E1998" s="0">
+        <v>98</v>
+      </c>
+      <c r="F1998" s="0">
+        <v>3.93732422659703E-02</v>
+      </c>
+      <c r="G1998" s="0">
+        <v>877</v>
+      </c>
+      <c r="H1998" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="1999">
+      <c r="A1999" s="1">
+        <v>44109</v>
+      </c>
+      <c r="B1999" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C1999" s="0">
+        <v>339</v>
+      </c>
+      <c r="D1999" s="0">
+        <v>1.66422024654024E-03</v>
+      </c>
+      <c r="E1999" s="0">
+        <v>6</v>
+      </c>
+      <c r="F1999" s="0">
+        <v>2.41060666934512E-03</v>
+      </c>
+      <c r="G1999" s="0">
+        <v>0</v>
+      </c>
+      <c r="H1999" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2000">
+      <c r="A2000" s="1">
+        <v>44110</v>
+      </c>
+      <c r="B2000" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2000" s="0">
+        <v>10181</v>
+      </c>
+      <c r="D2000" s="0">
+        <v>0.049572732805843</v>
+      </c>
+      <c r="E2000" s="0">
+        <v>69</v>
+      </c>
+      <c r="F2000" s="0">
+        <v>4.11694510739857E-02</v>
+      </c>
+      <c r="G2000" s="0">
+        <v>6</v>
+      </c>
+      <c r="H2000" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2001">
+      <c r="A2001" s="1">
+        <v>44110</v>
+      </c>
+      <c r="B2001" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2001" s="0">
+        <v>27436</v>
+      </c>
+      <c r="D2001" s="0">
+        <v>0.133589774802191</v>
+      </c>
+      <c r="E2001" s="0">
+        <v>195</v>
+      </c>
+      <c r="F2001" s="0">
+        <v>0.116348448687351</v>
+      </c>
+      <c r="G2001" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2001" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2002">
+      <c r="A2002" s="1">
+        <v>44110</v>
+      </c>
+      <c r="B2002" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2002" s="0">
+        <v>42463</v>
+      </c>
+      <c r="D2002" s="0">
+        <v>0.206758368837492</v>
+      </c>
+      <c r="E2002" s="0">
+        <v>301</v>
+      </c>
+      <c r="F2002" s="0">
+        <v>0.179594272076372</v>
+      </c>
+      <c r="G2002" s="0">
+        <v>19</v>
+      </c>
+      <c r="H2002" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2003">
+      <c r="A2003" s="1">
+        <v>44110</v>
+      </c>
+      <c r="B2003" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2003" s="0">
+        <v>33899</v>
+      </c>
+      <c r="D2003" s="0">
+        <v>0.165059038344492</v>
+      </c>
+      <c r="E2003" s="0">
+        <v>256</v>
+      </c>
+      <c r="F2003" s="0">
+        <v>0.152744630071599</v>
+      </c>
+      <c r="G2003" s="0">
+        <v>38</v>
+      </c>
+      <c r="H2003" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2004">
+      <c r="A2004" s="1">
+        <v>44110</v>
+      </c>
+      <c r="B2004" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2004" s="0">
+        <v>30520</v>
+      </c>
+      <c r="D2004" s="0">
+        <v>0.148606208155813</v>
+      </c>
+      <c r="E2004" s="0">
+        <v>241</v>
+      </c>
+      <c r="F2004" s="0">
+        <v>0.143794749403341</v>
+      </c>
+      <c r="G2004" s="0">
+        <v>108</v>
+      </c>
+      <c r="H2004" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2005">
+      <c r="A2005" s="1">
+        <v>44110</v>
+      </c>
+      <c r="B2005" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2005" s="0">
+        <v>26557</v>
+      </c>
+      <c r="D2005" s="0">
+        <v>0.1293097991479</v>
+      </c>
+      <c r="E2005" s="0">
+        <v>243</v>
+      </c>
+      <c r="F2005" s="0">
+        <v>0.144988066825776</v>
+      </c>
+      <c r="G2005" s="0">
+        <v>264</v>
+      </c>
+      <c r="H2005" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2006">
+      <c r="A2006" s="1">
+        <v>44110</v>
+      </c>
+      <c r="B2006" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2006" s="0">
+        <v>17952</v>
+      </c>
+      <c r="D2006" s="0">
+        <v>8.74108338405356E-02</v>
+      </c>
+      <c r="E2006" s="0">
+        <v>180</v>
+      </c>
+      <c r="F2006" s="0">
+        <v>0.107398568019093</v>
+      </c>
+      <c r="G2006" s="0">
+        <v>520</v>
+      </c>
+      <c r="H2006" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2007">
+      <c r="A2007" s="1">
+        <v>44110</v>
+      </c>
+      <c r="B2007" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2007" s="0">
+        <v>10370</v>
+      </c>
+      <c r="D2007" s="0">
+        <v>5.04930006086427E-02</v>
+      </c>
+      <c r="E2007" s="0">
+        <v>128</v>
+      </c>
+      <c r="F2007" s="0">
+        <v>7.63723150357995E-02</v>
+      </c>
+      <c r="G2007" s="0">
+        <v>778</v>
+      </c>
+      <c r="H2007" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2008">
+      <c r="A2008" s="1">
+        <v>44110</v>
+      </c>
+      <c r="B2008" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2008" s="0">
+        <v>5671</v>
+      </c>
+      <c r="D2008" s="0">
+        <v>2.76129032258065E-02</v>
+      </c>
+      <c r="E2008" s="0">
+        <v>76</v>
+      </c>
+      <c r="F2008" s="0">
+        <v>0.045346062052506</v>
+      </c>
+      <c r="G2008" s="0">
+        <v>887</v>
+      </c>
+      <c r="H2008" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2009">
+      <c r="A2009" s="1">
+        <v>44110</v>
+      </c>
+      <c r="B2009" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2009" s="0">
+        <v>326</v>
+      </c>
+      <c r="D2009" s="0">
+        <v>1.58734023128424E-03</v>
+      </c>
+      <c r="E2009" s="0">
+        <v>-13</v>
+      </c>
+      <c r="F2009" s="0">
+        <v>-7.75656324582339E-03</v>
+      </c>
+      <c r="G2009" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2009" s="0">
         <v>0</v>
       </c>
     </row>
@@ -54371,13 +55771,6 @@
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <Home xmlns="f83d9bd0-d5f5-484c-bfdf-0c10f1e052c8">false</Home>
-    <_dlc_DocId xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">HJYU5V3E37X6-122305290-700</_dlc_DocId>
-    <Present xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2">false</Present>
-    <_dlc_DocIdUrl xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">
-      <Url>https://tennessee.sharepoint.com/sites/health/PRG/COVID/_layouts/15/DocIdRedir.aspx?ID=HJYU5V3E37X6-122305290-700</Url>
-      <Description>HJYU5V3E37X6-122305290-700</Description>
-    </_dlc_DocIdUrl>
     <Project_x0020_ID xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2" xsi:nil="true"/>
     <Doc_x0020_Subject xmlns="2773c6ec-81e5-4cca-8f30-56e38046ef00" xsi:nil="true"/>
     <e67c2c055ae043d09da25150149f3d62 xmlns="2773c6ec-81e5-4cca-8f30-56e38046ef00">
@@ -54392,24 +55785,31 @@
     </Assigned_x0020_To0>
     <TaxCatchAll xmlns="2773c6ec-81e5-4cca-8f30-56e38046ef00"/>
     <Doc_x0020_Type xmlns="2773c6ec-81e5-4cca-8f30-56e38046ef00" xsi:nil="true"/>
+    <Home xmlns="f83d9bd0-d5f5-484c-bfdf-0c10f1e052c8">false</Home>
     <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Present xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2">false</Present>
+    <_dlc_DocId xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">HJYU5V3E37X6-122305290-773</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">
+      <Url>https://tennessee.sharepoint.com/sites/health/PRG/COVID/_layouts/15/DocIdRedir.aspx?ID=HJYU5V3E37X6-122305290-773</Url>
+      <Description>HJYU5V3E37X6-122305290-773</Description>
+    </_dlc_DocIdUrl>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8F0D409-07BE-4D6E-AB0A-12494333DE14}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{279B6548-5DFD-4AA2-8A87-B4E45B4FBB90}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33D5A2B7-6B3F-435F-BEE8-39428669A5D1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{670BC0FF-F22D-4D7E-896D-306073EE4DE3}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02A1DA1-5F8F-48A8-978D-1AFAE3E36E8F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC565563-0258-49E5-9D3D-1585337CD384}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79C17201-C9DC-4B1F-B53B-0436F6BB7069}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73FA42DF-142A-4C55-8023-63BAD999BA9B}"/>
 </file>
</xml_diff>

<commit_message>
update data from update data branch
</commit_message>
<xml_diff>
--- a/data/tn.xlsx
+++ b/data/tn.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="ALL_AGE_FINAL"/>
   </sheets>
   <definedNames>
-    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$2009</definedName>
+    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$2079</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -347,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2009"/>
+  <dimension ref="A1:H2079"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -55340,6 +55340,1966 @@
         <v>0</v>
       </c>
       <c r="H2009" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2010">
+      <c r="A2010" s="1">
+        <v>44111</v>
+      </c>
+      <c r="B2010" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2010" s="0">
+        <v>10289</v>
+      </c>
+      <c r="D2010" s="0">
+        <v>4.95962979923357E-02</v>
+      </c>
+      <c r="E2010" s="0">
+        <v>108</v>
+      </c>
+      <c r="F2010" s="0">
+        <v>5.19230769230769E-02</v>
+      </c>
+      <c r="G2010" s="0">
+        <v>5</v>
+      </c>
+      <c r="H2010" s="0">
+        <v>-1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2011">
+      <c r="A2011" s="1">
+        <v>44111</v>
+      </c>
+      <c r="B2011" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2011" s="0">
+        <v>27698</v>
+      </c>
+      <c r="D2011" s="0">
+        <v>0.133513292039237</v>
+      </c>
+      <c r="E2011" s="0">
+        <v>262</v>
+      </c>
+      <c r="F2011" s="0">
+        <v>0.125961538461538</v>
+      </c>
+      <c r="G2011" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2011" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2012">
+      <c r="A2012" s="1">
+        <v>44111</v>
+      </c>
+      <c r="B2012" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2012" s="0">
+        <v>42771</v>
+      </c>
+      <c r="D2012" s="0">
+        <v>0.206170012773855</v>
+      </c>
+      <c r="E2012" s="0">
+        <v>308</v>
+      </c>
+      <c r="F2012" s="0">
+        <v>0.148076923076923</v>
+      </c>
+      <c r="G2012" s="0">
+        <v>19</v>
+      </c>
+      <c r="H2012" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2013">
+      <c r="A2013" s="1">
+        <v>44111</v>
+      </c>
+      <c r="B2013" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2013" s="0">
+        <v>34155</v>
+      </c>
+      <c r="D2013" s="0">
+        <v>0.164638114289846</v>
+      </c>
+      <c r="E2013" s="0">
+        <v>256</v>
+      </c>
+      <c r="F2013" s="0">
+        <v>0.123076923076923</v>
+      </c>
+      <c r="G2013" s="0">
+        <v>38</v>
+      </c>
+      <c r="H2013" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2014">
+      <c r="A2014" s="1">
+        <v>44111</v>
+      </c>
+      <c r="B2014" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2014" s="0">
+        <v>30838</v>
+      </c>
+      <c r="D2014" s="0">
+        <v>0.148649104625099</v>
+      </c>
+      <c r="E2014" s="0">
+        <v>318</v>
+      </c>
+      <c r="F2014" s="0">
+        <v>0.152884615384615</v>
+      </c>
+      <c r="G2014" s="0">
+        <v>109</v>
+      </c>
+      <c r="H2014" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2015">
+      <c r="A2015" s="1">
+        <v>44111</v>
+      </c>
+      <c r="B2015" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2015" s="0">
+        <v>26924</v>
+      </c>
+      <c r="D2015" s="0">
+        <v>0.129782362440047</v>
+      </c>
+      <c r="E2015" s="0">
+        <v>367</v>
+      </c>
+      <c r="F2015" s="0">
+        <v>0.176442307692308</v>
+      </c>
+      <c r="G2015" s="0">
+        <v>266</v>
+      </c>
+      <c r="H2015" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2016">
+      <c r="A2016" s="1">
+        <v>44111</v>
+      </c>
+      <c r="B2016" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2016" s="0">
+        <v>18187</v>
+      </c>
+      <c r="D2016" s="0">
+        <v>8.76672049360102E-02</v>
+      </c>
+      <c r="E2016" s="0">
+        <v>235</v>
+      </c>
+      <c r="F2016" s="0">
+        <v>0.112980769230769</v>
+      </c>
+      <c r="G2016" s="0">
+        <v>525</v>
+      </c>
+      <c r="H2016" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2017">
+      <c r="A2017" s="1">
+        <v>44111</v>
+      </c>
+      <c r="B2017" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2017" s="0">
+        <v>10528</v>
+      </c>
+      <c r="D2017" s="0">
+        <v>5.07483550649538E-02</v>
+      </c>
+      <c r="E2017" s="0">
+        <v>158</v>
+      </c>
+      <c r="F2017" s="0">
+        <v>7.59615384615385E-02</v>
+      </c>
+      <c r="G2017" s="0">
+        <v>783</v>
+      </c>
+      <c r="H2017" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2018">
+      <c r="A2018" s="1">
+        <v>44111</v>
+      </c>
+      <c r="B2018" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2018" s="0">
+        <v>5742</v>
+      </c>
+      <c r="D2018" s="0">
+        <v>2.76782916777132E-02</v>
+      </c>
+      <c r="E2018" s="0">
+        <v>71</v>
+      </c>
+      <c r="F2018" s="0">
+        <v>3.41346153846154E-02</v>
+      </c>
+      <c r="G2018" s="0">
+        <v>896</v>
+      </c>
+      <c r="H2018" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2019">
+      <c r="A2019" s="1">
+        <v>44111</v>
+      </c>
+      <c r="B2019" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2019" s="0">
+        <v>323</v>
+      </c>
+      <c r="D2019" s="0">
+        <v>1.55696416090236E-03</v>
+      </c>
+      <c r="E2019" s="0">
+        <v>-3</v>
+      </c>
+      <c r="F2019" s="0">
+        <v>-1.44230769230769E-03</v>
+      </c>
+      <c r="G2019" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2019" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2020">
+      <c r="A2020" s="1">
+        <v>44112</v>
+      </c>
+      <c r="B2020" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2020" s="0">
+        <v>10378</v>
+      </c>
+      <c r="D2020" s="0">
+        <v>4.95495280428939E-02</v>
+      </c>
+      <c r="E2020" s="0">
+        <v>89</v>
+      </c>
+      <c r="F2020" s="0">
+        <v>4.46787148594378E-02</v>
+      </c>
+      <c r="G2020" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2020" s="0">
+        <v>-1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2021">
+      <c r="A2021" s="1">
+        <v>44112</v>
+      </c>
+      <c r="B2021" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2021" s="0">
+        <v>27954</v>
+      </c>
+      <c r="D2021" s="0">
+        <v>0.133465745510797</v>
+      </c>
+      <c r="E2021" s="0">
+        <v>256</v>
+      </c>
+      <c r="F2021" s="0">
+        <v>0.1285140562249</v>
+      </c>
+      <c r="G2021" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2021" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2022">
+      <c r="A2022" s="1">
+        <v>44112</v>
+      </c>
+      <c r="B2022" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2022" s="0">
+        <v>43092</v>
+      </c>
+      <c r="D2022" s="0">
+        <v>0.20574178670499</v>
+      </c>
+      <c r="E2022" s="0">
+        <v>321</v>
+      </c>
+      <c r="F2022" s="0">
+        <v>0.161144578313253</v>
+      </c>
+      <c r="G2022" s="0">
+        <v>19</v>
+      </c>
+      <c r="H2022" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2023">
+      <c r="A2023" s="1">
+        <v>44112</v>
+      </c>
+      <c r="B2023" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2023" s="0">
+        <v>34417</v>
+      </c>
+      <c r="D2023" s="0">
+        <v>0.164323193934504</v>
+      </c>
+      <c r="E2023" s="0">
+        <v>262</v>
+      </c>
+      <c r="F2023" s="0">
+        <v>0.131526104417671</v>
+      </c>
+      <c r="G2023" s="0">
+        <v>38</v>
+      </c>
+      <c r="H2023" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2024">
+      <c r="A2024" s="1">
+        <v>44112</v>
+      </c>
+      <c r="B2024" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2024" s="0">
+        <v>31130</v>
+      </c>
+      <c r="D2024" s="0">
+        <v>0.148629486218471</v>
+      </c>
+      <c r="E2024" s="0">
+        <v>292</v>
+      </c>
+      <c r="F2024" s="0">
+        <v>0.146586345381526</v>
+      </c>
+      <c r="G2024" s="0">
+        <v>111</v>
+      </c>
+      <c r="H2024" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2025">
+      <c r="A2025" s="1">
+        <v>44112</v>
+      </c>
+      <c r="B2025" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2025" s="0">
+        <v>27206</v>
+      </c>
+      <c r="D2025" s="0">
+        <v>0.129894436301308</v>
+      </c>
+      <c r="E2025" s="0">
+        <v>282</v>
+      </c>
+      <c r="F2025" s="0">
+        <v>0.141566265060241</v>
+      </c>
+      <c r="G2025" s="0">
+        <v>270</v>
+      </c>
+      <c r="H2025" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2026">
+      <c r="A2026" s="1">
+        <v>44112</v>
+      </c>
+      <c r="B2026" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2026" s="0">
+        <v>18445</v>
+      </c>
+      <c r="D2026" s="0">
+        <v>8.80652384612814E-02</v>
+      </c>
+      <c r="E2026" s="0">
+        <v>258</v>
+      </c>
+      <c r="F2026" s="0">
+        <v>0.129518072289157</v>
+      </c>
+      <c r="G2026" s="0">
+        <v>539</v>
+      </c>
+      <c r="H2026" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2027">
+      <c r="A2027" s="1">
+        <v>44112</v>
+      </c>
+      <c r="B2027" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2027" s="0">
+        <v>10682</v>
+      </c>
+      <c r="D2027" s="0">
+        <v>5.10009692189432E-02</v>
+      </c>
+      <c r="E2027" s="0">
+        <v>154</v>
+      </c>
+      <c r="F2027" s="0">
+        <v>7.73092369477912E-02</v>
+      </c>
+      <c r="G2027" s="0">
+        <v>802</v>
+      </c>
+      <c r="H2027" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2028">
+      <c r="A2028" s="1">
+        <v>44112</v>
+      </c>
+      <c r="B2028" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2028" s="0">
+        <v>5820</v>
+      </c>
+      <c r="D2028" s="0">
+        <v>2.77874593572598E-02</v>
+      </c>
+      <c r="E2028" s="0">
+        <v>78</v>
+      </c>
+      <c r="F2028" s="0">
+        <v>3.91566265060241E-02</v>
+      </c>
+      <c r="G2028" s="0">
+        <v>921</v>
+      </c>
+      <c r="H2028" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2029">
+      <c r="A2029" s="1">
+        <v>44112</v>
+      </c>
+      <c r="B2029" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2029" s="0">
+        <v>323</v>
+      </c>
+      <c r="D2029" s="0">
+        <v>1.54215624955239E-03</v>
+      </c>
+      <c r="E2029" s="0">
+        <v>0</v>
+      </c>
+      <c r="F2029" s="0">
+        <v>0</v>
+      </c>
+      <c r="G2029" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2029" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2030">
+      <c r="A2030" s="1">
+        <v>44113</v>
+      </c>
+      <c r="B2030" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2030" s="0">
+        <v>10443</v>
+      </c>
+      <c r="D2030" s="0">
+        <v>4.94921873148723E-02</v>
+      </c>
+      <c r="E2030" s="0">
+        <v>65</v>
+      </c>
+      <c r="F2030" s="0">
+        <v>4.17737789203085E-02</v>
+      </c>
+      <c r="G2030" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2030" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2031">
+      <c r="A2031" s="1">
+        <v>44113</v>
+      </c>
+      <c r="B2031" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2031" s="0">
+        <v>28158</v>
+      </c>
+      <c r="D2031" s="0">
+        <v>0.133448339597067</v>
+      </c>
+      <c r="E2031" s="0">
+        <v>204</v>
+      </c>
+      <c r="F2031" s="0">
+        <v>0.131105398457584</v>
+      </c>
+      <c r="G2031" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2031" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2032">
+      <c r="A2032" s="1">
+        <v>44113</v>
+      </c>
+      <c r="B2032" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2032" s="0">
+        <v>43390</v>
+      </c>
+      <c r="D2032" s="0">
+        <v>0.205636886679336</v>
+      </c>
+      <c r="E2032" s="0">
+        <v>298</v>
+      </c>
+      <c r="F2032" s="0">
+        <v>0.191516709511568</v>
+      </c>
+      <c r="G2032" s="0">
+        <v>19</v>
+      </c>
+      <c r="H2032" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2033">
+      <c r="A2033" s="1">
+        <v>44113</v>
+      </c>
+      <c r="B2033" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2033" s="0">
+        <v>34622</v>
+      </c>
+      <c r="D2033" s="0">
+        <v>0.164082975123576</v>
+      </c>
+      <c r="E2033" s="0">
+        <v>205</v>
+      </c>
+      <c r="F2033" s="0">
+        <v>0.131748071979434</v>
+      </c>
+      <c r="G2033" s="0">
+        <v>38</v>
+      </c>
+      <c r="H2033" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2034">
+      <c r="A2034" s="1">
+        <v>44113</v>
+      </c>
+      <c r="B2034" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2034" s="0">
+        <v>31341</v>
+      </c>
+      <c r="D2034" s="0">
+        <v>0.148533433173936</v>
+      </c>
+      <c r="E2034" s="0">
+        <v>211</v>
+      </c>
+      <c r="F2034" s="0">
+        <v>0.13560411311054</v>
+      </c>
+      <c r="G2034" s="0">
+        <v>112</v>
+      </c>
+      <c r="H2034" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2035">
+      <c r="A2035" s="1">
+        <v>44113</v>
+      </c>
+      <c r="B2035" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2035" s="0">
+        <v>27428</v>
+      </c>
+      <c r="D2035" s="0">
+        <v>0.129988673146827</v>
+      </c>
+      <c r="E2035" s="0">
+        <v>222</v>
+      </c>
+      <c r="F2035" s="0">
+        <v>0.1426735218509</v>
+      </c>
+      <c r="G2035" s="0">
+        <v>272</v>
+      </c>
+      <c r="H2035" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2036">
+      <c r="A2036" s="1">
+        <v>44113</v>
+      </c>
+      <c r="B2036" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2036" s="0">
+        <v>18610</v>
+      </c>
+      <c r="D2036" s="0">
+        <v>8.81977981355715E-02</v>
+      </c>
+      <c r="E2036" s="0">
+        <v>165</v>
+      </c>
+      <c r="F2036" s="0">
+        <v>0.106041131105398</v>
+      </c>
+      <c r="G2036" s="0">
+        <v>543</v>
+      </c>
+      <c r="H2036" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2037">
+      <c r="A2037" s="1">
+        <v>44113</v>
+      </c>
+      <c r="B2037" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2037" s="0">
+        <v>10795</v>
+      </c>
+      <c r="D2037" s="0">
+        <v>5.11604100415634E-02</v>
+      </c>
+      <c r="E2037" s="0">
+        <v>113</v>
+      </c>
+      <c r="F2037" s="0">
+        <v>7.26221079691517E-02</v>
+      </c>
+      <c r="G2037" s="0">
+        <v>813</v>
+      </c>
+      <c r="H2037" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2038">
+      <c r="A2038" s="1">
+        <v>44113</v>
+      </c>
+      <c r="B2038" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2038" s="0">
+        <v>5892</v>
+      </c>
+      <c r="D2038" s="0">
+        <v>2.79237735956361E-02</v>
+      </c>
+      <c r="E2038" s="0">
+        <v>72</v>
+      </c>
+      <c r="F2038" s="0">
+        <v>4.62724935732648E-02</v>
+      </c>
+      <c r="G2038" s="0">
+        <v>930</v>
+      </c>
+      <c r="H2038" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2039">
+      <c r="A2039" s="1">
+        <v>44113</v>
+      </c>
+      <c r="B2039" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2039" s="0">
+        <v>324</v>
+      </c>
+      <c r="D2039" s="0">
+        <v>1.53552319161339E-03</v>
+      </c>
+      <c r="E2039" s="0">
+        <v>1</v>
+      </c>
+      <c r="F2039" s="0">
+        <v>6.426735218509E-04</v>
+      </c>
+      <c r="G2039" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2039" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2040">
+      <c r="A2040" s="1">
+        <v>44114</v>
+      </c>
+      <c r="B2040" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2040" s="0">
+        <v>10525</v>
+      </c>
+      <c r="D2040" s="0">
+        <v>4.94947072405701E-02</v>
+      </c>
+      <c r="E2040" s="0">
+        <v>82</v>
+      </c>
+      <c r="F2040" s="0">
+        <v>4.98177399756987E-02</v>
+      </c>
+      <c r="G2040" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2040" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2041">
+      <c r="A2041" s="1">
+        <v>44114</v>
+      </c>
+      <c r="B2041" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2041" s="0">
+        <v>28356</v>
+      </c>
+      <c r="D2041" s="0">
+        <v>0.133346500571364</v>
+      </c>
+      <c r="E2041" s="0">
+        <v>198</v>
+      </c>
+      <c r="F2041" s="0">
+        <v>0.120291616038882</v>
+      </c>
+      <c r="G2041" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2041" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2042">
+      <c r="A2042" s="1">
+        <v>44114</v>
+      </c>
+      <c r="B2042" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2042" s="0">
+        <v>43674</v>
+      </c>
+      <c r="D2042" s="0">
+        <v>0.205380697769564</v>
+      </c>
+      <c r="E2042" s="0">
+        <v>284</v>
+      </c>
+      <c r="F2042" s="0">
+        <v>0.172539489671932</v>
+      </c>
+      <c r="G2042" s="0">
+        <v>19</v>
+      </c>
+      <c r="H2042" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2043">
+      <c r="A2043" s="1">
+        <v>44114</v>
+      </c>
+      <c r="B2043" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2043" s="0">
+        <v>34875</v>
+      </c>
+      <c r="D2043" s="0">
+        <v>0.164002652257946</v>
+      </c>
+      <c r="E2043" s="0">
+        <v>253</v>
+      </c>
+      <c r="F2043" s="0">
+        <v>0.153705953827461</v>
+      </c>
+      <c r="G2043" s="0">
+        <v>39</v>
+      </c>
+      <c r="H2043" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2044">
+      <c r="A2044" s="1">
+        <v>44114</v>
+      </c>
+      <c r="B2044" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2044" s="0">
+        <v>31608</v>
+      </c>
+      <c r="D2044" s="0">
+        <v>0.148639307027073</v>
+      </c>
+      <c r="E2044" s="0">
+        <v>267</v>
+      </c>
+      <c r="F2044" s="0">
+        <v>0.16221142162819</v>
+      </c>
+      <c r="G2044" s="0">
+        <v>112</v>
+      </c>
+      <c r="H2044" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2045">
+      <c r="A2045" s="1">
+        <v>44114</v>
+      </c>
+      <c r="B2045" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2045" s="0">
+        <v>27643</v>
+      </c>
+      <c r="D2045" s="0">
+        <v>0.129993557458535</v>
+      </c>
+      <c r="E2045" s="0">
+        <v>215</v>
+      </c>
+      <c r="F2045" s="0">
+        <v>0.130619684082625</v>
+      </c>
+      <c r="G2045" s="0">
+        <v>276</v>
+      </c>
+      <c r="H2045" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2046">
+      <c r="A2046" s="1">
+        <v>44114</v>
+      </c>
+      <c r="B2046" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2046" s="0">
+        <v>18763</v>
+      </c>
+      <c r="D2046" s="0">
+        <v>8.82346025610278E-02</v>
+      </c>
+      <c r="E2046" s="0">
+        <v>153</v>
+      </c>
+      <c r="F2046" s="0">
+        <v>9.29526123936816E-02</v>
+      </c>
+      <c r="G2046" s="0">
+        <v>546</v>
+      </c>
+      <c r="H2046" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2047">
+      <c r="A2047" s="1">
+        <v>44114</v>
+      </c>
+      <c r="B2047" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2047" s="0">
+        <v>10904</v>
+      </c>
+      <c r="D2047" s="0">
+        <v>5.12769869597318E-02</v>
+      </c>
+      <c r="E2047" s="0">
+        <v>109</v>
+      </c>
+      <c r="F2047" s="0">
+        <v>6.62211421628189E-02</v>
+      </c>
+      <c r="G2047" s="0">
+        <v>820</v>
+      </c>
+      <c r="H2047" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2048">
+      <c r="A2048" s="1">
+        <v>44114</v>
+      </c>
+      <c r="B2048" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2048" s="0">
+        <v>5972</v>
+      </c>
+      <c r="D2048" s="0">
+        <v>2.80838376855758E-02</v>
+      </c>
+      <c r="E2048" s="0">
+        <v>80</v>
+      </c>
+      <c r="F2048" s="0">
+        <v>4.86026731470231E-02</v>
+      </c>
+      <c r="G2048" s="0">
+        <v>941</v>
+      </c>
+      <c r="H2048" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2049">
+      <c r="A2049" s="1">
+        <v>44114</v>
+      </c>
+      <c r="B2049" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2049" s="0">
+        <v>329</v>
+      </c>
+      <c r="D2049" s="0">
+        <v>1.5471504686126E-03</v>
+      </c>
+      <c r="E2049" s="0">
+        <v>5</v>
+      </c>
+      <c r="F2049" s="0">
+        <v>3.03766707168894E-03</v>
+      </c>
+      <c r="G2049" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2049" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2050">
+      <c r="A2050" s="1">
+        <v>44115</v>
+      </c>
+      <c r="B2050" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2050" s="0">
+        <v>10627</v>
+      </c>
+      <c r="D2050" s="0">
+        <v>4.94930536473591E-02</v>
+      </c>
+      <c r="E2050" s="0">
+        <v>102</v>
+      </c>
+      <c r="F2050" s="0">
+        <v>4.93230174081238E-02</v>
+      </c>
+      <c r="G2050" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2050" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2051">
+      <c r="A2051" s="1">
+        <v>44115</v>
+      </c>
+      <c r="B2051" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2051" s="0">
+        <v>28598</v>
+      </c>
+      <c r="D2051" s="0">
+        <v>0.133189267733808</v>
+      </c>
+      <c r="E2051" s="0">
+        <v>242</v>
+      </c>
+      <c r="F2051" s="0">
+        <v>0.117021276595745</v>
+      </c>
+      <c r="G2051" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2051" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2052">
+      <c r="A2052" s="1">
+        <v>44115</v>
+      </c>
+      <c r="B2052" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2052" s="0">
+        <v>44027</v>
+      </c>
+      <c r="D2052" s="0">
+        <v>0.205046642790277</v>
+      </c>
+      <c r="E2052" s="0">
+        <v>353</v>
+      </c>
+      <c r="F2052" s="0">
+        <v>0.170696324951644</v>
+      </c>
+      <c r="G2052" s="0">
+        <v>19</v>
+      </c>
+      <c r="H2052" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2053">
+      <c r="A2053" s="1">
+        <v>44115</v>
+      </c>
+      <c r="B2053" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2053" s="0">
+        <v>35182</v>
+      </c>
+      <c r="D2053" s="0">
+        <v>0.163852885425933</v>
+      </c>
+      <c r="E2053" s="0">
+        <v>307</v>
+      </c>
+      <c r="F2053" s="0">
+        <v>0.148452611218569</v>
+      </c>
+      <c r="G2053" s="0">
+        <v>40</v>
+      </c>
+      <c r="H2053" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2054">
+      <c r="A2054" s="1">
+        <v>44115</v>
+      </c>
+      <c r="B2054" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2054" s="0">
+        <v>31892</v>
+      </c>
+      <c r="D2054" s="0">
+        <v>0.148530391166046</v>
+      </c>
+      <c r="E2054" s="0">
+        <v>284</v>
+      </c>
+      <c r="F2054" s="0">
+        <v>0.137330754352031</v>
+      </c>
+      <c r="G2054" s="0">
+        <v>112</v>
+      </c>
+      <c r="H2054" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2055">
+      <c r="A2055" s="1">
+        <v>44115</v>
+      </c>
+      <c r="B2055" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2055" s="0">
+        <v>27931</v>
+      </c>
+      <c r="D2055" s="0">
+        <v>0.130082853244038</v>
+      </c>
+      <c r="E2055" s="0">
+        <v>288</v>
+      </c>
+      <c r="F2055" s="0">
+        <v>0.13926499032882</v>
+      </c>
+      <c r="G2055" s="0">
+        <v>276</v>
+      </c>
+      <c r="H2055" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2056">
+      <c r="A2056" s="1">
+        <v>44115</v>
+      </c>
+      <c r="B2056" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2056" s="0">
+        <v>19001</v>
+      </c>
+      <c r="D2056" s="0">
+        <v>8.84932259672033E-02</v>
+      </c>
+      <c r="E2056" s="0">
+        <v>238</v>
+      </c>
+      <c r="F2056" s="0">
+        <v>0.115087040618956</v>
+      </c>
+      <c r="G2056" s="0">
+        <v>548</v>
+      </c>
+      <c r="H2056" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2057">
+      <c r="A2057" s="1">
+        <v>44115</v>
+      </c>
+      <c r="B2057" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2057" s="0">
+        <v>11067</v>
+      </c>
+      <c r="D2057" s="0">
+        <v>5.15422626061281E-02</v>
+      </c>
+      <c r="E2057" s="0">
+        <v>163</v>
+      </c>
+      <c r="F2057" s="0">
+        <v>7.88201160541586E-02</v>
+      </c>
+      <c r="G2057" s="0">
+        <v>821</v>
+      </c>
+      <c r="H2057" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2058">
+      <c r="A2058" s="1">
+        <v>44115</v>
+      </c>
+      <c r="B2058" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2058" s="0">
+        <v>6061</v>
+      </c>
+      <c r="D2058" s="0">
+        <v>2.82278534070428E-02</v>
+      </c>
+      <c r="E2058" s="0">
+        <v>89</v>
+      </c>
+      <c r="F2058" s="0">
+        <v>0.043036750483559</v>
+      </c>
+      <c r="G2058" s="0">
+        <v>946</v>
+      </c>
+      <c r="H2058" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2059">
+      <c r="A2059" s="1">
+        <v>44115</v>
+      </c>
+      <c r="B2059" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2059" s="0">
+        <v>331</v>
+      </c>
+      <c r="D2059" s="0">
+        <v>1.54156401216485E-03</v>
+      </c>
+      <c r="E2059" s="0">
+        <v>2</v>
+      </c>
+      <c r="F2059" s="0">
+        <v>9.67117988394584E-04</v>
+      </c>
+      <c r="G2059" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2059" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2060">
+      <c r="A2060" s="1">
+        <v>44116</v>
+      </c>
+      <c r="B2060" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2060" s="0">
+        <v>10733</v>
+      </c>
+      <c r="D2060" s="0">
+        <v>4.93058681930523E-02</v>
+      </c>
+      <c r="E2060" s="0">
+        <v>106</v>
+      </c>
+      <c r="F2060" s="0">
+        <v>3.57504215851602E-02</v>
+      </c>
+      <c r="G2060" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2060" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2061">
+      <c r="A2061" s="1">
+        <v>44116</v>
+      </c>
+      <c r="B2061" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2061" s="0">
+        <v>28974</v>
+      </c>
+      <c r="D2061" s="0">
+        <v>0.13310241545006</v>
+      </c>
+      <c r="E2061" s="0">
+        <v>376</v>
+      </c>
+      <c r="F2061" s="0">
+        <v>0.12681281618887</v>
+      </c>
+      <c r="G2061" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2061" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2062">
+      <c r="A2062" s="1">
+        <v>44116</v>
+      </c>
+      <c r="B2062" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2062" s="0">
+        <v>44554</v>
+      </c>
+      <c r="D2062" s="0">
+        <v>0.204674708979153</v>
+      </c>
+      <c r="E2062" s="0">
+        <v>527</v>
+      </c>
+      <c r="F2062" s="0">
+        <v>0.177740303541315</v>
+      </c>
+      <c r="G2062" s="0">
+        <v>19</v>
+      </c>
+      <c r="H2062" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2063">
+      <c r="A2063" s="1">
+        <v>44116</v>
+      </c>
+      <c r="B2063" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2063" s="0">
+        <v>35607</v>
+      </c>
+      <c r="D2063" s="0">
+        <v>0.163573469556509</v>
+      </c>
+      <c r="E2063" s="0">
+        <v>425</v>
+      </c>
+      <c r="F2063" s="0">
+        <v>0.143338954468803</v>
+      </c>
+      <c r="G2063" s="0">
+        <v>40</v>
+      </c>
+      <c r="H2063" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2064">
+      <c r="A2064" s="1">
+        <v>44116</v>
+      </c>
+      <c r="B2064" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2064" s="0">
+        <v>32325</v>
+      </c>
+      <c r="D2064" s="0">
+        <v>0.148496430573038</v>
+      </c>
+      <c r="E2064" s="0">
+        <v>433</v>
+      </c>
+      <c r="F2064" s="0">
+        <v>0.146037099494098</v>
+      </c>
+      <c r="G2064" s="0">
+        <v>113</v>
+      </c>
+      <c r="H2064" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2065">
+      <c r="A2065" s="1">
+        <v>44116</v>
+      </c>
+      <c r="B2065" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2065" s="0">
+        <v>28373</v>
+      </c>
+      <c r="D2065" s="0">
+        <v>0.13034150733639</v>
+      </c>
+      <c r="E2065" s="0">
+        <v>442</v>
+      </c>
+      <c r="F2065" s="0">
+        <v>0.149072512647555</v>
+      </c>
+      <c r="G2065" s="0">
+        <v>276</v>
+      </c>
+      <c r="H2065" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2066">
+      <c r="A2066" s="1">
+        <v>44116</v>
+      </c>
+      <c r="B2066" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2066" s="0">
+        <v>19334</v>
+      </c>
+      <c r="D2066" s="0">
+        <v>8.88176330610707E-02</v>
+      </c>
+      <c r="E2066" s="0">
+        <v>333</v>
+      </c>
+      <c r="F2066" s="0">
+        <v>0.112310286677909</v>
+      </c>
+      <c r="G2066" s="0">
+        <v>549</v>
+      </c>
+      <c r="H2066" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2067">
+      <c r="A2067" s="1">
+        <v>44116</v>
+      </c>
+      <c r="B2067" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2067" s="0">
+        <v>11292</v>
+      </c>
+      <c r="D2067" s="0">
+        <v>5.18738343087623E-02</v>
+      </c>
+      <c r="E2067" s="0">
+        <v>225</v>
+      </c>
+      <c r="F2067" s="0">
+        <v>0.075885328836425</v>
+      </c>
+      <c r="G2067" s="0">
+        <v>825</v>
+      </c>
+      <c r="H2067" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2068">
+      <c r="A2068" s="1">
+        <v>44116</v>
+      </c>
+      <c r="B2068" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2068" s="0">
+        <v>6162</v>
+      </c>
+      <c r="D2068" s="0">
+        <v>2.83073474150366E-02</v>
+      </c>
+      <c r="E2068" s="0">
+        <v>101</v>
+      </c>
+      <c r="F2068" s="0">
+        <v>3.40640809443508E-02</v>
+      </c>
+      <c r="G2068" s="0">
+        <v>947</v>
+      </c>
+      <c r="H2068" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2069">
+      <c r="A2069" s="1">
+        <v>44116</v>
+      </c>
+      <c r="B2069" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2069" s="0">
+        <v>328</v>
+      </c>
+      <c r="D2069" s="0">
+        <v>1.50678512692827E-03</v>
+      </c>
+      <c r="E2069" s="0">
+        <v>-3</v>
+      </c>
+      <c r="F2069" s="0">
+        <v>-1.01180438448567E-03</v>
+      </c>
+      <c r="G2069" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2069" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2070">
+      <c r="A2070" s="1">
+        <v>44117</v>
+      </c>
+      <c r="B2070" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2070" s="0">
+        <v>10774</v>
+      </c>
+      <c r="D2070" s="0">
+        <v>4.92347906356105E-02</v>
+      </c>
+      <c r="E2070" s="0">
+        <v>41</v>
+      </c>
+      <c r="F2070" s="0">
+        <v>0.035745422842197</v>
+      </c>
+      <c r="G2070" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2070" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2071">
+      <c r="A2071" s="1">
+        <v>44117</v>
+      </c>
+      <c r="B2071" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2071" s="0">
+        <v>29099</v>
+      </c>
+      <c r="D2071" s="0">
+        <v>0.132975976675852</v>
+      </c>
+      <c r="E2071" s="0">
+        <v>125</v>
+      </c>
+      <c r="F2071" s="0">
+        <v>0.108979947689625</v>
+      </c>
+      <c r="G2071" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2071" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2072">
+      <c r="A2072" s="1">
+        <v>44117</v>
+      </c>
+      <c r="B2072" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2072" s="0">
+        <v>44765</v>
+      </c>
+      <c r="D2072" s="0">
+        <v>0.20456612240608</v>
+      </c>
+      <c r="E2072" s="0">
+        <v>211</v>
+      </c>
+      <c r="F2072" s="0">
+        <v>0.183958151700087</v>
+      </c>
+      <c r="G2072" s="0">
+        <v>19</v>
+      </c>
+      <c r="H2072" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2073">
+      <c r="A2073" s="1">
+        <v>44117</v>
+      </c>
+      <c r="B2073" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2073" s="0">
+        <v>35790</v>
+      </c>
+      <c r="D2073" s="0">
+        <v>0.163552362803833</v>
+      </c>
+      <c r="E2073" s="0">
+        <v>183</v>
+      </c>
+      <c r="F2073" s="0">
+        <v>0.159546643417611</v>
+      </c>
+      <c r="G2073" s="0">
+        <v>40</v>
+      </c>
+      <c r="H2073" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2074">
+      <c r="A2074" s="1">
+        <v>44117</v>
+      </c>
+      <c r="B2074" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2074" s="0">
+        <v>32501</v>
+      </c>
+      <c r="D2074" s="0">
+        <v>0.148522362209762</v>
+      </c>
+      <c r="E2074" s="0">
+        <v>176</v>
+      </c>
+      <c r="F2074" s="0">
+        <v>0.153443766346992</v>
+      </c>
+      <c r="G2074" s="0">
+        <v>114</v>
+      </c>
+      <c r="H2074" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2075">
+      <c r="A2075" s="1">
+        <v>44117</v>
+      </c>
+      <c r="B2075" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2075" s="0">
+        <v>28535</v>
+      </c>
+      <c r="D2075" s="0">
+        <v>0.130398621754886</v>
+      </c>
+      <c r="E2075" s="0">
+        <v>162</v>
+      </c>
+      <c r="F2075" s="0">
+        <v>0.141238012205754</v>
+      </c>
+      <c r="G2075" s="0">
+        <v>279</v>
+      </c>
+      <c r="H2075" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2076">
+      <c r="A2076" s="1">
+        <v>44117</v>
+      </c>
+      <c r="B2076" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2076" s="0">
+        <v>19458</v>
+      </c>
+      <c r="D2076" s="0">
+        <v>8.89187447733162E-02</v>
+      </c>
+      <c r="E2076" s="0">
+        <v>124</v>
+      </c>
+      <c r="F2076" s="0">
+        <v>0.108108108108108</v>
+      </c>
+      <c r="G2076" s="0">
+        <v>554</v>
+      </c>
+      <c r="H2076" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2077">
+      <c r="A2077" s="1">
+        <v>44117</v>
+      </c>
+      <c r="B2077" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2077" s="0">
+        <v>11397</v>
+      </c>
+      <c r="D2077" s="0">
+        <v>5.20817624720672E-02</v>
+      </c>
+      <c r="E2077" s="0">
+        <v>105</v>
+      </c>
+      <c r="F2077" s="0">
+        <v>9.15431560592851E-02</v>
+      </c>
+      <c r="G2077" s="0">
+        <v>833</v>
+      </c>
+      <c r="H2077" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2078">
+      <c r="A2078" s="1">
+        <v>44117</v>
+      </c>
+      <c r="B2078" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2078" s="0">
+        <v>6186</v>
+      </c>
+      <c r="D2078" s="0">
+        <v>2.82686481225066E-02</v>
+      </c>
+      <c r="E2078" s="0">
+        <v>24</v>
+      </c>
+      <c r="F2078" s="0">
+        <v>0.020924149956408</v>
+      </c>
+      <c r="G2078" s="0">
+        <v>953</v>
+      </c>
+      <c r="H2078" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2079">
+      <c r="A2079" s="1">
+        <v>44117</v>
+      </c>
+      <c r="B2079" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2079" s="0">
+        <v>324</v>
+      </c>
+      <c r="D2079" s="0">
+        <v>1.48060814608667E-03</v>
+      </c>
+      <c r="E2079" s="0">
+        <v>-4</v>
+      </c>
+      <c r="F2079" s="0">
+        <v>-0.003487358326068</v>
+      </c>
+      <c r="G2079" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2079" s="0">
         <v>0</v>
       </c>
     </row>
@@ -55771,6 +57731,13 @@
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
+    <Home xmlns="f83d9bd0-d5f5-484c-bfdf-0c10f1e052c8">false</Home>
+    <_dlc_DocId xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">HJYU5V3E37X6-122305290-870</_dlc_DocId>
+    <Present xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2">false</Present>
+    <_dlc_DocIdUrl xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">
+      <Url>https://tennessee.sharepoint.com/sites/health/PRG/COVID/_layouts/15/DocIdRedir.aspx?ID=HJYU5V3E37X6-122305290-870</Url>
+      <Description>HJYU5V3E37X6-122305290-870</Description>
+    </_dlc_DocIdUrl>
     <Project_x0020_ID xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2" xsi:nil="true"/>
     <Doc_x0020_Subject xmlns="2773c6ec-81e5-4cca-8f30-56e38046ef00" xsi:nil="true"/>
     <e67c2c055ae043d09da25150149f3d62 xmlns="2773c6ec-81e5-4cca-8f30-56e38046ef00">
@@ -55785,31 +57752,24 @@
     </Assigned_x0020_To0>
     <TaxCatchAll xmlns="2773c6ec-81e5-4cca-8f30-56e38046ef00"/>
     <Doc_x0020_Type xmlns="2773c6ec-81e5-4cca-8f30-56e38046ef00" xsi:nil="true"/>
-    <Home xmlns="f83d9bd0-d5f5-484c-bfdf-0c10f1e052c8">false</Home>
     <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Present xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2">false</Present>
-    <_dlc_DocId xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">HJYU5V3E37X6-122305290-773</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">
-      <Url>https://tennessee.sharepoint.com/sites/health/PRG/COVID/_layouts/15/DocIdRedir.aspx?ID=HJYU5V3E37X6-122305290-773</Url>
-      <Description>HJYU5V3E37X6-122305290-773</Description>
-    </_dlc_DocIdUrl>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{279B6548-5DFD-4AA2-8A87-B4E45B4FBB90}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059E8A7C-A8A3-47B5-9B3C-2AF7248024E1}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{670BC0FF-F22D-4D7E-896D-306073EE4DE3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69142BE4-B42F-437F-A31C-C88CC2555FF0}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC565563-0258-49E5-9D3D-1585337CD384}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F5DA645-4445-4D61-8DC2-A6BFF98A6E51}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73FA42DF-142A-4C55-8023-63BAD999BA9B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2600D85-6200-4F35-B6E2-D841BA5472E0}"/>
 </file>
</xml_diff>

<commit_message>
update data from update_data branch
</commit_message>
<xml_diff>
--- a/data/tn.xlsx
+++ b/data/tn.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="ALL_AGE_FINAL"/>
   </sheets>
   <definedNames>
-    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$2229</definedName>
+    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$2249</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -347,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2229"/>
+  <dimension ref="A1:H2249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -61500,6 +61500,566 @@
         <v>0</v>
       </c>
       <c r="H2229" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2230">
+      <c r="A2230" s="1">
+        <v>44133</v>
+      </c>
+      <c r="B2230" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2230" s="0">
+        <v>12535</v>
+      </c>
+      <c r="D2230" s="0">
+        <v>4.87971037060106E-02</v>
+      </c>
+      <c r="E2230" s="0">
+        <v>142</v>
+      </c>
+      <c r="F2230" s="0">
+        <v>5.33834586466165E-02</v>
+      </c>
+      <c r="G2230" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2230" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2231">
+      <c r="A2231" s="1">
+        <v>44133</v>
+      </c>
+      <c r="B2231" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2231" s="0">
+        <v>33993</v>
+      </c>
+      <c r="D2231" s="0">
+        <v>0.132330270943631</v>
+      </c>
+      <c r="E2231" s="0">
+        <v>368</v>
+      </c>
+      <c r="F2231" s="0">
+        <v>0.138345864661654</v>
+      </c>
+      <c r="G2231" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2231" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2232">
+      <c r="A2232" s="1">
+        <v>44133</v>
+      </c>
+      <c r="B2232" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2232" s="0">
+        <v>51295</v>
+      </c>
+      <c r="D2232" s="0">
+        <v>0.199684677670508</v>
+      </c>
+      <c r="E2232" s="0">
+        <v>432</v>
+      </c>
+      <c r="F2232" s="0">
+        <v>0.162406015037594</v>
+      </c>
+      <c r="G2232" s="0">
+        <v>21</v>
+      </c>
+      <c r="H2232" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2233">
+      <c r="A2233" s="1">
+        <v>44133</v>
+      </c>
+      <c r="B2233" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2233" s="0">
+        <v>41311</v>
+      </c>
+      <c r="D2233" s="0">
+        <v>0.160818280909374</v>
+      </c>
+      <c r="E2233" s="0">
+        <v>368</v>
+      </c>
+      <c r="F2233" s="0">
+        <v>0.138345864661654</v>
+      </c>
+      <c r="G2233" s="0">
+        <v>46</v>
+      </c>
+      <c r="H2233" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2234">
+      <c r="A2234" s="1">
+        <v>44133</v>
+      </c>
+      <c r="B2234" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2234" s="0">
+        <v>38068</v>
+      </c>
+      <c r="D2234" s="0">
+        <v>0.148193709124883</v>
+      </c>
+      <c r="E2234" s="0">
+        <v>422</v>
+      </c>
+      <c r="F2234" s="0">
+        <v>0.158646616541353</v>
+      </c>
+      <c r="G2234" s="0">
+        <v>126</v>
+      </c>
+      <c r="H2234" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2235">
+      <c r="A2235" s="1">
+        <v>44133</v>
+      </c>
+      <c r="B2235" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2235" s="0">
+        <v>34130</v>
+      </c>
+      <c r="D2235" s="0">
+        <v>0.132863593895983</v>
+      </c>
+      <c r="E2235" s="0">
+        <v>388</v>
+      </c>
+      <c r="F2235" s="0">
+        <v>0.145864661654135</v>
+      </c>
+      <c r="G2235" s="0">
+        <v>317</v>
+      </c>
+      <c r="H2235" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2236">
+      <c r="A2236" s="1">
+        <v>44133</v>
+      </c>
+      <c r="B2236" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2236" s="0">
+        <v>23562</v>
+      </c>
+      <c r="D2236" s="0">
+        <v>9.17237620678916E-02</v>
+      </c>
+      <c r="E2236" s="0">
+        <v>283</v>
+      </c>
+      <c r="F2236" s="0">
+        <v>0.106390977443609</v>
+      </c>
+      <c r="G2236" s="0">
+        <v>648</v>
+      </c>
+      <c r="H2236" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2237">
+      <c r="A2237" s="1">
+        <v>44133</v>
+      </c>
+      <c r="B2237" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2237" s="0">
+        <v>14014</v>
+      </c>
+      <c r="D2237" s="0">
+        <v>5.45546558704453E-02</v>
+      </c>
+      <c r="E2237" s="0">
+        <v>182</v>
+      </c>
+      <c r="F2237" s="0">
+        <v>0.068421052631579</v>
+      </c>
+      <c r="G2237" s="0">
+        <v>970</v>
+      </c>
+      <c r="H2237" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2238">
+      <c r="A2238" s="1">
+        <v>44133</v>
+      </c>
+      <c r="B2238" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2238" s="0">
+        <v>7616</v>
+      </c>
+      <c r="D2238" s="0">
+        <v>2.96480847088135E-02</v>
+      </c>
+      <c r="E2238" s="0">
+        <v>79</v>
+      </c>
+      <c r="F2238" s="0">
+        <v>2.96992481203008E-02</v>
+      </c>
+      <c r="G2238" s="0">
+        <v>1130</v>
+      </c>
+      <c r="H2238" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2239">
+      <c r="A2239" s="1">
+        <v>44133</v>
+      </c>
+      <c r="B2239" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2239" s="0">
+        <v>356</v>
+      </c>
+      <c r="D2239" s="0">
+        <v>1.38586110246029E-03</v>
+      </c>
+      <c r="E2239" s="0">
+        <v>-4</v>
+      </c>
+      <c r="F2239" s="0">
+        <v>-1.50375939849624E-03</v>
+      </c>
+      <c r="G2239" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2239" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2240">
+      <c r="A2240" s="1">
+        <v>44134</v>
+      </c>
+      <c r="B2240" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2240" s="0">
+        <v>12674</v>
+      </c>
+      <c r="D2240" s="0">
+        <v>4.88423356764089E-02</v>
+      </c>
+      <c r="E2240" s="0">
+        <v>139</v>
+      </c>
+      <c r="F2240" s="0">
+        <v>5.32975460122699E-02</v>
+      </c>
+      <c r="G2240" s="0">
+        <v>5</v>
+      </c>
+      <c r="H2240" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2241">
+      <c r="A2241" s="1">
+        <v>44134</v>
+      </c>
+      <c r="B2241" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2241" s="0">
+        <v>34349</v>
+      </c>
+      <c r="D2241" s="0">
+        <v>0.132372209890245</v>
+      </c>
+      <c r="E2241" s="0">
+        <v>356</v>
+      </c>
+      <c r="F2241" s="0">
+        <v>0.136503067484663</v>
+      </c>
+      <c r="G2241" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2241" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2242">
+      <c r="A2242" s="1">
+        <v>44134</v>
+      </c>
+      <c r="B2242" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2242" s="0">
+        <v>51727</v>
+      </c>
+      <c r="D2242" s="0">
+        <v>0.199342551486003</v>
+      </c>
+      <c r="E2242" s="0">
+        <v>432</v>
+      </c>
+      <c r="F2242" s="0">
+        <v>0.165644171779141</v>
+      </c>
+      <c r="G2242" s="0">
+        <v>21</v>
+      </c>
+      <c r="H2242" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2243">
+      <c r="A2243" s="1">
+        <v>44134</v>
+      </c>
+      <c r="B2243" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2243" s="0">
+        <v>41704</v>
+      </c>
+      <c r="D2243" s="0">
+        <v>0.160716487853003</v>
+      </c>
+      <c r="E2243" s="0">
+        <v>393</v>
+      </c>
+      <c r="F2243" s="0">
+        <v>0.15069018404908</v>
+      </c>
+      <c r="G2243" s="0">
+        <v>46</v>
+      </c>
+      <c r="H2243" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2244">
+      <c r="A2244" s="1">
+        <v>44134</v>
+      </c>
+      <c r="B2244" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2244" s="0">
+        <v>38469</v>
+      </c>
+      <c r="D2244" s="0">
+        <v>0.148249630040696</v>
+      </c>
+      <c r="E2244" s="0">
+        <v>401</v>
+      </c>
+      <c r="F2244" s="0">
+        <v>0.153757668711656</v>
+      </c>
+      <c r="G2244" s="0">
+        <v>127</v>
+      </c>
+      <c r="H2244" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2245">
+      <c r="A2245" s="1">
+        <v>44134</v>
+      </c>
+      <c r="B2245" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2245" s="0">
+        <v>34482</v>
+      </c>
+      <c r="D2245" s="0">
+        <v>0.132884757676656</v>
+      </c>
+      <c r="E2245" s="0">
+        <v>352</v>
+      </c>
+      <c r="F2245" s="0">
+        <v>0.134969325153374</v>
+      </c>
+      <c r="G2245" s="0">
+        <v>324</v>
+      </c>
+      <c r="H2245" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2246">
+      <c r="A2246" s="1">
+        <v>44134</v>
+      </c>
+      <c r="B2246" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2246" s="0">
+        <v>23860</v>
+      </c>
+      <c r="D2246" s="0">
+        <v>0.091950302133432</v>
+      </c>
+      <c r="E2246" s="0">
+        <v>298</v>
+      </c>
+      <c r="F2246" s="0">
+        <v>0.114263803680982</v>
+      </c>
+      <c r="G2246" s="0">
+        <v>657</v>
+      </c>
+      <c r="H2246" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2247">
+      <c r="A2247" s="1">
+        <v>44134</v>
+      </c>
+      <c r="B2247" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2247" s="0">
+        <v>14181</v>
+      </c>
+      <c r="D2247" s="0">
+        <v>5.46499260081391E-02</v>
+      </c>
+      <c r="E2247" s="0">
+        <v>167</v>
+      </c>
+      <c r="F2247" s="0">
+        <v>6.40337423312883E-02</v>
+      </c>
+      <c r="G2247" s="0">
+        <v>999</v>
+      </c>
+      <c r="H2247" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2248">
+      <c r="A2248" s="1">
+        <v>44134</v>
+      </c>
+      <c r="B2248" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2248" s="0">
+        <v>7688</v>
+      </c>
+      <c r="D2248" s="0">
+        <v>2.96275743001603E-02</v>
+      </c>
+      <c r="E2248" s="0">
+        <v>72</v>
+      </c>
+      <c r="F2248" s="0">
+        <v>2.76073619631902E-02</v>
+      </c>
+      <c r="G2248" s="0">
+        <v>1161</v>
+      </c>
+      <c r="H2248" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2249">
+      <c r="A2249" s="1">
+        <v>44134</v>
+      </c>
+      <c r="B2249" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2249" s="0">
+        <v>354</v>
+      </c>
+      <c r="D2249" s="0">
+        <v>1.36422493525712E-03</v>
+      </c>
+      <c r="E2249" s="0">
+        <v>-2</v>
+      </c>
+      <c r="F2249" s="0">
+        <v>-7.66871165644172E-04</v>
+      </c>
+      <c r="G2249" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2249" s="0">
         <v>0</v>
       </c>
     </row>
@@ -61932,11 +62492,11 @@
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Home xmlns="f83d9bd0-d5f5-484c-bfdf-0c10f1e052c8">false</Home>
-    <_dlc_DocId xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">HJYU5V3E37X6-122305290-1146</_dlc_DocId>
+    <_dlc_DocId xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">HJYU5V3E37X6-122305290-1169</_dlc_DocId>
     <Present xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2">false</Present>
     <_dlc_DocIdUrl xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">
-      <Url>https://tennessee.sharepoint.com/sites/health/PRG/COVID/_layouts/15/DocIdRedir.aspx?ID=HJYU5V3E37X6-122305290-1146</Url>
-      <Description>HJYU5V3E37X6-122305290-1146</Description>
+      <Url>https://tennessee.sharepoint.com/sites/health/PRG/COVID/_layouts/15/DocIdRedir.aspx?ID=HJYU5V3E37X6-122305290-1169</Url>
+      <Description>HJYU5V3E37X6-122305290-1169</Description>
     </_dlc_DocIdUrl>
     <Project_x0020_ID xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2" xsi:nil="true"/>
     <Doc_x0020_Subject xmlns="2773c6ec-81e5-4cca-8f30-56e38046ef00" xsi:nil="true"/>
@@ -61959,17 +62519,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{639E6845-0142-43A6-9514-7494574381C5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0676BF-2703-417A-8948-C93620254169}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E06B6A4-F136-4EDD-B53E-7185BB9C71E0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27EB79C3-202B-44DD-971A-2E23424B4064}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE821E37-FE4E-4DDB-9F1A-50BF993942BC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B988423-51AA-4E44-B42E-DCABE31C8155}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9152AA7D-110E-4A4B-9D6A-48F34105B78D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CDFA6B2-8FB5-488B-807D-FE50A142CCB9}"/>
 </file>
</xml_diff>

<commit_message>
add data from update data
</commit_message>
<xml_diff>
--- a/data/tn.xlsx
+++ b/data/tn.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="ALL_AGE_FINAL"/>
   </sheets>
   <definedNames>
-    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$2249</definedName>
+    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$2309</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -347,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2249"/>
+  <dimension ref="A1:H2309"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -62060,6 +62060,1686 @@
         <v>0</v>
       </c>
       <c r="H2249" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2250">
+      <c r="A2250" s="1">
+        <v>44135</v>
+      </c>
+      <c r="B2250" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2250" s="0">
+        <v>12733</v>
+      </c>
+      <c r="D2250" s="0">
+        <v>4.88468266633931E-02</v>
+      </c>
+      <c r="E2250" s="0">
+        <v>59</v>
+      </c>
+      <c r="F2250" s="0">
+        <v>4.98310810810811E-02</v>
+      </c>
+      <c r="G2250" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2250" s="0">
+        <v>-1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2251">
+      <c r="A2251" s="1">
+        <v>44135</v>
+      </c>
+      <c r="B2251" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2251" s="0">
+        <v>34477</v>
+      </c>
+      <c r="D2251" s="0">
+        <v>0.132261999754481</v>
+      </c>
+      <c r="E2251" s="0">
+        <v>128</v>
+      </c>
+      <c r="F2251" s="0">
+        <v>0.108108108108108</v>
+      </c>
+      <c r="G2251" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2251" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2252">
+      <c r="A2252" s="1">
+        <v>44135</v>
+      </c>
+      <c r="B2252" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2252" s="0">
+        <v>51959</v>
+      </c>
+      <c r="D2252" s="0">
+        <v>0.199327123741714</v>
+      </c>
+      <c r="E2252" s="0">
+        <v>232</v>
+      </c>
+      <c r="F2252" s="0">
+        <v>0.195945945945946</v>
+      </c>
+      <c r="G2252" s="0">
+        <v>21</v>
+      </c>
+      <c r="H2252" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2253">
+      <c r="A2253" s="1">
+        <v>44135</v>
+      </c>
+      <c r="B2253" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2253" s="0">
+        <v>41866</v>
+      </c>
+      <c r="D2253" s="0">
+        <v>0.160607967100417</v>
+      </c>
+      <c r="E2253" s="0">
+        <v>162</v>
+      </c>
+      <c r="F2253" s="0">
+        <v>0.136824324324324</v>
+      </c>
+      <c r="G2253" s="0">
+        <v>46</v>
+      </c>
+      <c r="H2253" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2254">
+      <c r="A2254" s="1">
+        <v>44135</v>
+      </c>
+      <c r="B2254" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2254" s="0">
+        <v>38639</v>
+      </c>
+      <c r="D2254" s="0">
+        <v>0.148228424993862</v>
+      </c>
+      <c r="E2254" s="0">
+        <v>170</v>
+      </c>
+      <c r="F2254" s="0">
+        <v>0.143581081081081</v>
+      </c>
+      <c r="G2254" s="0">
+        <v>126</v>
+      </c>
+      <c r="H2254" s="0">
+        <v>-1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2255">
+      <c r="A2255" s="1">
+        <v>44135</v>
+      </c>
+      <c r="B2255" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2255" s="0">
+        <v>34644</v>
+      </c>
+      <c r="D2255" s="0">
+        <v>0.132902651608151</v>
+      </c>
+      <c r="E2255" s="0">
+        <v>162</v>
+      </c>
+      <c r="F2255" s="0">
+        <v>0.136824324324324</v>
+      </c>
+      <c r="G2255" s="0">
+        <v>325</v>
+      </c>
+      <c r="H2255" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2256">
+      <c r="A2256" s="1">
+        <v>44135</v>
+      </c>
+      <c r="B2256" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2256" s="0">
+        <v>24004</v>
+      </c>
+      <c r="D2256" s="0">
+        <v>9.20850724281856E-02</v>
+      </c>
+      <c r="E2256" s="0">
+        <v>144</v>
+      </c>
+      <c r="F2256" s="0">
+        <v>0.121621621621622</v>
+      </c>
+      <c r="G2256" s="0">
+        <v>657</v>
+      </c>
+      <c r="H2256" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2257">
+      <c r="A2257" s="1">
+        <v>44135</v>
+      </c>
+      <c r="B2257" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2257" s="0">
+        <v>14264</v>
+      </c>
+      <c r="D2257" s="0">
+        <v>5.47201080284802E-02</v>
+      </c>
+      <c r="E2257" s="0">
+        <v>83</v>
+      </c>
+      <c r="F2257" s="0">
+        <v>7.01013513513514E-02</v>
+      </c>
+      <c r="G2257" s="0">
+        <v>1003</v>
+      </c>
+      <c r="H2257" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2258">
+      <c r="A2258" s="1">
+        <v>44135</v>
+      </c>
+      <c r="B2258" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2258" s="0">
+        <v>7737</v>
+      </c>
+      <c r="D2258" s="0">
+        <v>0.029680978394304</v>
+      </c>
+      <c r="E2258" s="0">
+        <v>49</v>
+      </c>
+      <c r="F2258" s="0">
+        <v>4.13851351351351E-02</v>
+      </c>
+      <c r="G2258" s="0">
+        <v>1170</v>
+      </c>
+      <c r="H2258" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2259">
+      <c r="A2259" s="1">
+        <v>44135</v>
+      </c>
+      <c r="B2259" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2259" s="0">
+        <v>349</v>
+      </c>
+      <c r="D2259" s="0">
+        <v>1.33884728701203E-03</v>
+      </c>
+      <c r="E2259" s="0">
+        <v>-5</v>
+      </c>
+      <c r="F2259" s="0">
+        <v>-4.22297297297297E-03</v>
+      </c>
+      <c r="G2259" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2259" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2260">
+      <c r="A2260" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B2260" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2260" s="0">
+        <v>12759</v>
+      </c>
+      <c r="D2260" s="0">
+        <v>4.88053980858828E-02</v>
+      </c>
+      <c r="E2260" s="0">
+        <v>26</v>
+      </c>
+      <c r="F2260" s="0">
+        <v>3.44827586206897E-02</v>
+      </c>
+      <c r="G2260" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2260" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2261">
+      <c r="A2261" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B2261" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2261" s="0">
+        <v>34575</v>
+      </c>
+      <c r="D2261" s="0">
+        <v>0.132255399233435</v>
+      </c>
+      <c r="E2261" s="0">
+        <v>98</v>
+      </c>
+      <c r="F2261" s="0">
+        <v>0.129973474801061</v>
+      </c>
+      <c r="G2261" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2261" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2262">
+      <c r="A2262" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B2262" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2262" s="0">
+        <v>52109</v>
+      </c>
+      <c r="D2262" s="0">
+        <v>0.199326004299496</v>
+      </c>
+      <c r="E2262" s="0">
+        <v>150</v>
+      </c>
+      <c r="F2262" s="0">
+        <v>0.19893899204244</v>
+      </c>
+      <c r="G2262" s="0">
+        <v>21</v>
+      </c>
+      <c r="H2262" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2263">
+      <c r="A2263" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B2263" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2263" s="0">
+        <v>41970</v>
+      </c>
+      <c r="D2263" s="0">
+        <v>0.160542562713732</v>
+      </c>
+      <c r="E2263" s="0">
+        <v>104</v>
+      </c>
+      <c r="F2263" s="0">
+        <v>0.137931034482759</v>
+      </c>
+      <c r="G2263" s="0">
+        <v>46</v>
+      </c>
+      <c r="H2263" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2264">
+      <c r="A2264" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B2264" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2264" s="0">
+        <v>38761</v>
+      </c>
+      <c r="D2264" s="0">
+        <v>0.148267578588205</v>
+      </c>
+      <c r="E2264" s="0">
+        <v>122</v>
+      </c>
+      <c r="F2264" s="0">
+        <v>0.161803713527851</v>
+      </c>
+      <c r="G2264" s="0">
+        <v>126</v>
+      </c>
+      <c r="H2264" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2265">
+      <c r="A2265" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B2265" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2265" s="0">
+        <v>34754</v>
+      </c>
+      <c r="D2265" s="0">
+        <v>0.132940105421802</v>
+      </c>
+      <c r="E2265" s="0">
+        <v>110</v>
+      </c>
+      <c r="F2265" s="0">
+        <v>0.145888594164456</v>
+      </c>
+      <c r="G2265" s="0">
+        <v>325</v>
+      </c>
+      <c r="H2265" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2266">
+      <c r="A2266" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B2266" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2266" s="0">
+        <v>24062</v>
+      </c>
+      <c r="D2266" s="0">
+        <v>9.20413424831501E-02</v>
+      </c>
+      <c r="E2266" s="0">
+        <v>58</v>
+      </c>
+      <c r="F2266" s="0">
+        <v>7.69230769230769E-02</v>
+      </c>
+      <c r="G2266" s="0">
+        <v>657</v>
+      </c>
+      <c r="H2266" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2267">
+      <c r="A2267" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B2267" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2267" s="0">
+        <v>14313</v>
+      </c>
+      <c r="D2267" s="0">
+        <v>5.47497188496936E-02</v>
+      </c>
+      <c r="E2267" s="0">
+        <v>49</v>
+      </c>
+      <c r="F2267" s="0">
+        <v>6.49867374005305E-02</v>
+      </c>
+      <c r="G2267" s="0">
+        <v>1003</v>
+      </c>
+      <c r="H2267" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2268">
+      <c r="A2268" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B2268" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2268" s="0">
+        <v>7763</v>
+      </c>
+      <c r="D2268" s="0">
+        <v>2.96948275993972E-02</v>
+      </c>
+      <c r="E2268" s="0">
+        <v>26</v>
+      </c>
+      <c r="F2268" s="0">
+        <v>3.44827586206897E-02</v>
+      </c>
+      <c r="G2268" s="0">
+        <v>1170</v>
+      </c>
+      <c r="H2268" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2269">
+      <c r="A2269" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B2269" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2269" s="0">
+        <v>360</v>
+      </c>
+      <c r="D2269" s="0">
+        <v>1.37706272520713E-03</v>
+      </c>
+      <c r="E2269" s="0">
+        <v>11</v>
+      </c>
+      <c r="F2269" s="0">
+        <v>1.45888594164456E-02</v>
+      </c>
+      <c r="G2269" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2269" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2270">
+      <c r="A2270" s="1">
+        <v>44137</v>
+      </c>
+      <c r="B2270" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2270" s="0">
+        <v>12897</v>
+      </c>
+      <c r="D2270" s="0">
+        <v>0.048743891423237</v>
+      </c>
+      <c r="E2270" s="0">
+        <v>138</v>
+      </c>
+      <c r="F2270" s="0">
+        <v>4.36570705472952E-02</v>
+      </c>
+      <c r="G2270" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2270" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2271">
+      <c r="A2271" s="1">
+        <v>44137</v>
+      </c>
+      <c r="B2271" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2271" s="0">
+        <v>34987</v>
+      </c>
+      <c r="D2271" s="0">
+        <v>0.132232498195301</v>
+      </c>
+      <c r="E2271" s="0">
+        <v>412</v>
+      </c>
+      <c r="F2271" s="0">
+        <v>0.130338500474533</v>
+      </c>
+      <c r="G2271" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2271" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2272">
+      <c r="A2272" s="1">
+        <v>44137</v>
+      </c>
+      <c r="B2272" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2272" s="0">
+        <v>52661</v>
+      </c>
+      <c r="D2272" s="0">
+        <v>0.199030942563316</v>
+      </c>
+      <c r="E2272" s="0">
+        <v>552</v>
+      </c>
+      <c r="F2272" s="0">
+        <v>0.174628282189181</v>
+      </c>
+      <c r="G2272" s="0">
+        <v>22</v>
+      </c>
+      <c r="H2272" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2273">
+      <c r="A2273" s="1">
+        <v>44137</v>
+      </c>
+      <c r="B2273" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2273" s="0">
+        <v>42410</v>
+      </c>
+      <c r="D2273" s="0">
+        <v>0.160287542471852</v>
+      </c>
+      <c r="E2273" s="0">
+        <v>440</v>
+      </c>
+      <c r="F2273" s="0">
+        <v>0.139196456817463</v>
+      </c>
+      <c r="G2273" s="0">
+        <v>47</v>
+      </c>
+      <c r="H2273" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2274">
+      <c r="A2274" s="1">
+        <v>44137</v>
+      </c>
+      <c r="B2274" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2274" s="0">
+        <v>39212</v>
+      </c>
+      <c r="D2274" s="0">
+        <v>0.148200780839573</v>
+      </c>
+      <c r="E2274" s="0">
+        <v>451</v>
+      </c>
+      <c r="F2274" s="0">
+        <v>0.142676368237899</v>
+      </c>
+      <c r="G2274" s="0">
+        <v>127</v>
+      </c>
+      <c r="H2274" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2275">
+      <c r="A2275" s="1">
+        <v>44137</v>
+      </c>
+      <c r="B2275" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2275" s="0">
+        <v>35208</v>
+      </c>
+      <c r="D2275" s="0">
+        <v>0.133067762210539</v>
+      </c>
+      <c r="E2275" s="0">
+        <v>454</v>
+      </c>
+      <c r="F2275" s="0">
+        <v>0.143625434988928</v>
+      </c>
+      <c r="G2275" s="0">
+        <v>329</v>
+      </c>
+      <c r="H2275" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2276">
+      <c r="A2276" s="1">
+        <v>44137</v>
+      </c>
+      <c r="B2276" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2276" s="0">
+        <v>24394</v>
+      </c>
+      <c r="D2276" s="0">
+        <v>9.21965175915672E-02</v>
+      </c>
+      <c r="E2276" s="0">
+        <v>332</v>
+      </c>
+      <c r="F2276" s="0">
+        <v>0.105030053780449</v>
+      </c>
+      <c r="G2276" s="0">
+        <v>657</v>
+      </c>
+      <c r="H2276" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2277">
+      <c r="A2277" s="1">
+        <v>44137</v>
+      </c>
+      <c r="B2277" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2277" s="0">
+        <v>14566</v>
+      </c>
+      <c r="D2277" s="0">
+        <v>5.50518355021222E-02</v>
+      </c>
+      <c r="E2277" s="0">
+        <v>253</v>
+      </c>
+      <c r="F2277" s="0">
+        <v>8.00379626700411E-02</v>
+      </c>
+      <c r="G2277" s="0">
+        <v>1018</v>
+      </c>
+      <c r="H2277" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2278">
+      <c r="A2278" s="1">
+        <v>44137</v>
+      </c>
+      <c r="B2278" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2278" s="0">
+        <v>7892</v>
+      </c>
+      <c r="D2278" s="0">
+        <v>2.98276181369455E-02</v>
+      </c>
+      <c r="E2278" s="0">
+        <v>129</v>
+      </c>
+      <c r="F2278" s="0">
+        <v>4.08098702942107E-02</v>
+      </c>
+      <c r="G2278" s="0">
+        <v>1174</v>
+      </c>
+      <c r="H2278" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2279">
+      <c r="A2279" s="1">
+        <v>44137</v>
+      </c>
+      <c r="B2279" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2279" s="0">
+        <v>360</v>
+      </c>
+      <c r="D2279" s="0">
+        <v>1.36061106554744E-03</v>
+      </c>
+      <c r="E2279" s="0">
+        <v>0</v>
+      </c>
+      <c r="F2279" s="0">
+        <v>0</v>
+      </c>
+      <c r="G2279" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2279" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2280">
+      <c r="A2280" s="1">
+        <v>44138</v>
+      </c>
+      <c r="B2280" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2280" s="0">
+        <v>12972</v>
+      </c>
+      <c r="D2280" s="0">
+        <v>4.87015546803726E-02</v>
+      </c>
+      <c r="E2280" s="0">
+        <v>75</v>
+      </c>
+      <c r="F2280" s="0">
+        <v>4.23728813559322E-02</v>
+      </c>
+      <c r="G2280" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2280" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2281">
+      <c r="A2281" s="1">
+        <v>44138</v>
+      </c>
+      <c r="B2281" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2281" s="0">
+        <v>35233</v>
+      </c>
+      <c r="D2281" s="0">
+        <v>0.13227735708091</v>
+      </c>
+      <c r="E2281" s="0">
+        <v>246</v>
+      </c>
+      <c r="F2281" s="0">
+        <v>0.138983050847458</v>
+      </c>
+      <c r="G2281" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2281" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2282">
+      <c r="A2282" s="1">
+        <v>44138</v>
+      </c>
+      <c r="B2282" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2282" s="0">
+        <v>53003</v>
+      </c>
+      <c r="D2282" s="0">
+        <v>0.19899232984303</v>
+      </c>
+      <c r="E2282" s="0">
+        <v>342</v>
+      </c>
+      <c r="F2282" s="0">
+        <v>0.193220338983051</v>
+      </c>
+      <c r="G2282" s="0">
+        <v>22</v>
+      </c>
+      <c r="H2282" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2283">
+      <c r="A2283" s="1">
+        <v>44138</v>
+      </c>
+      <c r="B2283" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2283" s="0">
+        <v>42662</v>
+      </c>
+      <c r="D2283" s="0">
+        <v>0.160168495665592</v>
+      </c>
+      <c r="E2283" s="0">
+        <v>252</v>
+      </c>
+      <c r="F2283" s="0">
+        <v>0.142372881355932</v>
+      </c>
+      <c r="G2283" s="0">
+        <v>48</v>
+      </c>
+      <c r="H2283" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2284">
+      <c r="A2284" s="1">
+        <v>44138</v>
+      </c>
+      <c r="B2284" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2284" s="0">
+        <v>39476</v>
+      </c>
+      <c r="D2284" s="0">
+        <v>0.148207105501263</v>
+      </c>
+      <c r="E2284" s="0">
+        <v>264</v>
+      </c>
+      <c r="F2284" s="0">
+        <v>0.149152542372881</v>
+      </c>
+      <c r="G2284" s="0">
+        <v>128</v>
+      </c>
+      <c r="H2284" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2285">
+      <c r="A2285" s="1">
+        <v>44138</v>
+      </c>
+      <c r="B2285" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2285" s="0">
+        <v>35449</v>
+      </c>
+      <c r="D2285" s="0">
+        <v>0.133088298786966</v>
+      </c>
+      <c r="E2285" s="0">
+        <v>241</v>
+      </c>
+      <c r="F2285" s="0">
+        <v>0.136158192090395</v>
+      </c>
+      <c r="G2285" s="0">
+        <v>333</v>
+      </c>
+      <c r="H2285" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2286">
+      <c r="A2286" s="1">
+        <v>44138</v>
+      </c>
+      <c r="B2286" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2286" s="0">
+        <v>24574</v>
+      </c>
+      <c r="D2286" s="0">
+        <v>0.092259636502889</v>
+      </c>
+      <c r="E2286" s="0">
+        <v>180</v>
+      </c>
+      <c r="F2286" s="0">
+        <v>0.101694915254237</v>
+      </c>
+      <c r="G2286" s="0">
+        <v>673</v>
+      </c>
+      <c r="H2286" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2287">
+      <c r="A2287" s="1">
+        <v>44138</v>
+      </c>
+      <c r="B2287" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2287" s="0">
+        <v>14683</v>
+      </c>
+      <c r="D2287" s="0">
+        <v>5.51252642130674E-02</v>
+      </c>
+      <c r="E2287" s="0">
+        <v>117</v>
+      </c>
+      <c r="F2287" s="0">
+        <v>6.61016949152542E-02</v>
+      </c>
+      <c r="G2287" s="0">
+        <v>1046</v>
+      </c>
+      <c r="H2287" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2288">
+      <c r="A2288" s="1">
+        <v>44138</v>
+      </c>
+      <c r="B2288" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2288" s="0">
+        <v>7950</v>
+      </c>
+      <c r="D2288" s="0">
+        <v>2.98471600145669E-02</v>
+      </c>
+      <c r="E2288" s="0">
+        <v>58</v>
+      </c>
+      <c r="F2288" s="0">
+        <v>3.27683615819209E-02</v>
+      </c>
+      <c r="G2288" s="0">
+        <v>1199</v>
+      </c>
+      <c r="H2288" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2289">
+      <c r="A2289" s="1">
+        <v>44138</v>
+      </c>
+      <c r="B2289" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2289" s="0">
+        <v>355</v>
+      </c>
+      <c r="D2289" s="0">
+        <v>1.3327977113423E-03</v>
+      </c>
+      <c r="E2289" s="0">
+        <v>-5</v>
+      </c>
+      <c r="F2289" s="0">
+        <v>-2.82485875706215E-03</v>
+      </c>
+      <c r="G2289" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2289" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2290">
+      <c r="A2290" s="1">
+        <v>44139</v>
+      </c>
+      <c r="B2290" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2290" s="0">
+        <v>13158</v>
+      </c>
+      <c r="D2290" s="0">
+        <v>4.87690973380479E-02</v>
+      </c>
+      <c r="E2290" s="0">
+        <v>186</v>
+      </c>
+      <c r="F2290" s="0">
+        <v>5.39912917271408E-02</v>
+      </c>
+      <c r="G2290" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2290" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2291">
+      <c r="A2291" s="1">
+        <v>44139</v>
+      </c>
+      <c r="B2291" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2291" s="0">
+        <v>35703</v>
+      </c>
+      <c r="D2291" s="0">
+        <v>0.13233037560878</v>
+      </c>
+      <c r="E2291" s="0">
+        <v>470</v>
+      </c>
+      <c r="F2291" s="0">
+        <v>0.136429608127721</v>
+      </c>
+      <c r="G2291" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2291" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2292">
+      <c r="A2292" s="1">
+        <v>44139</v>
+      </c>
+      <c r="B2292" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2292" s="0">
+        <v>53579</v>
+      </c>
+      <c r="D2292" s="0">
+        <v>0.198586370745954</v>
+      </c>
+      <c r="E2292" s="0">
+        <v>576</v>
+      </c>
+      <c r="F2292" s="0">
+        <v>0.167198838896952</v>
+      </c>
+      <c r="G2292" s="0">
+        <v>22</v>
+      </c>
+      <c r="H2292" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2293">
+      <c r="A2293" s="1">
+        <v>44139</v>
+      </c>
+      <c r="B2293" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2293" s="0">
+        <v>43194</v>
+      </c>
+      <c r="D2293" s="0">
+        <v>0.160095180910445</v>
+      </c>
+      <c r="E2293" s="0">
+        <v>532</v>
+      </c>
+      <c r="F2293" s="0">
+        <v>0.154426705370102</v>
+      </c>
+      <c r="G2293" s="0">
+        <v>48</v>
+      </c>
+      <c r="H2293" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2294">
+      <c r="A2294" s="1">
+        <v>44139</v>
+      </c>
+      <c r="B2294" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2294" s="0">
+        <v>39991</v>
+      </c>
+      <c r="D2294" s="0">
+        <v>0.14822351205699</v>
+      </c>
+      <c r="E2294" s="0">
+        <v>515</v>
+      </c>
+      <c r="F2294" s="0">
+        <v>0.149492017416546</v>
+      </c>
+      <c r="G2294" s="0">
+        <v>128</v>
+      </c>
+      <c r="H2294" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2295">
+      <c r="A2295" s="1">
+        <v>44139</v>
+      </c>
+      <c r="B2295" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2295" s="0">
+        <v>35928</v>
+      </c>
+      <c r="D2295" s="0">
+        <v>0.133164320501701</v>
+      </c>
+      <c r="E2295" s="0">
+        <v>479</v>
+      </c>
+      <c r="F2295" s="0">
+        <v>0.139042089985486</v>
+      </c>
+      <c r="G2295" s="0">
+        <v>335</v>
+      </c>
+      <c r="H2295" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2296">
+      <c r="A2296" s="1">
+        <v>44139</v>
+      </c>
+      <c r="B2296" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2296" s="0">
+        <v>24936</v>
+      </c>
+      <c r="D2296" s="0">
+        <v>9.24233326661774E-02</v>
+      </c>
+      <c r="E2296" s="0">
+        <v>362</v>
+      </c>
+      <c r="F2296" s="0">
+        <v>0.105079825834543</v>
+      </c>
+      <c r="G2296" s="0">
+        <v>678</v>
+      </c>
+      <c r="H2296" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2297">
+      <c r="A2297" s="1">
+        <v>44139</v>
+      </c>
+      <c r="B2297" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2297" s="0">
+        <v>14933</v>
+      </c>
+      <c r="D2297" s="0">
+        <v>5.53479959377618E-02</v>
+      </c>
+      <c r="E2297" s="0">
+        <v>250</v>
+      </c>
+      <c r="F2297" s="0">
+        <v>7.25689404934688E-02</v>
+      </c>
+      <c r="G2297" s="0">
+        <v>1058</v>
+      </c>
+      <c r="H2297" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2298">
+      <c r="A2298" s="1">
+        <v>44139</v>
+      </c>
+      <c r="B2298" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2298" s="0">
+        <v>8017</v>
+      </c>
+      <c r="D2298" s="0">
+        <v>2.97143831402288E-02</v>
+      </c>
+      <c r="E2298" s="0">
+        <v>67</v>
+      </c>
+      <c r="F2298" s="0">
+        <v>1.94484760522496E-02</v>
+      </c>
+      <c r="G2298" s="0">
+        <v>1204</v>
+      </c>
+      <c r="H2298" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2299">
+      <c r="A2299" s="1">
+        <v>44139</v>
+      </c>
+      <c r="B2299" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2299" s="0">
+        <v>363</v>
+      </c>
+      <c r="D2299" s="0">
+        <v>1.34543109391331E-03</v>
+      </c>
+      <c r="E2299" s="0">
+        <v>8</v>
+      </c>
+      <c r="F2299" s="0">
+        <v>0.002322206095791</v>
+      </c>
+      <c r="G2299" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2299" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2300">
+      <c r="A2300" s="1">
+        <v>44140</v>
+      </c>
+      <c r="B2300" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2300" s="0">
+        <v>13265</v>
+      </c>
+      <c r="D2300" s="0">
+        <v>4.88094756246987E-02</v>
+      </c>
+      <c r="E2300" s="0">
+        <v>107</v>
+      </c>
+      <c r="F2300" s="0">
+        <v>5.43423057389538E-02</v>
+      </c>
+      <c r="G2300" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2300" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2301">
+      <c r="A2301" s="1">
+        <v>44140</v>
+      </c>
+      <c r="B2301" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2301" s="0">
+        <v>35946</v>
+      </c>
+      <c r="D2301" s="0">
+        <v>0.132265767870744</v>
+      </c>
+      <c r="E2301" s="0">
+        <v>243</v>
+      </c>
+      <c r="F2301" s="0">
+        <v>0.123412899949213</v>
+      </c>
+      <c r="G2301" s="0">
+        <v>2</v>
+      </c>
+      <c r="H2301" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2302">
+      <c r="A2302" s="1">
+        <v>44140</v>
+      </c>
+      <c r="B2302" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2302" s="0">
+        <v>53919</v>
+      </c>
+      <c r="D2302" s="0">
+        <v>0.198398651806116</v>
+      </c>
+      <c r="E2302" s="0">
+        <v>340</v>
+      </c>
+      <c r="F2302" s="0">
+        <v>0.172676485525648</v>
+      </c>
+      <c r="G2302" s="0">
+        <v>22</v>
+      </c>
+      <c r="H2302" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2303">
+      <c r="A2303" s="1">
+        <v>44140</v>
+      </c>
+      <c r="B2303" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2303" s="0">
+        <v>43487</v>
+      </c>
+      <c r="D2303" s="0">
+        <v>0.160013393629195</v>
+      </c>
+      <c r="E2303" s="0">
+        <v>293</v>
+      </c>
+      <c r="F2303" s="0">
+        <v>0.148806500761808</v>
+      </c>
+      <c r="G2303" s="0">
+        <v>49</v>
+      </c>
+      <c r="H2303" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2304">
+      <c r="A2304" s="1">
+        <v>44140</v>
+      </c>
+      <c r="B2304" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2304" s="0">
+        <v>40269</v>
+      </c>
+      <c r="D2304" s="0">
+        <v>0.148172542324236</v>
+      </c>
+      <c r="E2304" s="0">
+        <v>278</v>
+      </c>
+      <c r="F2304" s="0">
+        <v>0.141188420518029</v>
+      </c>
+      <c r="G2304" s="0">
+        <v>128</v>
+      </c>
+      <c r="H2304" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2305">
+      <c r="A2305" s="1">
+        <v>44140</v>
+      </c>
+      <c r="B2305" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2305" s="0">
+        <v>36234</v>
+      </c>
+      <c r="D2305" s="0">
+        <v>0.133325483587285</v>
+      </c>
+      <c r="E2305" s="0">
+        <v>306</v>
+      </c>
+      <c r="F2305" s="0">
+        <v>0.155408836973083</v>
+      </c>
+      <c r="G2305" s="0">
+        <v>340</v>
+      </c>
+      <c r="H2305" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2306">
+      <c r="A2306" s="1">
+        <v>44140</v>
+      </c>
+      <c r="B2306" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2306" s="0">
+        <v>25157</v>
+      </c>
+      <c r="D2306" s="0">
+        <v>9.25669037535278E-02</v>
+      </c>
+      <c r="E2306" s="0">
+        <v>221</v>
+      </c>
+      <c r="F2306" s="0">
+        <v>0.112239715591671</v>
+      </c>
+      <c r="G2306" s="0">
+        <v>681</v>
+      </c>
+      <c r="H2306" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2307">
+      <c r="A2307" s="1">
+        <v>44140</v>
+      </c>
+      <c r="B2307" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2307" s="0">
+        <v>15057</v>
+      </c>
+      <c r="D2307" s="0">
+        <v>5.54032623053968E-02</v>
+      </c>
+      <c r="E2307" s="0">
+        <v>124</v>
+      </c>
+      <c r="F2307" s="0">
+        <v>6.29761300152362E-02</v>
+      </c>
+      <c r="G2307" s="0">
+        <v>1068</v>
+      </c>
+      <c r="H2307" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2308">
+      <c r="A2308" s="1">
+        <v>44140</v>
+      </c>
+      <c r="B2308" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2308" s="0">
+        <v>8071</v>
+      </c>
+      <c r="D2308" s="0">
+        <v>2.96977970423629E-02</v>
+      </c>
+      <c r="E2308" s="0">
+        <v>54</v>
+      </c>
+      <c r="F2308" s="0">
+        <v>2.74250888776028E-02</v>
+      </c>
+      <c r="G2308" s="0">
+        <v>1215</v>
+      </c>
+      <c r="H2308" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2309">
+      <c r="A2309" s="1">
+        <v>44140</v>
+      </c>
+      <c r="B2309" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2309" s="0">
+        <v>366</v>
+      </c>
+      <c r="D2309" s="0">
+        <v>1.34672205643722E-03</v>
+      </c>
+      <c r="E2309" s="0">
+        <v>3</v>
+      </c>
+      <c r="F2309" s="0">
+        <v>1.52361604875571E-03</v>
+      </c>
+      <c r="G2309" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2309" s="0">
         <v>0</v>
       </c>
     </row>
@@ -62492,11 +64172,11 @@
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Home xmlns="f83d9bd0-d5f5-484c-bfdf-0c10f1e052c8">false</Home>
-    <_dlc_DocId xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">HJYU5V3E37X6-122305290-1169</_dlc_DocId>
+    <_dlc_DocId xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">HJYU5V3E37X6-122305290-1295</_dlc_DocId>
     <Present xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2">false</Present>
     <_dlc_DocIdUrl xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">
-      <Url>https://tennessee.sharepoint.com/sites/health/PRG/COVID/_layouts/15/DocIdRedir.aspx?ID=HJYU5V3E37X6-122305290-1169</Url>
-      <Description>HJYU5V3E37X6-122305290-1169</Description>
+      <Url>https://tennessee.sharepoint.com/sites/health/PRG/COVID/_layouts/15/DocIdRedir.aspx?ID=HJYU5V3E37X6-122305290-1295</Url>
+      <Description>HJYU5V3E37X6-122305290-1295</Description>
     </_dlc_DocIdUrl>
     <Project_x0020_ID xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2" xsi:nil="true"/>
     <Doc_x0020_Subject xmlns="2773c6ec-81e5-4cca-8f30-56e38046ef00" xsi:nil="true"/>
@@ -62519,17 +64199,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0676BF-2703-417A-8948-C93620254169}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8CC401A-B7C6-46E3-BA8D-AE9B9F9D90D7}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27EB79C3-202B-44DD-971A-2E23424B4064}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32755B54-2489-4E74-B58B-F717CE6479DE}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B988423-51AA-4E44-B42E-DCABE31C8155}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE36221C-A317-4BEC-B0AD-1721A835E070}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CDFA6B2-8FB5-488B-807D-FE50A142CCB9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C63240-A0F9-4DD8-981A-15082435354B}"/>
 </file>
</xml_diff>

<commit_message>
processed data for 2020-11-26
</commit_message>
<xml_diff>
--- a/data/tn.xlsx
+++ b/data/tn.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="ALL_AGE_FINAL"/>
   </sheets>
   <definedNames>
-    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$2479</definedName>
+    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$2519</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -347,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2479"/>
+  <dimension ref="A1:H2519"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -68500,6 +68500,1126 @@
         <v>0</v>
       </c>
       <c r="H2479" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2480">
+      <c r="A2480" s="1">
+        <v>44158</v>
+      </c>
+      <c r="B2480" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2480" s="0">
+        <v>16983</v>
+      </c>
+      <c r="D2480" s="0">
+        <v>4.92903787548977E-02</v>
+      </c>
+      <c r="E2480" s="0">
+        <v>231</v>
+      </c>
+      <c r="F2480" s="0">
+        <v>5.67010309278351E-02</v>
+      </c>
+      <c r="G2480" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2480" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2481">
+      <c r="A2481" s="1">
+        <v>44158</v>
+      </c>
+      <c r="B2481" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2481" s="0">
+        <v>45947</v>
+      </c>
+      <c r="D2481" s="0">
+        <v>0.133353649687999</v>
+      </c>
+      <c r="E2481" s="0">
+        <v>574</v>
+      </c>
+      <c r="F2481" s="0">
+        <v>0.140893470790378</v>
+      </c>
+      <c r="G2481" s="0">
+        <v>2</v>
+      </c>
+      <c r="H2481" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2482">
+      <c r="A2482" s="1">
+        <v>44158</v>
+      </c>
+      <c r="B2482" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2482" s="0">
+        <v>66533</v>
+      </c>
+      <c r="D2482" s="0">
+        <v>0.19310114642287</v>
+      </c>
+      <c r="E2482" s="0">
+        <v>709</v>
+      </c>
+      <c r="F2482" s="0">
+        <v>0.174030436917035</v>
+      </c>
+      <c r="G2482" s="0">
+        <v>27</v>
+      </c>
+      <c r="H2482" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2483">
+      <c r="A2483" s="1">
+        <v>44158</v>
+      </c>
+      <c r="B2483" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2483" s="0">
+        <v>54441</v>
+      </c>
+      <c r="D2483" s="0">
+        <v>0.1580060949064</v>
+      </c>
+      <c r="E2483" s="0">
+        <v>584</v>
+      </c>
+      <c r="F2483" s="0">
+        <v>0.143348060873834</v>
+      </c>
+      <c r="G2483" s="0">
+        <v>57</v>
+      </c>
+      <c r="H2483" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2484">
+      <c r="A2484" s="1">
+        <v>44158</v>
+      </c>
+      <c r="B2484" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2484" s="0">
+        <v>51173</v>
+      </c>
+      <c r="D2484" s="0">
+        <v>0.148521259613989</v>
+      </c>
+      <c r="E2484" s="0">
+        <v>591</v>
+      </c>
+      <c r="F2484" s="0">
+        <v>0.145066273932253</v>
+      </c>
+      <c r="G2484" s="0">
+        <v>147</v>
+      </c>
+      <c r="H2484" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2485">
+      <c r="A2485" s="1">
+        <v>44158</v>
+      </c>
+      <c r="B2485" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2485" s="0">
+        <v>46422</v>
+      </c>
+      <c r="D2485" s="0">
+        <v>0.134732259468872</v>
+      </c>
+      <c r="E2485" s="0">
+        <v>644</v>
+      </c>
+      <c r="F2485" s="0">
+        <v>0.15807560137457</v>
+      </c>
+      <c r="G2485" s="0">
+        <v>399</v>
+      </c>
+      <c r="H2485" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2486">
+      <c r="A2486" s="1">
+        <v>44158</v>
+      </c>
+      <c r="B2486" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2486" s="0">
+        <v>32571</v>
+      </c>
+      <c r="D2486" s="0">
+        <v>9.45319982585982E-02</v>
+      </c>
+      <c r="E2486" s="0">
+        <v>396</v>
+      </c>
+      <c r="F2486" s="0">
+        <v>9.72017673048601E-02</v>
+      </c>
+      <c r="G2486" s="0">
+        <v>818</v>
+      </c>
+      <c r="H2486" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2487">
+      <c r="A2487" s="1">
+        <v>44158</v>
+      </c>
+      <c r="B2487" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2487" s="0">
+        <v>19489</v>
+      </c>
+      <c r="D2487" s="0">
+        <v>5.65636337251487E-02</v>
+      </c>
+      <c r="E2487" s="0">
+        <v>228</v>
+      </c>
+      <c r="F2487" s="0">
+        <v>5.59646539027982E-02</v>
+      </c>
+      <c r="G2487" s="0">
+        <v>1298</v>
+      </c>
+      <c r="H2487" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2488">
+      <c r="A2488" s="1">
+        <v>44158</v>
+      </c>
+      <c r="B2488" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2488" s="0">
+        <v>10482</v>
+      </c>
+      <c r="D2488" s="0">
+        <v>3.04222899434044E-02</v>
+      </c>
+      <c r="E2488" s="0">
+        <v>102</v>
+      </c>
+      <c r="F2488" s="0">
+        <v>2.50368188512518E-02</v>
+      </c>
+      <c r="G2488" s="0">
+        <v>1549</v>
+      </c>
+      <c r="H2488" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2489">
+      <c r="A2489" s="1">
+        <v>44158</v>
+      </c>
+      <c r="B2489" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2489" s="0">
+        <v>509</v>
+      </c>
+      <c r="D2489" s="0">
+        <v>1.47728921782035E-03</v>
+      </c>
+      <c r="E2489" s="0">
+        <v>15</v>
+      </c>
+      <c r="F2489" s="0">
+        <v>3.68188512518409E-03</v>
+      </c>
+      <c r="G2489" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2489" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2490">
+      <c r="A2490" s="1">
+        <v>44159</v>
+      </c>
+      <c r="B2490" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2490" s="0">
+        <v>17049</v>
+      </c>
+      <c r="D2490" s="0">
+        <v>4.92953674093693E-02</v>
+      </c>
+      <c r="E2490" s="0">
+        <v>66</v>
+      </c>
+      <c r="F2490" s="0">
+        <v>5.06134969325153E-02</v>
+      </c>
+      <c r="G2490" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2490" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2491">
+      <c r="A2491" s="1">
+        <v>44159</v>
+      </c>
+      <c r="B2491" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2491" s="0">
+        <v>46115</v>
+      </c>
+      <c r="D2491" s="0">
+        <v>0.133336610245942</v>
+      </c>
+      <c r="E2491" s="0">
+        <v>168</v>
+      </c>
+      <c r="F2491" s="0">
+        <v>0.128834355828221</v>
+      </c>
+      <c r="G2491" s="0">
+        <v>2</v>
+      </c>
+      <c r="H2491" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2492">
+      <c r="A2492" s="1">
+        <v>44159</v>
+      </c>
+      <c r="B2492" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2492" s="0">
+        <v>66742</v>
+      </c>
+      <c r="D2492" s="0">
+        <v>0.192977383520214</v>
+      </c>
+      <c r="E2492" s="0">
+        <v>209</v>
+      </c>
+      <c r="F2492" s="0">
+        <v>0.160276073619632</v>
+      </c>
+      <c r="G2492" s="0">
+        <v>27</v>
+      </c>
+      <c r="H2492" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2493">
+      <c r="A2493" s="1">
+        <v>44159</v>
+      </c>
+      <c r="B2493" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2493" s="0">
+        <v>54617</v>
+      </c>
+      <c r="D2493" s="0">
+        <v>0.157919237597368</v>
+      </c>
+      <c r="E2493" s="0">
+        <v>176</v>
+      </c>
+      <c r="F2493" s="0">
+        <v>0.134969325153374</v>
+      </c>
+      <c r="G2493" s="0">
+        <v>58</v>
+      </c>
+      <c r="H2493" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2494">
+      <c r="A2494" s="1">
+        <v>44159</v>
+      </c>
+      <c r="B2494" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2494" s="0">
+        <v>51371</v>
+      </c>
+      <c r="D2494" s="0">
+        <v>0.148533774367219</v>
+      </c>
+      <c r="E2494" s="0">
+        <v>198</v>
+      </c>
+      <c r="F2494" s="0">
+        <v>0.151840490797546</v>
+      </c>
+      <c r="G2494" s="0">
+        <v>148</v>
+      </c>
+      <c r="H2494" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2495">
+      <c r="A2495" s="1">
+        <v>44159</v>
+      </c>
+      <c r="B2495" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2495" s="0">
+        <v>46606</v>
+      </c>
+      <c r="D2495" s="0">
+        <v>0.134756284443725</v>
+      </c>
+      <c r="E2495" s="0">
+        <v>184</v>
+      </c>
+      <c r="F2495" s="0">
+        <v>0.141104294478528</v>
+      </c>
+      <c r="G2495" s="0">
+        <v>403</v>
+      </c>
+      <c r="H2495" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2496">
+      <c r="A2496" s="1">
+        <v>44159</v>
+      </c>
+      <c r="B2496" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2496" s="0">
+        <v>32723</v>
+      </c>
+      <c r="D2496" s="0">
+        <v>9.46150687862508E-02</v>
+      </c>
+      <c r="E2496" s="0">
+        <v>152</v>
+      </c>
+      <c r="F2496" s="0">
+        <v>0.116564417177914</v>
+      </c>
+      <c r="G2496" s="0">
+        <v>828</v>
+      </c>
+      <c r="H2496" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2497">
+      <c r="A2497" s="1">
+        <v>44159</v>
+      </c>
+      <c r="B2497" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2497" s="0">
+        <v>19601</v>
+      </c>
+      <c r="D2497" s="0">
+        <v>5.66742035656664E-02</v>
+      </c>
+      <c r="E2497" s="0">
+        <v>112</v>
+      </c>
+      <c r="F2497" s="0">
+        <v>8.58895705521472E-02</v>
+      </c>
+      <c r="G2497" s="0">
+        <v>1317</v>
+      </c>
+      <c r="H2497" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2498">
+      <c r="A2498" s="1">
+        <v>44159</v>
+      </c>
+      <c r="B2498" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2498" s="0">
+        <v>10527</v>
+      </c>
+      <c r="D2498" s="0">
+        <v>3.04376991447258E-02</v>
+      </c>
+      <c r="E2498" s="0">
+        <v>45</v>
+      </c>
+      <c r="F2498" s="0">
+        <v>3.45092024539877E-02</v>
+      </c>
+      <c r="G2498" s="0">
+        <v>1587</v>
+      </c>
+      <c r="H2498" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2499">
+      <c r="A2499" s="1">
+        <v>44159</v>
+      </c>
+      <c r="B2499" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2499" s="0">
+        <v>503</v>
+      </c>
+      <c r="D2499" s="0">
+        <v>1.45437091952095E-03</v>
+      </c>
+      <c r="E2499" s="0">
+        <v>-6</v>
+      </c>
+      <c r="F2499" s="0">
+        <v>-4.60122699386503E-03</v>
+      </c>
+      <c r="G2499" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2499" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2500">
+      <c r="A2500" s="1">
+        <v>44160</v>
+      </c>
+      <c r="B2500" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2500" s="0">
+        <v>17157</v>
+      </c>
+      <c r="D2500" s="0">
+        <v>4.93056912625154E-02</v>
+      </c>
+      <c r="E2500" s="0">
+        <v>108</v>
+      </c>
+      <c r="F2500" s="0">
+        <v>5.09915014164306E-02</v>
+      </c>
+      <c r="G2500" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2500" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2501">
+      <c r="A2501" s="1">
+        <v>44160</v>
+      </c>
+      <c r="B2501" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2501" s="0">
+        <v>46433</v>
+      </c>
+      <c r="D2501" s="0">
+        <v>0.133438897382548</v>
+      </c>
+      <c r="E2501" s="0">
+        <v>318</v>
+      </c>
+      <c r="F2501" s="0">
+        <v>0.15014164305949</v>
+      </c>
+      <c r="G2501" s="0">
+        <v>2</v>
+      </c>
+      <c r="H2501" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2502">
+      <c r="A2502" s="1">
+        <v>44160</v>
+      </c>
+      <c r="B2502" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2502" s="0">
+        <v>67048</v>
+      </c>
+      <c r="D2502" s="0">
+        <v>0.192682169829756</v>
+      </c>
+      <c r="E2502" s="0">
+        <v>306</v>
+      </c>
+      <c r="F2502" s="0">
+        <v>0.144475920679887</v>
+      </c>
+      <c r="G2502" s="0">
+        <v>27</v>
+      </c>
+      <c r="H2502" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2503">
+      <c r="A2503" s="1">
+        <v>44160</v>
+      </c>
+      <c r="B2503" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2503" s="0">
+        <v>54878</v>
+      </c>
+      <c r="D2503" s="0">
+        <v>0.157708091455634</v>
+      </c>
+      <c r="E2503" s="0">
+        <v>261</v>
+      </c>
+      <c r="F2503" s="0">
+        <v>0.123229461756374</v>
+      </c>
+      <c r="G2503" s="0">
+        <v>58</v>
+      </c>
+      <c r="H2503" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2504">
+      <c r="A2504" s="1">
+        <v>44160</v>
+      </c>
+      <c r="B2504" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2504" s="0">
+        <v>51682</v>
+      </c>
+      <c r="D2504" s="0">
+        <v>0.148523444415068</v>
+      </c>
+      <c r="E2504" s="0">
+        <v>311</v>
+      </c>
+      <c r="F2504" s="0">
+        <v>0.146836638338055</v>
+      </c>
+      <c r="G2504" s="0">
+        <v>150</v>
+      </c>
+      <c r="H2504" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2505">
+      <c r="A2505" s="1">
+        <v>44160</v>
+      </c>
+      <c r="B2505" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2505" s="0">
+        <v>46902</v>
+      </c>
+      <c r="D2505" s="0">
+        <v>0.134786706976423</v>
+      </c>
+      <c r="E2505" s="0">
+        <v>296</v>
+      </c>
+      <c r="F2505" s="0">
+        <v>0.139754485363551</v>
+      </c>
+      <c r="G2505" s="0">
+        <v>416</v>
+      </c>
+      <c r="H2505" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2506">
+      <c r="A2506" s="1">
+        <v>44160</v>
+      </c>
+      <c r="B2506" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2506" s="0">
+        <v>32937</v>
+      </c>
+      <c r="D2506" s="0">
+        <v>9.46541675767016E-02</v>
+      </c>
+      <c r="E2506" s="0">
+        <v>214</v>
+      </c>
+      <c r="F2506" s="0">
+        <v>0.101038715769594</v>
+      </c>
+      <c r="G2506" s="0">
+        <v>843</v>
+      </c>
+      <c r="H2506" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2507">
+      <c r="A2507" s="1">
+        <v>44160</v>
+      </c>
+      <c r="B2507" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2507" s="0">
+        <v>19787</v>
+      </c>
+      <c r="D2507" s="0">
+        <v>5.68637706482131E-02</v>
+      </c>
+      <c r="E2507" s="0">
+        <v>186</v>
+      </c>
+      <c r="F2507" s="0">
+        <v>8.78186968838527E-02</v>
+      </c>
+      <c r="G2507" s="0">
+        <v>1339</v>
+      </c>
+      <c r="H2507" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2508">
+      <c r="A2508" s="1">
+        <v>44160</v>
+      </c>
+      <c r="B2508" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2508" s="0">
+        <v>10647</v>
+      </c>
+      <c r="D2508" s="0">
+        <v>3.05972894370811E-02</v>
+      </c>
+      <c r="E2508" s="0">
+        <v>120</v>
+      </c>
+      <c r="F2508" s="0">
+        <v>0.056657223796034</v>
+      </c>
+      <c r="G2508" s="0">
+        <v>1626</v>
+      </c>
+      <c r="H2508" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2509">
+      <c r="A2509" s="1">
+        <v>44160</v>
+      </c>
+      <c r="B2509" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2509" s="0">
+        <v>501</v>
+      </c>
+      <c r="D2509" s="0">
+        <v>1.43977101605876E-03</v>
+      </c>
+      <c r="E2509" s="0">
+        <v>-2</v>
+      </c>
+      <c r="F2509" s="0">
+        <v>-9.44287063267233E-04</v>
+      </c>
+      <c r="G2509" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2509" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2510">
+      <c r="A2510" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B2510" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2510" s="0">
+        <v>17372</v>
+      </c>
+      <c r="D2510" s="0">
+        <v>4.92996117783277E-02</v>
+      </c>
+      <c r="E2510" s="0">
+        <v>215</v>
+      </c>
+      <c r="F2510" s="0">
+        <v>0.048819255222525</v>
+      </c>
+      <c r="G2510" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2510" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2511">
+      <c r="A2511" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B2511" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2511" s="0">
+        <v>47002</v>
+      </c>
+      <c r="D2511" s="0">
+        <v>0.133385928667106</v>
+      </c>
+      <c r="E2511" s="0">
+        <v>569</v>
+      </c>
+      <c r="F2511" s="0">
+        <v>0.129200726612171</v>
+      </c>
+      <c r="G2511" s="0">
+        <v>2</v>
+      </c>
+      <c r="H2511" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2512">
+      <c r="A2512" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B2512" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2512" s="0">
+        <v>67824</v>
+      </c>
+      <c r="D2512" s="0">
+        <v>0.192476218584694</v>
+      </c>
+      <c r="E2512" s="0">
+        <v>776</v>
+      </c>
+      <c r="F2512" s="0">
+        <v>0.176203451407811</v>
+      </c>
+      <c r="G2512" s="0">
+        <v>28</v>
+      </c>
+      <c r="H2512" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2513">
+      <c r="A2513" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B2513" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2513" s="0">
+        <v>55525</v>
+      </c>
+      <c r="D2513" s="0">
+        <v>0.157573160487661</v>
+      </c>
+      <c r="E2513" s="0">
+        <v>647</v>
+      </c>
+      <c r="F2513" s="0">
+        <v>0.146911898274296</v>
+      </c>
+      <c r="G2513" s="0">
+        <v>58</v>
+      </c>
+      <c r="H2513" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2514">
+      <c r="A2514" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B2514" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2514" s="0">
+        <v>52304</v>
+      </c>
+      <c r="D2514" s="0">
+        <v>0.14843235634663</v>
+      </c>
+      <c r="E2514" s="0">
+        <v>622</v>
+      </c>
+      <c r="F2514" s="0">
+        <v>0.141235240690282</v>
+      </c>
+      <c r="G2514" s="0">
+        <v>153</v>
+      </c>
+      <c r="H2514" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2515">
+      <c r="A2515" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B2515" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2515" s="0">
+        <v>47513</v>
+      </c>
+      <c r="D2515" s="0">
+        <v>0.134836084182805</v>
+      </c>
+      <c r="E2515" s="0">
+        <v>611</v>
+      </c>
+      <c r="F2515" s="0">
+        <v>0.138737511353315</v>
+      </c>
+      <c r="G2515" s="0">
+        <v>419</v>
+      </c>
+      <c r="H2515" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2516">
+      <c r="A2516" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B2516" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2516" s="0">
+        <v>33428</v>
+      </c>
+      <c r="D2516" s="0">
+        <v>9.48645764751288E-02</v>
+      </c>
+      <c r="E2516" s="0">
+        <v>491</v>
+      </c>
+      <c r="F2516" s="0">
+        <v>0.111489554950045</v>
+      </c>
+      <c r="G2516" s="0">
+        <v>854</v>
+      </c>
+      <c r="H2516" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2517">
+      <c r="A2517" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B2517" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2517" s="0">
+        <v>20076</v>
+      </c>
+      <c r="D2517" s="0">
+        <v>5.69732331373306E-02</v>
+      </c>
+      <c r="E2517" s="0">
+        <v>289</v>
+      </c>
+      <c r="F2517" s="0">
+        <v>0.065622161671208</v>
+      </c>
+      <c r="G2517" s="0">
+        <v>1354</v>
+      </c>
+      <c r="H2517" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2518">
+      <c r="A2518" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B2518" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2518" s="0">
+        <v>10817</v>
+      </c>
+      <c r="D2518" s="0">
+        <v>3.06973233137331E-02</v>
+      </c>
+      <c r="E2518" s="0">
+        <v>170</v>
+      </c>
+      <c r="F2518" s="0">
+        <v>3.86012715712988E-02</v>
+      </c>
+      <c r="G2518" s="0">
+        <v>1646</v>
+      </c>
+      <c r="H2518" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2519">
+      <c r="A2519" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B2519" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2519" s="0">
+        <v>515</v>
+      </c>
+      <c r="D2519" s="0">
+        <v>1.46150702658524E-03</v>
+      </c>
+      <c r="E2519" s="0">
+        <v>14</v>
+      </c>
+      <c r="F2519" s="0">
+        <v>3.17892824704814E-03</v>
+      </c>
+      <c r="G2519" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2519" s="0">
         <v>0</v>
       </c>
     </row>
@@ -68932,11 +70052,11 @@
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Home xmlns="f83d9bd0-d5f5-484c-bfdf-0c10f1e052c8">false</Home>
-    <_dlc_DocId xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">HJYU5V3E37X6-122305290-1584</_dlc_DocId>
+    <_dlc_DocId xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">HJYU5V3E37X6-122305290-1629</_dlc_DocId>
     <Present xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2">false</Present>
     <_dlc_DocIdUrl xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">
-      <Url>https://tennessee.sharepoint.com/sites/health/PRG/COVID/_layouts/15/DocIdRedir.aspx?ID=HJYU5V3E37X6-122305290-1584</Url>
-      <Description>HJYU5V3E37X6-122305290-1584</Description>
+      <Url>https://tennessee.sharepoint.com/sites/health/PRG/COVID/_layouts/15/DocIdRedir.aspx?ID=HJYU5V3E37X6-122305290-1629</Url>
+      <Description>HJYU5V3E37X6-122305290-1629</Description>
     </_dlc_DocIdUrl>
     <Project_x0020_ID xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2" xsi:nil="true"/>
     <Doc_x0020_Subject xmlns="2773c6ec-81e5-4cca-8f30-56e38046ef00" xsi:nil="true"/>
@@ -68959,17 +70079,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6F494F8-E5E8-4838-A12C-28950F5703B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA40A4CD-5221-49C8-A10C-7F1D26521E1B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1C9C968-6855-49BC-8C4C-04503CD1CC70}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92CB6363-C8BA-4F26-9DAF-ED90BCADED60}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F99B31-482A-4212-B9F7-E2B79F760423}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4982E737-C843-4E8E-8C99-AF9BC6DEB929}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB964717-4827-4291-B233-8827B484034B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F76E3AB-D79F-4447-A4A1-3DC464491A21}"/>
 </file>
</xml_diff>

<commit_message>
add missing age group
</commit_message>
<xml_diff>
--- a/data/tn.xlsx
+++ b/data/tn.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="ALL_AGE_FINAL"/>
   </sheets>
   <definedNames>
-    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$2519</definedName>
+    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$2589</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -347,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2519"/>
+  <dimension ref="A1:H2589"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -69620,6 +69620,1966 @@
         <v>1</v>
       </c>
       <c r="H2519" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2520">
+      <c r="A2520" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B2520" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2520" s="0">
+        <v>17616</v>
+      </c>
+      <c r="D2520" s="0">
+        <v>4.93838235459021E-02</v>
+      </c>
+      <c r="E2520" s="0">
+        <v>244</v>
+      </c>
+      <c r="F2520" s="0">
+        <v>0.056221198156682</v>
+      </c>
+      <c r="G2520" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2520" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2521">
+      <c r="A2521" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B2521" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2521" s="0">
+        <v>47544</v>
+      </c>
+      <c r="D2521" s="0">
+        <v>0.133282499243095</v>
+      </c>
+      <c r="E2521" s="0">
+        <v>542</v>
+      </c>
+      <c r="F2521" s="0">
+        <v>0.124884792626728</v>
+      </c>
+      <c r="G2521" s="0">
+        <v>2</v>
+      </c>
+      <c r="H2521" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2522">
+      <c r="A2522" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B2522" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2522" s="0">
+        <v>68631</v>
+      </c>
+      <c r="D2522" s="0">
+        <v>0.192396752598706</v>
+      </c>
+      <c r="E2522" s="0">
+        <v>807</v>
+      </c>
+      <c r="F2522" s="0">
+        <v>0.18594470046083</v>
+      </c>
+      <c r="G2522" s="0">
+        <v>28</v>
+      </c>
+      <c r="H2522" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2523">
+      <c r="A2523" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B2523" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2523" s="0">
+        <v>56221</v>
+      </c>
+      <c r="D2523" s="0">
+        <v>0.157607172092084</v>
+      </c>
+      <c r="E2523" s="0">
+        <v>696</v>
+      </c>
+      <c r="F2523" s="0">
+        <v>0.16036866359447</v>
+      </c>
+      <c r="G2523" s="0">
+        <v>58</v>
+      </c>
+      <c r="H2523" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2524">
+      <c r="A2524" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B2524" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2524" s="0">
+        <v>52952</v>
+      </c>
+      <c r="D2524" s="0">
+        <v>0.148443019096424</v>
+      </c>
+      <c r="E2524" s="0">
+        <v>648</v>
+      </c>
+      <c r="F2524" s="0">
+        <v>0.149308755760369</v>
+      </c>
+      <c r="G2524" s="0">
+        <v>154</v>
+      </c>
+      <c r="H2524" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2525">
+      <c r="A2525" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B2525" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2525" s="0">
+        <v>48104</v>
+      </c>
+      <c r="D2525" s="0">
+        <v>0.134852375559268</v>
+      </c>
+      <c r="E2525" s="0">
+        <v>591</v>
+      </c>
+      <c r="F2525" s="0">
+        <v>0.136175115207373</v>
+      </c>
+      <c r="G2525" s="0">
+        <v>419</v>
+      </c>
+      <c r="H2525" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2526">
+      <c r="A2526" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B2526" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2526" s="0">
+        <v>33891</v>
+      </c>
+      <c r="D2526" s="0">
+        <v>9.50083539846825E-02</v>
+      </c>
+      <c r="E2526" s="0">
+        <v>463</v>
+      </c>
+      <c r="F2526" s="0">
+        <v>0.10668202764977</v>
+      </c>
+      <c r="G2526" s="0">
+        <v>855</v>
+      </c>
+      <c r="H2526" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2527">
+      <c r="A2527" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B2527" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2527" s="0">
+        <v>20314</v>
+      </c>
+      <c r="D2527" s="0">
+        <v>5.69472633691788E-02</v>
+      </c>
+      <c r="E2527" s="0">
+        <v>238</v>
+      </c>
+      <c r="F2527" s="0">
+        <v>5.48387096774194E-02</v>
+      </c>
+      <c r="G2527" s="0">
+        <v>1357</v>
+      </c>
+      <c r="H2527" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2528">
+      <c r="A2528" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B2528" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2528" s="0">
+        <v>10924</v>
+      </c>
+      <c r="D2528" s="0">
+        <v>3.06238015676336E-02</v>
+      </c>
+      <c r="E2528" s="0">
+        <v>107</v>
+      </c>
+      <c r="F2528" s="0">
+        <v>2.46543778801843E-02</v>
+      </c>
+      <c r="G2528" s="0">
+        <v>1648</v>
+      </c>
+      <c r="H2528" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2529">
+      <c r="A2529" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B2529" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2529" s="0">
+        <v>519</v>
+      </c>
+      <c r="D2529" s="0">
+        <v>1.4549389430247E-03</v>
+      </c>
+      <c r="E2529" s="0">
+        <v>4</v>
+      </c>
+      <c r="F2529" s="0">
+        <v>9.21658986175115E-04</v>
+      </c>
+      <c r="G2529" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2529" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2530">
+      <c r="A2530" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B2530" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2530" s="0">
+        <v>17938</v>
+      </c>
+      <c r="D2530" s="0">
+        <v>0.049352621703268</v>
+      </c>
+      <c r="E2530" s="0">
+        <v>322</v>
+      </c>
+      <c r="F2530" s="0">
+        <v>4.77037037037037E-02</v>
+      </c>
+      <c r="G2530" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2530" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2531">
+      <c r="A2531" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B2531" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2531" s="0">
+        <v>48409</v>
+      </c>
+      <c r="D2531" s="0">
+        <v>0.133187148178922</v>
+      </c>
+      <c r="E2531" s="0">
+        <v>865</v>
+      </c>
+      <c r="F2531" s="0">
+        <v>0.128148148148148</v>
+      </c>
+      <c r="G2531" s="0">
+        <v>2</v>
+      </c>
+      <c r="H2531" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2532">
+      <c r="A2532" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B2532" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2532" s="0">
+        <v>69774</v>
+      </c>
+      <c r="D2532" s="0">
+        <v>0.191968437212834</v>
+      </c>
+      <c r="E2532" s="0">
+        <v>1143</v>
+      </c>
+      <c r="F2532" s="0">
+        <v>0.169333333333333</v>
+      </c>
+      <c r="G2532" s="0">
+        <v>28</v>
+      </c>
+      <c r="H2532" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2533">
+      <c r="A2533" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B2533" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2533" s="0">
+        <v>57216</v>
+      </c>
+      <c r="D2533" s="0">
+        <v>0.157417750215976</v>
+      </c>
+      <c r="E2533" s="0">
+        <v>995</v>
+      </c>
+      <c r="F2533" s="0">
+        <v>0.147407407407407</v>
+      </c>
+      <c r="G2533" s="0">
+        <v>58</v>
+      </c>
+      <c r="H2533" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2534">
+      <c r="A2534" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B2534" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2534" s="0">
+        <v>53963</v>
+      </c>
+      <c r="D2534" s="0">
+        <v>0.148467807167658</v>
+      </c>
+      <c r="E2534" s="0">
+        <v>1011</v>
+      </c>
+      <c r="F2534" s="0">
+        <v>0.149777777777778</v>
+      </c>
+      <c r="G2534" s="0">
+        <v>154</v>
+      </c>
+      <c r="H2534" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2535">
+      <c r="A2535" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B2535" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2535" s="0">
+        <v>49055</v>
+      </c>
+      <c r="D2535" s="0">
+        <v>0.134964480859283</v>
+      </c>
+      <c r="E2535" s="0">
+        <v>951</v>
+      </c>
+      <c r="F2535" s="0">
+        <v>0.140888888888889</v>
+      </c>
+      <c r="G2535" s="0">
+        <v>421</v>
+      </c>
+      <c r="H2535" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2536">
+      <c r="A2536" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B2536" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2536" s="0">
+        <v>34638</v>
+      </c>
+      <c r="D2536" s="0">
+        <v>9.52991476506743E-02</v>
+      </c>
+      <c r="E2536" s="0">
+        <v>747</v>
+      </c>
+      <c r="F2536" s="0">
+        <v>0.110666666666667</v>
+      </c>
+      <c r="G2536" s="0">
+        <v>856</v>
+      </c>
+      <c r="H2536" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2537">
+      <c r="A2537" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B2537" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2537" s="0">
+        <v>20761</v>
+      </c>
+      <c r="D2537" s="0">
+        <v>5.71195104906649E-02</v>
+      </c>
+      <c r="E2537" s="0">
+        <v>447</v>
+      </c>
+      <c r="F2537" s="0">
+        <v>6.62222222222222E-02</v>
+      </c>
+      <c r="G2537" s="0">
+        <v>1361</v>
+      </c>
+      <c r="H2537" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2538">
+      <c r="A2538" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B2538" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2538" s="0">
+        <v>11178</v>
+      </c>
+      <c r="D2538" s="0">
+        <v>3.07539082059945E-02</v>
+      </c>
+      <c r="E2538" s="0">
+        <v>254</v>
+      </c>
+      <c r="F2538" s="0">
+        <v>3.76296296296296E-02</v>
+      </c>
+      <c r="G2538" s="0">
+        <v>1656</v>
+      </c>
+      <c r="H2538" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2539">
+      <c r="A2539" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B2539" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2539" s="0">
+        <v>534</v>
+      </c>
+      <c r="D2539" s="0">
+        <v>1.46918831472545E-03</v>
+      </c>
+      <c r="E2539" s="0">
+        <v>15</v>
+      </c>
+      <c r="F2539" s="0">
+        <v>2.22222222222222E-03</v>
+      </c>
+      <c r="G2539" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2539" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2540">
+      <c r="A2540" s="1">
+        <v>44164</v>
+      </c>
+      <c r="B2540" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2540" s="0">
+        <v>18111</v>
+      </c>
+      <c r="D2540" s="0">
+        <v>4.94136713612974E-02</v>
+      </c>
+      <c r="E2540" s="0">
+        <v>173</v>
+      </c>
+      <c r="F2540" s="0">
+        <v>5.66841415465269E-02</v>
+      </c>
+      <c r="G2540" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2540" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2541">
+      <c r="A2541" s="1">
+        <v>44164</v>
+      </c>
+      <c r="B2541" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2541" s="0">
+        <v>48783</v>
+      </c>
+      <c r="D2541" s="0">
+        <v>0.133098510850763</v>
+      </c>
+      <c r="E2541" s="0">
+        <v>374</v>
+      </c>
+      <c r="F2541" s="0">
+        <v>0.122542595019659</v>
+      </c>
+      <c r="G2541" s="0">
+        <v>2</v>
+      </c>
+      <c r="H2541" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2542">
+      <c r="A2542" s="1">
+        <v>44164</v>
+      </c>
+      <c r="B2542" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2542" s="0">
+        <v>70283</v>
+      </c>
+      <c r="D2542" s="0">
+        <v>0.191758658510632</v>
+      </c>
+      <c r="E2542" s="0">
+        <v>509</v>
+      </c>
+      <c r="F2542" s="0">
+        <v>0.166775884665793</v>
+      </c>
+      <c r="G2542" s="0">
+        <v>28</v>
+      </c>
+      <c r="H2542" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2543">
+      <c r="A2543" s="1">
+        <v>44164</v>
+      </c>
+      <c r="B2543" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2543" s="0">
+        <v>57677</v>
+      </c>
+      <c r="D2543" s="0">
+        <v>0.157364713329223</v>
+      </c>
+      <c r="E2543" s="0">
+        <v>461</v>
+      </c>
+      <c r="F2543" s="0">
+        <v>0.151048492791612</v>
+      </c>
+      <c r="G2543" s="0">
+        <v>59</v>
+      </c>
+      <c r="H2543" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2544">
+      <c r="A2544" s="1">
+        <v>44164</v>
+      </c>
+      <c r="B2544" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2544" s="0">
+        <v>54433</v>
+      </c>
+      <c r="D2544" s="0">
+        <v>0.148513851979985</v>
+      </c>
+      <c r="E2544" s="0">
+        <v>470</v>
+      </c>
+      <c r="F2544" s="0">
+        <v>0.153997378768021</v>
+      </c>
+      <c r="G2544" s="0">
+        <v>154</v>
+      </c>
+      <c r="H2544" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2545">
+      <c r="A2545" s="1">
+        <v>44164</v>
+      </c>
+      <c r="B2545" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2545" s="0">
+        <v>49529</v>
+      </c>
+      <c r="D2545" s="0">
+        <v>0.135133881555613</v>
+      </c>
+      <c r="E2545" s="0">
+        <v>474</v>
+      </c>
+      <c r="F2545" s="0">
+        <v>0.155307994757536</v>
+      </c>
+      <c r="G2545" s="0">
+        <v>423</v>
+      </c>
+      <c r="H2545" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2546">
+      <c r="A2546" s="1">
+        <v>44164</v>
+      </c>
+      <c r="B2546" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2546" s="0">
+        <v>34943</v>
+      </c>
+      <c r="D2546" s="0">
+        <v>9.53377460315728E-02</v>
+      </c>
+      <c r="E2546" s="0">
+        <v>305</v>
+      </c>
+      <c r="F2546" s="0">
+        <v>9.99344692005242E-02</v>
+      </c>
+      <c r="G2546" s="0">
+        <v>859</v>
+      </c>
+      <c r="H2546" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2547">
+      <c r="A2547" s="1">
+        <v>44164</v>
+      </c>
+      <c r="B2547" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2547" s="0">
+        <v>20976</v>
+      </c>
+      <c r="D2547" s="0">
+        <v>5.72304770843451E-02</v>
+      </c>
+      <c r="E2547" s="0">
+        <v>215</v>
+      </c>
+      <c r="F2547" s="0">
+        <v>7.04456094364351E-02</v>
+      </c>
+      <c r="G2547" s="0">
+        <v>1364</v>
+      </c>
+      <c r="H2547" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2548">
+      <c r="A2548" s="1">
+        <v>44164</v>
+      </c>
+      <c r="B2548" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2548" s="0">
+        <v>11242</v>
+      </c>
+      <c r="D2548" s="0">
+        <v>3.06724362787094E-02</v>
+      </c>
+      <c r="E2548" s="0">
+        <v>64</v>
+      </c>
+      <c r="F2548" s="0">
+        <v>2.09698558322412E-02</v>
+      </c>
+      <c r="G2548" s="0">
+        <v>1660</v>
+      </c>
+      <c r="H2548" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2549">
+      <c r="A2549" s="1">
+        <v>44164</v>
+      </c>
+      <c r="B2549" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2549" s="0">
+        <v>541</v>
+      </c>
+      <c r="D2549" s="0">
+        <v>1.47605301785997E-03</v>
+      </c>
+      <c r="E2549" s="0">
+        <v>7</v>
+      </c>
+      <c r="F2549" s="0">
+        <v>2.29357798165138E-03</v>
+      </c>
+      <c r="G2549" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2549" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2550">
+      <c r="A2550" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B2550" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2550" s="0">
+        <v>18534</v>
+      </c>
+      <c r="D2550" s="0">
+        <v>4.94909117126355E-02</v>
+      </c>
+      <c r="E2550" s="0">
+        <v>423</v>
+      </c>
+      <c r="F2550" s="0">
+        <v>5.30407523510972E-02</v>
+      </c>
+      <c r="G2550" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2550" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2551">
+      <c r="A2551" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B2551" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2551" s="0">
+        <v>49787</v>
+      </c>
+      <c r="D2551" s="0">
+        <v>0.132945075074835</v>
+      </c>
+      <c r="E2551" s="0">
+        <v>1004</v>
+      </c>
+      <c r="F2551" s="0">
+        <v>0.1258934169279</v>
+      </c>
+      <c r="G2551" s="0">
+        <v>2</v>
+      </c>
+      <c r="H2551" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2552">
+      <c r="A2552" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B2552" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2552" s="0">
+        <v>71667</v>
+      </c>
+      <c r="D2552" s="0">
+        <v>0.191370733231329</v>
+      </c>
+      <c r="E2552" s="0">
+        <v>1384</v>
+      </c>
+      <c r="F2552" s="0">
+        <v>0.173542319749216</v>
+      </c>
+      <c r="G2552" s="0">
+        <v>29</v>
+      </c>
+      <c r="H2552" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2553">
+      <c r="A2553" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B2553" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2553" s="0">
+        <v>58909</v>
+      </c>
+      <c r="D2553" s="0">
+        <v>0.157303340783406</v>
+      </c>
+      <c r="E2553" s="0">
+        <v>1232</v>
+      </c>
+      <c r="F2553" s="0">
+        <v>0.15448275862069</v>
+      </c>
+      <c r="G2553" s="0">
+        <v>59</v>
+      </c>
+      <c r="H2553" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2554">
+      <c r="A2554" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B2554" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2554" s="0">
+        <v>55713</v>
+      </c>
+      <c r="D2554" s="0">
+        <v>0.148769135871699</v>
+      </c>
+      <c r="E2554" s="0">
+        <v>1280</v>
+      </c>
+      <c r="F2554" s="0">
+        <v>0.160501567398119</v>
+      </c>
+      <c r="G2554" s="0">
+        <v>156</v>
+      </c>
+      <c r="H2554" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2555">
+      <c r="A2555" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B2555" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2555" s="0">
+        <v>50671</v>
+      </c>
+      <c r="D2555" s="0">
+        <v>0.135305599837647</v>
+      </c>
+      <c r="E2555" s="0">
+        <v>1142</v>
+      </c>
+      <c r="F2555" s="0">
+        <v>0.143197492163009</v>
+      </c>
+      <c r="G2555" s="0">
+        <v>426</v>
+      </c>
+      <c r="H2555" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2556">
+      <c r="A2556" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B2556" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2556" s="0">
+        <v>35747</v>
+      </c>
+      <c r="D2556" s="0">
+        <v>0.095454387665457</v>
+      </c>
+      <c r="E2556" s="0">
+        <v>804</v>
+      </c>
+      <c r="F2556" s="0">
+        <v>0.100815047021944</v>
+      </c>
+      <c r="G2556" s="0">
+        <v>869</v>
+      </c>
+      <c r="H2556" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2557">
+      <c r="A2557" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B2557" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2557" s="0">
+        <v>21470</v>
+      </c>
+      <c r="D2557" s="0">
+        <v>5.73308446352802E-02</v>
+      </c>
+      <c r="E2557" s="0">
+        <v>494</v>
+      </c>
+      <c r="F2557" s="0">
+        <v>6.19435736677116E-02</v>
+      </c>
+      <c r="G2557" s="0">
+        <v>1380</v>
+      </c>
+      <c r="H2557" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2558">
+      <c r="A2558" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B2558" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2558" s="0">
+        <v>11450</v>
+      </c>
+      <c r="D2558" s="0">
+        <v>3.05746702875621E-02</v>
+      </c>
+      <c r="E2558" s="0">
+        <v>208</v>
+      </c>
+      <c r="F2558" s="0">
+        <v>2.60815047021944E-02</v>
+      </c>
+      <c r="G2558" s="0">
+        <v>1676</v>
+      </c>
+      <c r="H2558" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2559">
+      <c r="A2559" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B2559" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2559" s="0">
+        <v>545</v>
+      </c>
+      <c r="D2559" s="0">
+        <v>1.45530090015034E-03</v>
+      </c>
+      <c r="E2559" s="0">
+        <v>4</v>
+      </c>
+      <c r="F2559" s="0">
+        <v>5.01567398119122E-04</v>
+      </c>
+      <c r="G2559" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2559" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2560">
+      <c r="A2560" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B2560" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2560" s="0">
+        <v>18876</v>
+      </c>
+      <c r="D2560" s="0">
+        <v>4.96493821445293E-02</v>
+      </c>
+      <c r="E2560" s="0">
+        <v>342</v>
+      </c>
+      <c r="F2560" s="0">
+        <v>6.00737748111716E-02</v>
+      </c>
+      <c r="G2560" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2560" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2561">
+      <c r="A2561" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B2561" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2561" s="0">
+        <v>50396</v>
+      </c>
+      <c r="D2561" s="0">
+        <v>0.132556169874746</v>
+      </c>
+      <c r="E2561" s="0">
+        <v>609</v>
+      </c>
+      <c r="F2561" s="0">
+        <v>0.106973476198841</v>
+      </c>
+      <c r="G2561" s="0">
+        <v>2</v>
+      </c>
+      <c r="H2561" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2562">
+      <c r="A2562" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B2562" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2562" s="0">
+        <v>72623</v>
+      </c>
+      <c r="D2562" s="0">
+        <v>0.191019658798588</v>
+      </c>
+      <c r="E2562" s="0">
+        <v>956</v>
+      </c>
+      <c r="F2562" s="0">
+        <v>0.167925522571579</v>
+      </c>
+      <c r="G2562" s="0">
+        <v>29</v>
+      </c>
+      <c r="H2562" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2563">
+      <c r="A2563" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B2563" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2563" s="0">
+        <v>59784</v>
+      </c>
+      <c r="D2563" s="0">
+        <v>0.157249346372565</v>
+      </c>
+      <c r="E2563" s="0">
+        <v>875</v>
+      </c>
+      <c r="F2563" s="0">
+        <v>0.153697523274196</v>
+      </c>
+      <c r="G2563" s="0">
+        <v>60</v>
+      </c>
+      <c r="H2563" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2564">
+      <c r="A2564" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B2564" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2564" s="0">
+        <v>56592</v>
+      </c>
+      <c r="D2564" s="0">
+        <v>0.148853455939987</v>
+      </c>
+      <c r="E2564" s="0">
+        <v>879</v>
+      </c>
+      <c r="F2564" s="0">
+        <v>0.15440014052345</v>
+      </c>
+      <c r="G2564" s="0">
+        <v>156</v>
+      </c>
+      <c r="H2564" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2565">
+      <c r="A2565" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B2565" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2565" s="0">
+        <v>51525</v>
+      </c>
+      <c r="D2565" s="0">
+        <v>0.135525768965717</v>
+      </c>
+      <c r="E2565" s="0">
+        <v>854</v>
+      </c>
+      <c r="F2565" s="0">
+        <v>0.150008782715616</v>
+      </c>
+      <c r="G2565" s="0">
+        <v>431</v>
+      </c>
+      <c r="H2565" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2566">
+      <c r="A2566" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B2566" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2566" s="0">
+        <v>36375</v>
+      </c>
+      <c r="D2566" s="0">
+        <v>9.56768529088394E-02</v>
+      </c>
+      <c r="E2566" s="0">
+        <v>628</v>
+      </c>
+      <c r="F2566" s="0">
+        <v>0.110310908132795</v>
+      </c>
+      <c r="G2566" s="0">
+        <v>874</v>
+      </c>
+      <c r="H2566" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2567">
+      <c r="A2567" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B2567" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2567" s="0">
+        <v>21842</v>
+      </c>
+      <c r="D2567" s="0">
+        <v>0.057450826700615</v>
+      </c>
+      <c r="E2567" s="0">
+        <v>372</v>
+      </c>
+      <c r="F2567" s="0">
+        <v>6.53434041805726E-02</v>
+      </c>
+      <c r="G2567" s="0">
+        <v>1399</v>
+      </c>
+      <c r="H2567" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2568">
+      <c r="A2568" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B2568" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2568" s="0">
+        <v>11629</v>
+      </c>
+      <c r="D2568" s="0">
+        <v>3.05876597244507E-02</v>
+      </c>
+      <c r="E2568" s="0">
+        <v>179</v>
+      </c>
+      <c r="F2568" s="0">
+        <v>3.14421219040927E-02</v>
+      </c>
+      <c r="G2568" s="0">
+        <v>1681</v>
+      </c>
+      <c r="H2568" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2569">
+      <c r="A2569" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B2569" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2569" s="0">
+        <v>544</v>
+      </c>
+      <c r="D2569" s="0">
+        <v>1.43087856996312E-03</v>
+      </c>
+      <c r="E2569" s="0">
+        <v>-1</v>
+      </c>
+      <c r="F2569" s="0">
+        <v>-1.75654312313367E-04</v>
+      </c>
+      <c r="G2569" s="0">
+        <v>2</v>
+      </c>
+      <c r="H2569" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2570">
+      <c r="A2570" s="1">
+        <v>44167</v>
+      </c>
+      <c r="B2570" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2570" s="0">
+        <v>19085</v>
+      </c>
+      <c r="D2570" s="0">
+        <v>4.96636610848719E-02</v>
+      </c>
+      <c r="E2570" s="0">
+        <v>209</v>
+      </c>
+      <c r="F2570" s="0">
+        <v>5.09880458648451E-02</v>
+      </c>
+      <c r="G2570" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2570" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2571">
+      <c r="A2571" s="1">
+        <v>44167</v>
+      </c>
+      <c r="B2571" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2571" s="0">
+        <v>50849</v>
+      </c>
+      <c r="D2571" s="0">
+        <v>0.132321063793799</v>
+      </c>
+      <c r="E2571" s="0">
+        <v>453</v>
+      </c>
+      <c r="F2571" s="0">
+        <v>0.110514759697487</v>
+      </c>
+      <c r="G2571" s="0">
+        <v>2</v>
+      </c>
+      <c r="H2571" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2572">
+      <c r="A2572" s="1">
+        <v>44167</v>
+      </c>
+      <c r="B2572" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2572" s="0">
+        <v>73337</v>
+      </c>
+      <c r="D2572" s="0">
+        <v>0.190840131673107</v>
+      </c>
+      <c r="E2572" s="0">
+        <v>714</v>
+      </c>
+      <c r="F2572" s="0">
+        <v>0.174188826543059</v>
+      </c>
+      <c r="G2572" s="0">
+        <v>30</v>
+      </c>
+      <c r="H2572" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2573">
+      <c r="A2573" s="1">
+        <v>44167</v>
+      </c>
+      <c r="B2573" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2573" s="0">
+        <v>60430</v>
+      </c>
+      <c r="D2573" s="0">
+        <v>0.15725308039606</v>
+      </c>
+      <c r="E2573" s="0">
+        <v>646</v>
+      </c>
+      <c r="F2573" s="0">
+        <v>0.157599414491339</v>
+      </c>
+      <c r="G2573" s="0">
+        <v>60</v>
+      </c>
+      <c r="H2573" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2574">
+      <c r="A2574" s="1">
+        <v>44167</v>
+      </c>
+      <c r="B2574" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2574" s="0">
+        <v>57197</v>
+      </c>
+      <c r="D2574" s="0">
+        <v>0.148840053606048</v>
+      </c>
+      <c r="E2574" s="0">
+        <v>605</v>
+      </c>
+      <c r="F2574" s="0">
+        <v>0.14759697487192</v>
+      </c>
+      <c r="G2574" s="0">
+        <v>159</v>
+      </c>
+      <c r="H2574" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2575">
+      <c r="A2575" s="1">
+        <v>44167</v>
+      </c>
+      <c r="B2575" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2575" s="0">
+        <v>52099</v>
+      </c>
+      <c r="D2575" s="0">
+        <v>0.135573857943974</v>
+      </c>
+      <c r="E2575" s="0">
+        <v>574</v>
+      </c>
+      <c r="F2575" s="0">
+        <v>0.140034154671871</v>
+      </c>
+      <c r="G2575" s="0">
+        <v>432</v>
+      </c>
+      <c r="H2575" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2576">
+      <c r="A2576" s="1">
+        <v>44167</v>
+      </c>
+      <c r="B2576" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2576" s="0">
+        <v>36822</v>
+      </c>
+      <c r="D2576" s="0">
+        <v>9.58195089581951E-02</v>
+      </c>
+      <c r="E2576" s="0">
+        <v>447</v>
+      </c>
+      <c r="F2576" s="0">
+        <v>0.109050988045865</v>
+      </c>
+      <c r="G2576" s="0">
+        <v>888</v>
+      </c>
+      <c r="H2576" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2577">
+      <c r="A2577" s="1">
+        <v>44167</v>
+      </c>
+      <c r="B2577" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2577" s="0">
+        <v>22156</v>
+      </c>
+      <c r="D2577" s="0">
+        <v>5.76551257530218E-02</v>
+      </c>
+      <c r="E2577" s="0">
+        <v>314</v>
+      </c>
+      <c r="F2577" s="0">
+        <v>7.66040497682361E-02</v>
+      </c>
+      <c r="G2577" s="0">
+        <v>1416</v>
+      </c>
+      <c r="H2577" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2578">
+      <c r="A2578" s="1">
+        <v>44167</v>
+      </c>
+      <c r="B2578" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2578" s="0">
+        <v>11768</v>
+      </c>
+      <c r="D2578" s="0">
+        <v>3.06231052474075E-02</v>
+      </c>
+      <c r="E2578" s="0">
+        <v>139</v>
+      </c>
+      <c r="F2578" s="0">
+        <v>0.033910709929251</v>
+      </c>
+      <c r="G2578" s="0">
+        <v>1696</v>
+      </c>
+      <c r="H2578" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2579">
+      <c r="A2579" s="1">
+        <v>44167</v>
+      </c>
+      <c r="B2579" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2579" s="0">
+        <v>542</v>
+      </c>
+      <c r="D2579" s="0">
+        <v>1.41041154351588E-03</v>
+      </c>
+      <c r="E2579" s="0">
+        <v>-2</v>
+      </c>
+      <c r="F2579" s="0">
+        <v>-4.87923883874116E-04</v>
+      </c>
+      <c r="G2579" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2579" s="0">
+        <v>-1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2580">
+      <c r="A2580" s="1">
+        <v>44168</v>
+      </c>
+      <c r="B2580" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2580" s="0">
+        <v>19332</v>
+      </c>
+      <c r="D2580" s="0">
+        <v>4.97924028723613E-02</v>
+      </c>
+      <c r="E2580" s="0">
+        <v>247</v>
+      </c>
+      <c r="F2580" s="0">
+        <v>6.22636753214016E-02</v>
+      </c>
+      <c r="G2580" s="0">
+        <v>5</v>
+      </c>
+      <c r="H2580" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2581">
+      <c r="A2581" s="1">
+        <v>44168</v>
+      </c>
+      <c r="B2581" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2581" s="0">
+        <v>51330</v>
+      </c>
+      <c r="D2581" s="0">
+        <v>0.132207947415596</v>
+      </c>
+      <c r="E2581" s="0">
+        <v>481</v>
+      </c>
+      <c r="F2581" s="0">
+        <v>0.121250315099571</v>
+      </c>
+      <c r="G2581" s="0">
+        <v>3</v>
+      </c>
+      <c r="H2581" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2582">
+      <c r="A2582" s="1">
+        <v>44168</v>
+      </c>
+      <c r="B2582" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2582" s="0">
+        <v>74027</v>
+      </c>
+      <c r="D2582" s="0">
+        <v>0.190667401584538</v>
+      </c>
+      <c r="E2582" s="0">
+        <v>690</v>
+      </c>
+      <c r="F2582" s="0">
+        <v>0.17393496344845</v>
+      </c>
+      <c r="G2582" s="0">
+        <v>31</v>
+      </c>
+      <c r="H2582" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2583">
+      <c r="A2583" s="1">
+        <v>44168</v>
+      </c>
+      <c r="B2583" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2583" s="0">
+        <v>61015</v>
+      </c>
+      <c r="D2583" s="0">
+        <v>0.15715308613993</v>
+      </c>
+      <c r="E2583" s="0">
+        <v>585</v>
+      </c>
+      <c r="F2583" s="0">
+        <v>0.147466599445425</v>
+      </c>
+      <c r="G2583" s="0">
+        <v>61</v>
+      </c>
+      <c r="H2583" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2584">
+      <c r="A2584" s="1">
+        <v>44168</v>
+      </c>
+      <c r="B2584" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2584" s="0">
+        <v>57821</v>
+      </c>
+      <c r="D2584" s="0">
+        <v>0.148926470436727</v>
+      </c>
+      <c r="E2584" s="0">
+        <v>624</v>
+      </c>
+      <c r="F2584" s="0">
+        <v>0.15729770607512</v>
+      </c>
+      <c r="G2584" s="0">
+        <v>161</v>
+      </c>
+      <c r="H2584" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2585">
+      <c r="A2585" s="1">
+        <v>44168</v>
+      </c>
+      <c r="B2585" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2585" s="0">
+        <v>52665</v>
+      </c>
+      <c r="D2585" s="0">
+        <v>0.135646435820034</v>
+      </c>
+      <c r="E2585" s="0">
+        <v>566</v>
+      </c>
+      <c r="F2585" s="0">
+        <v>0.142677085959163</v>
+      </c>
+      <c r="G2585" s="0">
+        <v>439</v>
+      </c>
+      <c r="H2585" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2586">
+      <c r="A2586" s="1">
+        <v>44168</v>
+      </c>
+      <c r="B2586" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2586" s="0">
+        <v>37236</v>
+      </c>
+      <c r="D2586" s="0">
+        <v>9.59067821930087E-02</v>
+      </c>
+      <c r="E2586" s="0">
+        <v>414</v>
+      </c>
+      <c r="F2586" s="0">
+        <v>0.10436097806907</v>
+      </c>
+      <c r="G2586" s="0">
+        <v>898</v>
+      </c>
+      <c r="H2586" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2587">
+      <c r="A2587" s="1">
+        <v>44168</v>
+      </c>
+      <c r="B2587" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2587" s="0">
+        <v>22390</v>
+      </c>
+      <c r="D2587" s="0">
+        <v>5.76687306182582E-02</v>
+      </c>
+      <c r="E2587" s="0">
+        <v>234</v>
+      </c>
+      <c r="F2587" s="0">
+        <v>5.89866397781699E-02</v>
+      </c>
+      <c r="G2587" s="0">
+        <v>1447</v>
+      </c>
+      <c r="H2587" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2588">
+      <c r="A2588" s="1">
+        <v>44168</v>
+      </c>
+      <c r="B2588" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2588" s="0">
+        <v>11889</v>
+      </c>
+      <c r="D2588" s="0">
+        <v>3.06218641500881E-02</v>
+      </c>
+      <c r="E2588" s="0">
+        <v>121</v>
+      </c>
+      <c r="F2588" s="0">
+        <v>3.05016385177716E-02</v>
+      </c>
+      <c r="G2588" s="0">
+        <v>1735</v>
+      </c>
+      <c r="H2588" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2589">
+      <c r="A2589" s="1">
+        <v>44168</v>
+      </c>
+      <c r="B2589" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2589" s="0">
+        <v>547</v>
+      </c>
+      <c r="D2589" s="0">
+        <v>1.40887876945901E-03</v>
+      </c>
+      <c r="E2589" s="0">
+        <v>5</v>
+      </c>
+      <c r="F2589" s="0">
+        <v>1.26039828585833E-03</v>
+      </c>
+      <c r="G2589" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2589" s="0">
         <v>0</v>
       </c>
     </row>
@@ -70052,11 +72012,11 @@
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Home xmlns="f83d9bd0-d5f5-484c-bfdf-0c10f1e052c8">false</Home>
-    <_dlc_DocId xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">HJYU5V3E37X6-122305290-1629</_dlc_DocId>
+    <_dlc_DocId xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">HJYU5V3E37X6-122305290-1706</_dlc_DocId>
     <Present xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2">false</Present>
     <_dlc_DocIdUrl xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">
-      <Url>https://tennessee.sharepoint.com/sites/health/PRG/COVID/_layouts/15/DocIdRedir.aspx?ID=HJYU5V3E37X6-122305290-1629</Url>
-      <Description>HJYU5V3E37X6-122305290-1629</Description>
+      <Url>https://tennessee.sharepoint.com/sites/health/PRG/COVID/_layouts/15/DocIdRedir.aspx?ID=HJYU5V3E37X6-122305290-1706</Url>
+      <Description>HJYU5V3E37X6-122305290-1706</Description>
     </_dlc_DocIdUrl>
     <Project_x0020_ID xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2" xsi:nil="true"/>
     <Doc_x0020_Subject xmlns="2773c6ec-81e5-4cca-8f30-56e38046ef00" xsi:nil="true"/>
@@ -70079,17 +72039,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA40A4CD-5221-49C8-A10C-7F1D26521E1B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{353623D0-1903-41B1-890C-0F6B7369F91E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92CB6363-C8BA-4F26-9DAF-ED90BCADED60}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67A1B1BC-9176-4F96-B60C-03E0384DCFE2}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4982E737-C843-4E8E-8C99-AF9BC6DEB929}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E0D239-8513-4986-806D-F68543C83D45}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F76E3AB-D79F-4447-A4A1-3DC464491A21}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0CE616E-8412-4720-911C-21A146EB5E4E}"/>
 </file>
</xml_diff>

<commit_message>
new data from update_data
</commit_message>
<xml_diff>
--- a/data/tn.xlsx
+++ b/data/tn.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="ALL_AGE_FINAL"/>
   </sheets>
   <definedNames>
-    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$2629</definedName>
+    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$2699</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -347,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2629"/>
+  <dimension ref="A1:H2699"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -72700,6 +72700,1966 @@
         <v>0</v>
       </c>
       <c r="H2629" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2630">
+      <c r="A2630" s="1">
+        <v>44173</v>
+      </c>
+      <c r="B2630" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2630" s="0">
+        <v>20668</v>
+      </c>
+      <c r="D2630" s="0">
+        <v>4.98325493250134E-02</v>
+      </c>
+      <c r="E2630" s="0">
+        <v>301</v>
+      </c>
+      <c r="F2630" s="0">
+        <v>5.00083070277455E-02</v>
+      </c>
+      <c r="G2630" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2630" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2631">
+      <c r="A2631" s="1">
+        <v>44173</v>
+      </c>
+      <c r="B2631" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2631" s="0">
+        <v>54422</v>
+      </c>
+      <c r="D2631" s="0">
+        <v>0.131216711794362</v>
+      </c>
+      <c r="E2631" s="0">
+        <v>697</v>
+      </c>
+      <c r="F2631" s="0">
+        <v>0.115799966771889</v>
+      </c>
+      <c r="G2631" s="0">
+        <v>3</v>
+      </c>
+      <c r="H2631" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2632">
+      <c r="A2632" s="1">
+        <v>44173</v>
+      </c>
+      <c r="B2632" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2632" s="0">
+        <v>78495</v>
+      </c>
+      <c r="D2632" s="0">
+        <v>0.18925904583254</v>
+      </c>
+      <c r="E2632" s="0">
+        <v>999</v>
+      </c>
+      <c r="F2632" s="0">
+        <v>0.165974414354544</v>
+      </c>
+      <c r="G2632" s="0">
+        <v>31</v>
+      </c>
+      <c r="H2632" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2633">
+      <c r="A2633" s="1">
+        <v>44173</v>
+      </c>
+      <c r="B2633" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2633" s="0">
+        <v>65071</v>
+      </c>
+      <c r="D2633" s="0">
+        <v>0.156892481958968</v>
+      </c>
+      <c r="E2633" s="0">
+        <v>883</v>
+      </c>
+      <c r="F2633" s="0">
+        <v>0.146702109985047</v>
+      </c>
+      <c r="G2633" s="0">
+        <v>63</v>
+      </c>
+      <c r="H2633" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2634">
+      <c r="A2634" s="1">
+        <v>44173</v>
+      </c>
+      <c r="B2634" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2634" s="0">
+        <v>62006</v>
+      </c>
+      <c r="D2634" s="0">
+        <v>0.149502470168704</v>
+      </c>
+      <c r="E2634" s="0">
+        <v>923</v>
+      </c>
+      <c r="F2634" s="0">
+        <v>0.153347732181425</v>
+      </c>
+      <c r="G2634" s="0">
+        <v>167</v>
+      </c>
+      <c r="H2634" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2635">
+      <c r="A2635" s="1">
+        <v>44173</v>
+      </c>
+      <c r="B2635" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2635" s="0">
+        <v>56560</v>
+      </c>
+      <c r="D2635" s="0">
+        <v>0.136371636821306</v>
+      </c>
+      <c r="E2635" s="0">
+        <v>874</v>
+      </c>
+      <c r="F2635" s="0">
+        <v>0.145206844990862</v>
+      </c>
+      <c r="G2635" s="0">
+        <v>468</v>
+      </c>
+      <c r="H2635" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2636">
+      <c r="A2636" s="1">
+        <v>44173</v>
+      </c>
+      <c r="B2636" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2636" s="0">
+        <v>40115</v>
+      </c>
+      <c r="D2636" s="0">
+        <v>9.67211494180818E-02</v>
+      </c>
+      <c r="E2636" s="0">
+        <v>667</v>
+      </c>
+      <c r="F2636" s="0">
+        <v>0.110815750124605</v>
+      </c>
+      <c r="G2636" s="0">
+        <v>960</v>
+      </c>
+      <c r="H2636" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2637">
+      <c r="A2637" s="1">
+        <v>44173</v>
+      </c>
+      <c r="B2637" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2637" s="0">
+        <v>24033</v>
+      </c>
+      <c r="D2637" s="0">
+        <v>5.79458901648949E-02</v>
+      </c>
+      <c r="E2637" s="0">
+        <v>429</v>
+      </c>
+      <c r="F2637" s="0">
+        <v>7.12742980561555E-02</v>
+      </c>
+      <c r="G2637" s="0">
+        <v>1544</v>
+      </c>
+      <c r="H2637" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2638">
+      <c r="A2638" s="1">
+        <v>44173</v>
+      </c>
+      <c r="B2638" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2638" s="0">
+        <v>12819</v>
+      </c>
+      <c r="D2638" s="0">
+        <v>3.09078502901755E-02</v>
+      </c>
+      <c r="E2638" s="0">
+        <v>235</v>
+      </c>
+      <c r="F2638" s="0">
+        <v>3.90430304037215E-02</v>
+      </c>
+      <c r="G2638" s="0">
+        <v>1869</v>
+      </c>
+      <c r="H2638" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2639">
+      <c r="A2639" s="1">
+        <v>44173</v>
+      </c>
+      <c r="B2639" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2639" s="0">
+        <v>560</v>
+      </c>
+      <c r="D2639" s="0">
+        <v>1.35021422595353E-03</v>
+      </c>
+      <c r="E2639" s="0">
+        <v>11</v>
+      </c>
+      <c r="F2639" s="0">
+        <v>1.82754610400399E-03</v>
+      </c>
+      <c r="G2639" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2639" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2640">
+      <c r="A2640" s="1">
+        <v>44174</v>
+      </c>
+      <c r="B2640" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2640" s="0">
+        <v>21146</v>
+      </c>
+      <c r="D2640" s="0">
+        <v>4.99950350149659E-02</v>
+      </c>
+      <c r="E2640" s="0">
+        <v>478</v>
+      </c>
+      <c r="F2640" s="0">
+        <v>0.05820041397784</v>
+      </c>
+      <c r="G2640" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2640" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2641">
+      <c r="A2641" s="1">
+        <v>44174</v>
+      </c>
+      <c r="B2641" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2641" s="0">
+        <v>55518</v>
+      </c>
+      <c r="D2641" s="0">
+        <v>0.131260018630515</v>
+      </c>
+      <c r="E2641" s="0">
+        <v>1096</v>
+      </c>
+      <c r="F2641" s="0">
+        <v>0.133446974309022</v>
+      </c>
+      <c r="G2641" s="0">
+        <v>2</v>
+      </c>
+      <c r="H2641" s="0">
+        <v>-1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2642">
+      <c r="A2642" s="1">
+        <v>44174</v>
+      </c>
+      <c r="B2642" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2642" s="0">
+        <v>79935</v>
+      </c>
+      <c r="D2642" s="0">
+        <v>0.188988608905765</v>
+      </c>
+      <c r="E2642" s="0">
+        <v>1440</v>
+      </c>
+      <c r="F2642" s="0">
+        <v>0.175331791062949</v>
+      </c>
+      <c r="G2642" s="0">
+        <v>31</v>
+      </c>
+      <c r="H2642" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2643">
+      <c r="A2643" s="1">
+        <v>44174</v>
+      </c>
+      <c r="B2643" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2643" s="0">
+        <v>66342</v>
+      </c>
+      <c r="D2643" s="0">
+        <v>0.156850970063505</v>
+      </c>
+      <c r="E2643" s="0">
+        <v>1271</v>
+      </c>
+      <c r="F2643" s="0">
+        <v>0.1547546572507</v>
+      </c>
+      <c r="G2643" s="0">
+        <v>63</v>
+      </c>
+      <c r="H2643" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2644">
+      <c r="A2644" s="1">
+        <v>44174</v>
+      </c>
+      <c r="B2644" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2644" s="0">
+        <v>63217</v>
+      </c>
+      <c r="D2644" s="0">
+        <v>0.149462599477022</v>
+      </c>
+      <c r="E2644" s="0">
+        <v>1211</v>
+      </c>
+      <c r="F2644" s="0">
+        <v>0.147449165956411</v>
+      </c>
+      <c r="G2644" s="0">
+        <v>170</v>
+      </c>
+      <c r="H2644" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2645">
+      <c r="A2645" s="1">
+        <v>44174</v>
+      </c>
+      <c r="B2645" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2645" s="0">
+        <v>57696</v>
+      </c>
+      <c r="D2645" s="0">
+        <v>0.13640941739447</v>
+      </c>
+      <c r="E2645" s="0">
+        <v>1136</v>
+      </c>
+      <c r="F2645" s="0">
+        <v>0.138317301838549</v>
+      </c>
+      <c r="G2645" s="0">
+        <v>471</v>
+      </c>
+      <c r="H2645" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2646">
+      <c r="A2646" s="1">
+        <v>44174</v>
+      </c>
+      <c r="B2646" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2646" s="0">
+        <v>40940</v>
+      </c>
+      <c r="D2646" s="0">
+        <v>9.67935653793958E-02</v>
+      </c>
+      <c r="E2646" s="0">
+        <v>825</v>
+      </c>
+      <c r="F2646" s="0">
+        <v>0.100450505296481</v>
+      </c>
+      <c r="G2646" s="0">
+        <v>975</v>
+      </c>
+      <c r="H2646" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2647">
+      <c r="A2647" s="1">
+        <v>44174</v>
+      </c>
+      <c r="B2647" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2647" s="0">
+        <v>24560</v>
+      </c>
+      <c r="D2647" s="0">
+        <v>5.80666821132868E-02</v>
+      </c>
+      <c r="E2647" s="0">
+        <v>527</v>
+      </c>
+      <c r="F2647" s="0">
+        <v>6.41665652015098E-02</v>
+      </c>
+      <c r="G2647" s="0">
+        <v>1563</v>
+      </c>
+      <c r="H2647" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2648">
+      <c r="A2648" s="1">
+        <v>44174</v>
+      </c>
+      <c r="B2648" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2648" s="0">
+        <v>13060</v>
+      </c>
+      <c r="D2648" s="0">
+        <v>3.08774783550295E-02</v>
+      </c>
+      <c r="E2648" s="0">
+        <v>241</v>
+      </c>
+      <c r="F2648" s="0">
+        <v>2.93437233653963E-02</v>
+      </c>
+      <c r="G2648" s="0">
+        <v>1892</v>
+      </c>
+      <c r="H2648" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2649">
+      <c r="A2649" s="1">
+        <v>44174</v>
+      </c>
+      <c r="B2649" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2649" s="0">
+        <v>548</v>
+      </c>
+      <c r="D2649" s="0">
+        <v>1.29562466604565E-03</v>
+      </c>
+      <c r="E2649" s="0">
+        <v>-12</v>
+      </c>
+      <c r="F2649" s="0">
+        <v>-1.46109825885791E-03</v>
+      </c>
+      <c r="G2649" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2649" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2650">
+      <c r="A2650" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B2650" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2650" s="0">
+        <v>21516</v>
+      </c>
+      <c r="D2650" s="0">
+        <v>5.01570028882937E-02</v>
+      </c>
+      <c r="E2650" s="0">
+        <v>370</v>
+      </c>
+      <c r="F2650" s="0">
+        <v>6.15538180003327E-02</v>
+      </c>
+      <c r="G2650" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2650" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2651">
+      <c r="A2651" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B2651" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2651" s="0">
+        <v>56292</v>
+      </c>
+      <c r="D2651" s="0">
+        <v>0.131225042135519</v>
+      </c>
+      <c r="E2651" s="0">
+        <v>774</v>
+      </c>
+      <c r="F2651" s="0">
+        <v>0.128763932789885</v>
+      </c>
+      <c r="G2651" s="0">
+        <v>3</v>
+      </c>
+      <c r="H2651" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2652">
+      <c r="A2652" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B2652" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2652" s="0">
+        <v>80949</v>
+      </c>
+      <c r="D2652" s="0">
+        <v>0.188704184179424</v>
+      </c>
+      <c r="E2652" s="0">
+        <v>1014</v>
+      </c>
+      <c r="F2652" s="0">
+        <v>0.168690733654966</v>
+      </c>
+      <c r="G2652" s="0">
+        <v>31</v>
+      </c>
+      <c r="H2652" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2653">
+      <c r="A2653" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B2653" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2653" s="0">
+        <v>67256</v>
+      </c>
+      <c r="D2653" s="0">
+        <v>0.156783760283281</v>
+      </c>
+      <c r="E2653" s="0">
+        <v>914</v>
+      </c>
+      <c r="F2653" s="0">
+        <v>0.152054566627849</v>
+      </c>
+      <c r="G2653" s="0">
+        <v>63</v>
+      </c>
+      <c r="H2653" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2654">
+      <c r="A2654" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B2654" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2654" s="0">
+        <v>64113</v>
+      </c>
+      <c r="D2654" s="0">
+        <v>0.149456958829577</v>
+      </c>
+      <c r="E2654" s="0">
+        <v>896</v>
+      </c>
+      <c r="F2654" s="0">
+        <v>0.149060056562968</v>
+      </c>
+      <c r="G2654" s="0">
+        <v>174</v>
+      </c>
+      <c r="H2654" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2655">
+      <c r="A2655" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B2655" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2655" s="0">
+        <v>58533</v>
+      </c>
+      <c r="D2655" s="0">
+        <v>0.136449147149121</v>
+      </c>
+      <c r="E2655" s="0">
+        <v>837</v>
+      </c>
+      <c r="F2655" s="0">
+        <v>0.139244718016969</v>
+      </c>
+      <c r="G2655" s="0">
+        <v>471</v>
+      </c>
+      <c r="H2655" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2656">
+      <c r="A2656" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B2656" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2656" s="0">
+        <v>41570</v>
+      </c>
+      <c r="D2656" s="0">
+        <v>9.69058658703462E-02</v>
+      </c>
+      <c r="E2656" s="0">
+        <v>630</v>
+      </c>
+      <c r="F2656" s="0">
+        <v>0.104807852270837</v>
+      </c>
+      <c r="G2656" s="0">
+        <v>988</v>
+      </c>
+      <c r="H2656" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2657">
+      <c r="A2657" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B2657" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2657" s="0">
+        <v>24940</v>
+      </c>
+      <c r="D2657" s="0">
+        <v>5.81388572241143E-02</v>
+      </c>
+      <c r="E2657" s="0">
+        <v>380</v>
+      </c>
+      <c r="F2657" s="0">
+        <v>6.32174347030444E-02</v>
+      </c>
+      <c r="G2657" s="0">
+        <v>1587</v>
+      </c>
+      <c r="H2657" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2658">
+      <c r="A2658" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B2658" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2658" s="0">
+        <v>13263</v>
+      </c>
+      <c r="D2658" s="0">
+        <v>3.09180298060717E-02</v>
+      </c>
+      <c r="E2658" s="0">
+        <v>203</v>
+      </c>
+      <c r="F2658" s="0">
+        <v>3.37714190650474E-02</v>
+      </c>
+      <c r="G2658" s="0">
+        <v>1919</v>
+      </c>
+      <c r="H2658" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2659">
+      <c r="A2659" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B2659" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2659" s="0">
+        <v>541</v>
+      </c>
+      <c r="D2659" s="0">
+        <v>1.26115163425204E-03</v>
+      </c>
+      <c r="E2659" s="0">
+        <v>-7</v>
+      </c>
+      <c r="F2659" s="0">
+        <v>-1.16453169189819E-03</v>
+      </c>
+      <c r="G2659" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2659" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2660">
+      <c r="A2660" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B2660" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2660" s="0">
+        <v>21986</v>
+      </c>
+      <c r="D2660" s="0">
+        <v>5.03963214765439E-02</v>
+      </c>
+      <c r="E2660" s="0">
+        <v>470</v>
+      </c>
+      <c r="F2660" s="0">
+        <v>6.44807243792015E-02</v>
+      </c>
+      <c r="G2660" s="0">
+        <v>5</v>
+      </c>
+      <c r="H2660" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2661">
+      <c r="A2661" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B2661" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2661" s="0">
+        <v>57228</v>
+      </c>
+      <c r="D2661" s="0">
+        <v>0.131178053554974</v>
+      </c>
+      <c r="E2661" s="0">
+        <v>936</v>
+      </c>
+      <c r="F2661" s="0">
+        <v>0.128412676636027</v>
+      </c>
+      <c r="G2661" s="0">
+        <v>3</v>
+      </c>
+      <c r="H2661" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2662">
+      <c r="A2662" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B2662" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2662" s="0">
+        <v>82089</v>
+      </c>
+      <c r="D2662" s="0">
+        <v>0.18816445163686</v>
+      </c>
+      <c r="E2662" s="0">
+        <v>1140</v>
+      </c>
+      <c r="F2662" s="0">
+        <v>0.156400054877212</v>
+      </c>
+      <c r="G2662" s="0">
+        <v>31</v>
+      </c>
+      <c r="H2662" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2663">
+      <c r="A2663" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B2663" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2663" s="0">
+        <v>68358</v>
+      </c>
+      <c r="D2663" s="0">
+        <v>0.156690245769744</v>
+      </c>
+      <c r="E2663" s="0">
+        <v>1102</v>
+      </c>
+      <c r="F2663" s="0">
+        <v>0.151186719714638</v>
+      </c>
+      <c r="G2663" s="0">
+        <v>63</v>
+      </c>
+      <c r="H2663" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2664">
+      <c r="A2664" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B2664" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2664" s="0">
+        <v>65160</v>
+      </c>
+      <c r="D2664" s="0">
+        <v>0.149359788384044</v>
+      </c>
+      <c r="E2664" s="0">
+        <v>1047</v>
+      </c>
+      <c r="F2664" s="0">
+        <v>0.143641103031966</v>
+      </c>
+      <c r="G2664" s="0">
+        <v>174</v>
+      </c>
+      <c r="H2664" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2665">
+      <c r="A2665" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B2665" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2665" s="0">
+        <v>59591</v>
+      </c>
+      <c r="D2665" s="0">
+        <v>0.136594523474426</v>
+      </c>
+      <c r="E2665" s="0">
+        <v>1058</v>
+      </c>
+      <c r="F2665" s="0">
+        <v>0.1451502263685</v>
+      </c>
+      <c r="G2665" s="0">
+        <v>477</v>
+      </c>
+      <c r="H2665" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2666">
+      <c r="A2666" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B2666" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2666" s="0">
+        <v>42389</v>
+      </c>
+      <c r="D2666" s="0">
+        <v>9.71640894691722E-02</v>
+      </c>
+      <c r="E2666" s="0">
+        <v>819</v>
+      </c>
+      <c r="F2666" s="0">
+        <v>0.112361092056524</v>
+      </c>
+      <c r="G2666" s="0">
+        <v>1000</v>
+      </c>
+      <c r="H2666" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2667">
+      <c r="A2667" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B2667" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2667" s="0">
+        <v>25433</v>
+      </c>
+      <c r="D2667" s="0">
+        <v>0.05829753680128</v>
+      </c>
+      <c r="E2667" s="0">
+        <v>493</v>
+      </c>
+      <c r="F2667" s="0">
+        <v>6.76361640828646E-02</v>
+      </c>
+      <c r="G2667" s="0">
+        <v>1615</v>
+      </c>
+      <c r="H2667" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2668">
+      <c r="A2668" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B2668" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2668" s="0">
+        <v>13487</v>
+      </c>
+      <c r="D2668" s="0">
+        <v>3.09149089308718E-02</v>
+      </c>
+      <c r="E2668" s="0">
+        <v>224</v>
+      </c>
+      <c r="F2668" s="0">
+        <v>3.07312388530663E-02</v>
+      </c>
+      <c r="G2668" s="0">
+        <v>1959</v>
+      </c>
+      <c r="H2668" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2669">
+      <c r="A2669" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B2669" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2669" s="0">
+        <v>541</v>
+      </c>
+      <c r="D2669" s="0">
+        <v>1.24008050208361E-03</v>
+      </c>
+      <c r="E2669" s="0">
+        <v>0</v>
+      </c>
+      <c r="F2669" s="0">
+        <v>0</v>
+      </c>
+      <c r="G2669" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2669" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2670">
+      <c r="A2670" s="1">
+        <v>44177</v>
+      </c>
+      <c r="B2670" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2670" s="0">
+        <v>22375</v>
+      </c>
+      <c r="D2670" s="0">
+        <v>5.05132598718148E-02</v>
+      </c>
+      <c r="E2670" s="0">
+        <v>389</v>
+      </c>
+      <c r="F2670" s="0">
+        <v>5.81377970408011E-02</v>
+      </c>
+      <c r="G2670" s="0">
+        <v>6</v>
+      </c>
+      <c r="H2670" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2671">
+      <c r="A2671" s="1">
+        <v>44177</v>
+      </c>
+      <c r="B2671" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2671" s="0">
+        <v>58021</v>
+      </c>
+      <c r="D2671" s="0">
+        <v>0.130986808984249</v>
+      </c>
+      <c r="E2671" s="0">
+        <v>793</v>
+      </c>
+      <c r="F2671" s="0">
+        <v>0.118517411448214</v>
+      </c>
+      <c r="G2671" s="0">
+        <v>3</v>
+      </c>
+      <c r="H2671" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2672">
+      <c r="A2672" s="1">
+        <v>44177</v>
+      </c>
+      <c r="B2672" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2672" s="0">
+        <v>83218</v>
+      </c>
+      <c r="D2672" s="0">
+        <v>0.187870947933528</v>
+      </c>
+      <c r="E2672" s="0">
+        <v>1129</v>
+      </c>
+      <c r="F2672" s="0">
+        <v>0.16873412046032</v>
+      </c>
+      <c r="G2672" s="0">
+        <v>31</v>
+      </c>
+      <c r="H2672" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2673">
+      <c r="A2673" s="1">
+        <v>44177</v>
+      </c>
+      <c r="B2673" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2673" s="0">
+        <v>69450</v>
+      </c>
+      <c r="D2673" s="0">
+        <v>0.156788643490393</v>
+      </c>
+      <c r="E2673" s="0">
+        <v>1092</v>
+      </c>
+      <c r="F2673" s="0">
+        <v>0.163204304289344</v>
+      </c>
+      <c r="G2673" s="0">
+        <v>63</v>
+      </c>
+      <c r="H2673" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2674">
+      <c r="A2674" s="1">
+        <v>44177</v>
+      </c>
+      <c r="B2674" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2674" s="0">
+        <v>66148</v>
+      </c>
+      <c r="D2674" s="0">
+        <v>0.149334128000036</v>
+      </c>
+      <c r="E2674" s="0">
+        <v>988</v>
+      </c>
+      <c r="F2674" s="0">
+        <v>0.147661037214168</v>
+      </c>
+      <c r="G2674" s="0">
+        <v>175</v>
+      </c>
+      <c r="H2674" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2675">
+      <c r="A2675" s="1">
+        <v>44177</v>
+      </c>
+      <c r="B2675" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2675" s="0">
+        <v>60555</v>
+      </c>
+      <c r="D2675" s="0">
+        <v>0.136707506213978</v>
+      </c>
+      <c r="E2675" s="0">
+        <v>964</v>
+      </c>
+      <c r="F2675" s="0">
+        <v>0.144074129427589</v>
+      </c>
+      <c r="G2675" s="0">
+        <v>479</v>
+      </c>
+      <c r="H2675" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2676">
+      <c r="A2676" s="1">
+        <v>44177</v>
+      </c>
+      <c r="B2676" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2676" s="0">
+        <v>43075</v>
+      </c>
+      <c r="D2676" s="0">
+        <v>9.72450801778067E-02</v>
+      </c>
+      <c r="E2676" s="0">
+        <v>686</v>
+      </c>
+      <c r="F2676" s="0">
+        <v>0.102525780899716</v>
+      </c>
+      <c r="G2676" s="0">
+        <v>1015</v>
+      </c>
+      <c r="H2676" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2677">
+      <c r="A2677" s="1">
+        <v>44177</v>
+      </c>
+      <c r="B2677" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2677" s="0">
+        <v>25823</v>
+      </c>
+      <c r="D2677" s="0">
+        <v>5.82973814377598E-02</v>
+      </c>
+      <c r="E2677" s="0">
+        <v>390</v>
+      </c>
+      <c r="F2677" s="0">
+        <v>5.82872515319085E-02</v>
+      </c>
+      <c r="G2677" s="0">
+        <v>1640</v>
+      </c>
+      <c r="H2677" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2678">
+      <c r="A2678" s="1">
+        <v>44177</v>
+      </c>
+      <c r="B2678" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2678" s="0">
+        <v>13734</v>
+      </c>
+      <c r="D2678" s="0">
+        <v>3.10055468638885E-02</v>
+      </c>
+      <c r="E2678" s="0">
+        <v>247</v>
+      </c>
+      <c r="F2678" s="0">
+        <v>3.69152593035421E-02</v>
+      </c>
+      <c r="G2678" s="0">
+        <v>1988</v>
+      </c>
+      <c r="H2678" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2679">
+      <c r="A2679" s="1">
+        <v>44177</v>
+      </c>
+      <c r="B2679" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2679" s="0">
+        <v>554</v>
+      </c>
+      <c r="D2679" s="0">
+        <v>1.25069702654683E-03</v>
+      </c>
+      <c r="E2679" s="0">
+        <v>13</v>
+      </c>
+      <c r="F2679" s="0">
+        <v>1.94290838439695E-03</v>
+      </c>
+      <c r="G2679" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2679" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2680">
+      <c r="A2680" s="1">
+        <v>44178</v>
+      </c>
+      <c r="B2680" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2680" s="0">
+        <v>22982</v>
+      </c>
+      <c r="D2680" s="0">
+        <v>5.05871606079616E-02</v>
+      </c>
+      <c r="E2680" s="0">
+        <v>607</v>
+      </c>
+      <c r="F2680" s="0">
+        <v>5.34707540521494E-02</v>
+      </c>
+      <c r="G2680" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2680" s="0">
+        <v>-2</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2681">
+      <c r="A2681" s="1">
+        <v>44178</v>
+      </c>
+      <c r="B2681" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2681" s="0">
+        <v>59451</v>
+      </c>
+      <c r="D2681" s="0">
+        <v>0.130861425694192</v>
+      </c>
+      <c r="E2681" s="0">
+        <v>1430</v>
+      </c>
+      <c r="F2681" s="0">
+        <v>0.125968992248062</v>
+      </c>
+      <c r="G2681" s="0">
+        <v>3</v>
+      </c>
+      <c r="H2681" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2682">
+      <c r="A2682" s="1">
+        <v>44178</v>
+      </c>
+      <c r="B2682" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2682" s="0">
+        <v>85216</v>
+      </c>
+      <c r="D2682" s="0">
+        <v>0.187574426871815</v>
+      </c>
+      <c r="E2682" s="0">
+        <v>1998</v>
+      </c>
+      <c r="F2682" s="0">
+        <v>0.17600422832981</v>
+      </c>
+      <c r="G2682" s="0">
+        <v>31</v>
+      </c>
+      <c r="H2682" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2683">
+      <c r="A2683" s="1">
+        <v>44178</v>
+      </c>
+      <c r="B2683" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2683" s="0">
+        <v>71183</v>
+      </c>
+      <c r="D2683" s="0">
+        <v>0.156685486622423</v>
+      </c>
+      <c r="E2683" s="0">
+        <v>1733</v>
+      </c>
+      <c r="F2683" s="0">
+        <v>0.152660324171952</v>
+      </c>
+      <c r="G2683" s="0">
+        <v>64</v>
+      </c>
+      <c r="H2683" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2684">
+      <c r="A2684" s="1">
+        <v>44178</v>
+      </c>
+      <c r="B2684" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2684" s="0">
+        <v>67838</v>
+      </c>
+      <c r="D2684" s="0">
+        <v>0.149322591650983</v>
+      </c>
+      <c r="E2684" s="0">
+        <v>1690</v>
+      </c>
+      <c r="F2684" s="0">
+        <v>0.148872445384073</v>
+      </c>
+      <c r="G2684" s="0">
+        <v>176</v>
+      </c>
+      <c r="H2684" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2685">
+      <c r="A2685" s="1">
+        <v>44178</v>
+      </c>
+      <c r="B2685" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2685" s="0">
+        <v>62228</v>
+      </c>
+      <c r="D2685" s="0">
+        <v>0.136974059277358</v>
+      </c>
+      <c r="E2685" s="0">
+        <v>1673</v>
+      </c>
+      <c r="F2685" s="0">
+        <v>0.147374911909796</v>
+      </c>
+      <c r="G2685" s="0">
+        <v>483</v>
+      </c>
+      <c r="H2685" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2686">
+      <c r="A2686" s="1">
+        <v>44178</v>
+      </c>
+      <c r="B2686" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2686" s="0">
+        <v>44264</v>
+      </c>
+      <c r="D2686" s="0">
+        <v>9.74323417087639E-02</v>
+      </c>
+      <c r="E2686" s="0">
+        <v>1189</v>
+      </c>
+      <c r="F2686" s="0">
+        <v>0.104739252995067</v>
+      </c>
+      <c r="G2686" s="0">
+        <v>1024</v>
+      </c>
+      <c r="H2686" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2687">
+      <c r="A2687" s="1">
+        <v>44178</v>
+      </c>
+      <c r="B2687" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2687" s="0">
+        <v>26480</v>
+      </c>
+      <c r="D2687" s="0">
+        <v>5.82868337350458E-02</v>
+      </c>
+      <c r="E2687" s="0">
+        <v>657</v>
+      </c>
+      <c r="F2687" s="0">
+        <v>5.78752642706131E-02</v>
+      </c>
+      <c r="G2687" s="0">
+        <v>1659</v>
+      </c>
+      <c r="H2687" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2688">
+      <c r="A2688" s="1">
+        <v>44178</v>
+      </c>
+      <c r="B2688" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2688" s="0">
+        <v>14103</v>
+      </c>
+      <c r="D2688" s="0">
+        <v>3.10430217585103E-02</v>
+      </c>
+      <c r="E2688" s="0">
+        <v>369</v>
+      </c>
+      <c r="F2688" s="0">
+        <v>3.25052854122622E-02</v>
+      </c>
+      <c r="G2688" s="0">
+        <v>2018</v>
+      </c>
+      <c r="H2688" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2689">
+      <c r="A2689" s="1">
+        <v>44178</v>
+      </c>
+      <c r="B2689" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2689" s="0">
+        <v>560</v>
+      </c>
+      <c r="D2689" s="0">
+        <v>1.23265207294659E-03</v>
+      </c>
+      <c r="E2689" s="0">
+        <v>6</v>
+      </c>
+      <c r="F2689" s="0">
+        <v>5.28541226215645E-04</v>
+      </c>
+      <c r="G2689" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2689" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2690">
+      <c r="A2690" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B2690" s="0" t="inlineStr">
+        <is>
+          <t>0-10 years</t>
+        </is>
+      </c>
+      <c r="C2690" s="0">
+        <v>23562</v>
+      </c>
+      <c r="D2690" s="0">
+        <v>5.07119735528083E-02</v>
+      </c>
+      <c r="E2690" s="0">
+        <v>580</v>
+      </c>
+      <c r="F2690" s="0">
+        <v>5.62069968020157E-02</v>
+      </c>
+      <c r="G2690" s="0">
+        <v>4</v>
+      </c>
+      <c r="H2690" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2691">
+      <c r="A2691" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B2691" s="0" t="inlineStr">
+        <is>
+          <t>11-20 years</t>
+        </is>
+      </c>
+      <c r="C2691" s="0">
+        <v>60811</v>
+      </c>
+      <c r="D2691" s="0">
+        <v>0.130882175694755</v>
+      </c>
+      <c r="E2691" s="0">
+        <v>1360</v>
+      </c>
+      <c r="F2691" s="0">
+        <v>0.131795716639209</v>
+      </c>
+      <c r="G2691" s="0">
+        <v>3</v>
+      </c>
+      <c r="H2691" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2692">
+      <c r="A2692" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B2692" s="0" t="inlineStr">
+        <is>
+          <t>21-30 years</t>
+        </is>
+      </c>
+      <c r="C2692" s="0">
+        <v>87015</v>
+      </c>
+      <c r="D2692" s="0">
+        <v>0.187280467646958</v>
+      </c>
+      <c r="E2692" s="0">
+        <v>1799</v>
+      </c>
+      <c r="F2692" s="0">
+        <v>0.174338598701425</v>
+      </c>
+      <c r="G2692" s="0">
+        <v>31</v>
+      </c>
+      <c r="H2692" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2693">
+      <c r="A2693" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B2693" s="0" t="inlineStr">
+        <is>
+          <t>31-40 years</t>
+        </is>
+      </c>
+      <c r="C2693" s="0">
+        <v>72787</v>
+      </c>
+      <c r="D2693" s="0">
+        <v>0.156657856675505</v>
+      </c>
+      <c r="E2693" s="0">
+        <v>1604</v>
+      </c>
+      <c r="F2693" s="0">
+        <v>0.155441418742126</v>
+      </c>
+      <c r="G2693" s="0">
+        <v>64</v>
+      </c>
+      <c r="H2693" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2694">
+      <c r="A2694" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B2694" s="0" t="inlineStr">
+        <is>
+          <t>41-50 years</t>
+        </is>
+      </c>
+      <c r="C2694" s="0">
+        <v>69344</v>
+      </c>
+      <c r="D2694" s="0">
+        <v>0.149247563621337</v>
+      </c>
+      <c r="E2694" s="0">
+        <v>1506</v>
+      </c>
+      <c r="F2694" s="0">
+        <v>0.145944374454889</v>
+      </c>
+      <c r="G2694" s="0">
+        <v>176</v>
+      </c>
+      <c r="H2694" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2695">
+      <c r="A2695" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B2695" s="0" t="inlineStr">
+        <is>
+          <t>51-60 years</t>
+        </is>
+      </c>
+      <c r="C2695" s="0">
+        <v>63694</v>
+      </c>
+      <c r="D2695" s="0">
+        <v>0.137087193085161</v>
+      </c>
+      <c r="E2695" s="0">
+        <v>1466</v>
+      </c>
+      <c r="F2695" s="0">
+        <v>0.142068029847853</v>
+      </c>
+      <c r="G2695" s="0">
+        <v>487</v>
+      </c>
+      <c r="H2695" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2696">
+      <c r="A2696" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B2696" s="0" t="inlineStr">
+        <is>
+          <t>61-70 years</t>
+        </is>
+      </c>
+      <c r="C2696" s="0">
+        <v>45319</v>
+      </c>
+      <c r="D2696" s="0">
+        <v>9.75390853679534E-02</v>
+      </c>
+      <c r="E2696" s="0">
+        <v>1055</v>
+      </c>
+      <c r="F2696" s="0">
+        <v>0.102238589010563</v>
+      </c>
+      <c r="G2696" s="0">
+        <v>1036</v>
+      </c>
+      <c r="H2696" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2697">
+      <c r="A2697" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B2697" s="0" t="inlineStr">
+        <is>
+          <t>71-80 years</t>
+        </is>
+      </c>
+      <c r="C2697" s="0">
+        <v>27119</v>
+      </c>
+      <c r="D2697" s="0">
+        <v>5.83676262956713E-02</v>
+      </c>
+      <c r="E2697" s="0">
+        <v>639</v>
+      </c>
+      <c r="F2697" s="0">
+        <v>6.19246050973932E-02</v>
+      </c>
+      <c r="G2697" s="0">
+        <v>1681</v>
+      </c>
+      <c r="H2697" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2698">
+      <c r="A2698" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B2698" s="0" t="inlineStr">
+        <is>
+          <t>81+ years</t>
+        </is>
+      </c>
+      <c r="C2698" s="0">
+        <v>14406</v>
+      </c>
+      <c r="D2698" s="0">
+        <v>0.031005716450291</v>
+      </c>
+      <c r="E2698" s="0">
+        <v>303</v>
+      </c>
+      <c r="F2698" s="0">
+        <v>2.93633103982944E-02</v>
+      </c>
+      <c r="G2698" s="0">
+        <v>2059</v>
+      </c>
+      <c r="H2698" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2699">
+      <c r="A2699" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B2699" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2699" s="0">
+        <v>567</v>
+      </c>
+      <c r="D2699" s="0">
+        <v>1.22034160955956E-03</v>
+      </c>
+      <c r="E2699" s="0">
+        <v>7</v>
+      </c>
+      <c r="F2699" s="0">
+        <v>6.78360306231224E-04</v>
+      </c>
+      <c r="G2699" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2699" s="0">
         <v>0</v>
       </c>
     </row>
@@ -73132,11 +75092,11 @@
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Home xmlns="f83d9bd0-d5f5-484c-bfdf-0c10f1e052c8">false</Home>
-    <_dlc_DocId xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">HJYU5V3E37X6-122305290-2058</_dlc_DocId>
+    <_dlc_DocId xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">HJYU5V3E37X6-122305290-2180</_dlc_DocId>
     <Present xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2">false</Present>
     <_dlc_DocIdUrl xmlns="98a58c6c-0c6a-4735-9794-66dbf75df29f">
-      <Url>https://tennessee.sharepoint.com/sites/health/PRG/COVID/_layouts/15/DocIdRedir.aspx?ID=HJYU5V3E37X6-122305290-2058</Url>
-      <Description>HJYU5V3E37X6-122305290-2058</Description>
+      <Url>https://tennessee.sharepoint.com/sites/health/PRG/COVID/_layouts/15/DocIdRedir.aspx?ID=HJYU5V3E37X6-122305290-2180</Url>
+      <Description>HJYU5V3E37X6-122305290-2180</Description>
     </_dlc_DocIdUrl>
     <Project_x0020_ID xmlns="4fcd0e8f-9e8d-4d61-8b29-f5c2c64ff0a2" xsi:nil="true"/>
     <Doc_x0020_Subject xmlns="2773c6ec-81e5-4cca-8f30-56e38046ef00" xsi:nil="true"/>
@@ -73159,17 +75119,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201E8360-F0D4-4D67-9B68-26552B62A386}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95F45B08-AEB6-4C92-AE7E-8FC51A0C5D95}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ADA1471-4F2B-4F4E-988A-30A5BE9C7717}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F3C9948-3CD2-4857-B69D-7FC741CD6AF6}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA9AFD13-DDC0-4F03-B488-D01AC39DAD65}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0BD5A3B-9E66-4967-8669-1A6F1B0D1B9E}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{074219A2-2789-4416-87C8-CF2A07C6A47D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A80D8996-09FC-480D-B9F9-1B21953F5561}"/>
 </file>
</xml_diff>